<commit_message>
First Order Interactions & Building Model w/o quality of outfit predictor
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B9611C-137F-8A41-A7F0-C8C80E3C6F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E63813B-C964-0E49-BE48-49BCD8986527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
+    <workbookView xWindow="36720" yWindow="1660" windowWidth="23980" windowHeight="17500" activeTab="2" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
   <sheets>
-    <sheet name="RPDR" sheetId="1" r:id="rId1"/>
-    <sheet name="Bottom Two" sheetId="2" r:id="rId2"/>
-    <sheet name="Delta B" sheetId="3" r:id="rId3"/>
+    <sheet name="RPDR Effect Estimates" sheetId="1" r:id="rId1"/>
+    <sheet name="Bottom Two Effect Estimates" sheetId="2" r:id="rId2"/>
+    <sheet name="Delta B Comparisons" sheetId="3" r:id="rId3"/>
+    <sheet name="Variable Interactions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="254">
   <si>
     <t>Age</t>
   </si>
@@ -524,9 +525,6 @@
     <t>0.0023 **</t>
   </si>
   <si>
-    <t>Likelihood Ratio Tests</t>
-  </si>
-  <si>
     <t>Analysis of Maximum Likelihood Estimates</t>
   </si>
   <si>
@@ -645,13 +643,160 @@
   </si>
   <si>
     <t xml:space="preserve">B Estimate Comparisons </t>
+  </si>
+  <si>
+    <t>Interactions</t>
+  </si>
+  <si>
+    <t>Outfit_Reveal:Gender</t>
+  </si>
+  <si>
+    <t>Outfit_Reveal:Quality_Of_Outfit</t>
+  </si>
+  <si>
+    <t>Outfit_Reveal:Do_They_Know_Words</t>
+  </si>
+  <si>
+    <t>Outfit_Reveal:Sewing</t>
+  </si>
+  <si>
+    <t>Outfit_Reveal:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Outfit_Reveal:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Gender:Outfit_Reveal</t>
+  </si>
+  <si>
+    <t>Gender:Quality_Of_Outfit</t>
+  </si>
+  <si>
+    <t>Gender:Do_They_Know_Words</t>
+  </si>
+  <si>
+    <t>Gender:Sewing</t>
+  </si>
+  <si>
+    <t>Gender:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Gender:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>B Estimate Comparisons (excluding Quality of Outfit Variable)</t>
+  </si>
+  <si>
+    <t>Quality_Of_Outfit:Outfit_Reveal</t>
+  </si>
+  <si>
+    <t>Quality_Of_Outfit:Do_They_Know_Words</t>
+  </si>
+  <si>
+    <t>Quality_Of_Outfit:Sewing</t>
+  </si>
+  <si>
+    <t>Quality_Of_Outfit:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Quality_Of_Outfit:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Do_They_Know_Words:Sewing</t>
+  </si>
+  <si>
+    <t>Do_They_Know_Words:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Do_They_Know_Words:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Sewing:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Sewing:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Likelihood Ratio Tests with Null Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analysis of First Order Interactions in Bottom Two </t>
+  </si>
+  <si>
+    <t>Model 3</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Body Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried </t>
+  </si>
+  <si>
+    <t xml:space="preserve">outfit reveal </t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>carson</t>
+  </si>
+  <si>
+    <t>eliminated variables</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>body type</t>
+  </si>
+  <si>
+    <t>ross</t>
+  </si>
+  <si>
+    <t>dancing</t>
+  </si>
+  <si>
+    <t>outfit reveal</t>
+  </si>
+  <si>
+    <t>do they know words</t>
+  </si>
+  <si>
+    <t>sewing</t>
+  </si>
+  <si>
+    <t>singing</t>
+  </si>
+  <si>
+    <t>lip sync ass</t>
+  </si>
+  <si>
+    <t>expressed hardship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model </t>
+  </si>
+  <si>
+    <t>full model</t>
+  </si>
+  <si>
+    <t>delta b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -694,8 +839,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,8 +896,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -805,11 +975,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -858,6 +1050,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -882,11 +1079,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115F1DD9-A0CB-2E42-BC0A-13187B41B5A6}">
   <dimension ref="A1:L144"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1228,19 +1442,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="H1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="H1" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12">
@@ -1263,13 +1477,13 @@
         <v>28</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1329,7 +1543,7 @@
         <v>110.04</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1350,7 +1564,7 @@
         <v>36</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I5" s="6">
         <v>26</v>
@@ -1359,7 +1573,7 @@
         <v>39.835000000000001</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1380,7 +1594,7 @@
         <v>0.59231</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I6" s="6">
         <v>1</v>
@@ -1470,7 +1684,7 @@
         <v>0.61486200000000002</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I9" s="6">
         <v>3</v>
@@ -1479,7 +1693,7 @@
         <v>14.166</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1509,7 +1723,7 @@
         <v>22.661000000000001</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1629,7 +1843,7 @@
         <v>22.407</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1868,7 +2082,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B28" s="8">
         <v>1.24759</v>
@@ -2448,7 +2662,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B60" s="8">
         <v>1.6217999999999999</v>
@@ -3784,8 +3998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50848286-ED49-A74D-91E6-1EBE098B2888}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3800,19 +4014,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="H1" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="27"/>
+      <c r="A1" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="H1" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -3834,13 +4048,13 @@
         <v>28</v>
       </c>
       <c r="I2" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3904,7 +4118,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" s="6">
         <v>0.29809999999999998</v>
@@ -3920,7 +4134,7 @@
         <v>0.3659</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I5" s="8">
         <v>1</v>
@@ -3950,7 +4164,7 @@
         <v>0.88014000000000003</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I6" s="8">
         <v>1</v>
@@ -3980,7 +4194,7 @@
         <v>0.93620000000000003</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I7" s="8">
         <v>1</v>
@@ -4010,7 +4224,7 @@
         <v>0.1356</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I8" s="8">
         <v>1</v>
@@ -4019,7 +4233,7 @@
         <v>20.145</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4040,7 +4254,7 @@
         <v>159</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I9" s="8">
         <v>1</v>
@@ -4070,7 +4284,7 @@
         <v>0.33023000000000002</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I10" s="8">
         <v>1</v>
@@ -4100,7 +4314,7 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I11" s="8">
         <v>1</v>
@@ -4130,7 +4344,7 @@
         <v>0.39657999999999999</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I12" s="8">
         <v>1</v>
@@ -4160,7 +4374,7 @@
         <v>8.2400000000000001E-2</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I13" s="8">
         <v>1</v>
@@ -4190,7 +4404,7 @@
         <v>0.16059999999999999</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I14" s="8">
         <v>1</v>
@@ -4199,7 +4413,7 @@
         <v>7.6304999999999996</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -4220,7 +4434,7 @@
         <v>160</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I15" s="8">
         <v>1</v>
@@ -4250,7 +4464,7 @@
         <v>0.1003</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I16" s="6">
         <v>1</v>
@@ -4339,7 +4553,7 @@
         <v>0.76300000000000001</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I19" s="6">
         <v>3</v>
@@ -4378,7 +4592,7 @@
         <v>10.54</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -4438,7 +4652,7 @@
         <v>5.3457999999999997</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -4467,7 +4681,7 @@
         <v>46.604999999999997</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -4497,7 +4711,7 @@
         <v>9.3961000000000006</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -4587,6 +4801,9 @@
       </c>
       <c r="E29" s="7">
         <v>0.47099999999999997</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -4690,10 +4907,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B9891-AE0A-EC49-A442-8B89DE5C2A2B}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q73" sqref="Q73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4702,421 +4919,2774 @@
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="G1" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6">
+        <v>-0.95860000000000001</v>
+      </c>
+      <c r="C3" s="6">
+        <v>-0.99063000000000001</v>
+      </c>
+      <c r="D3" s="6">
+        <f>ABS((B3-C3)/C3)</f>
+        <v>3.233295983364122E-2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6">
+        <v>-0.40770000000000001</v>
+      </c>
+      <c r="I3" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J3" s="6">
+        <f>ABS((H3-I3)/I3)</f>
+        <v>0.1379050489826677</v>
+      </c>
+      <c r="L3" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>245</v>
+      </c>
+      <c r="S3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="6">
+        <v>-1.2376</v>
+      </c>
+      <c r="C4" s="6">
+        <v>-1.2237</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D9" si="0">ABS((B4-C4)/C4)</f>
+        <v>1.1358993217291839E-2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="6">
+        <v>-2.3365</v>
+      </c>
+      <c r="I4" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" ref="J4:J5" si="1">ABS((H4-I4)/I4)</f>
+        <v>5.2472736609294648E-2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>244</v>
+      </c>
+      <c r="S4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6">
+        <v>-2.5912999999999999</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-2.4157999999999999</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>7.2646742279990059E-2</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="6">
+        <v>-0.71250000000000002</v>
+      </c>
+      <c r="I5" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="1"/>
+        <v>3.615924678381563E-2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>243</v>
+      </c>
+      <c r="S5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.76439999999999997</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.63932999999999995</v>
+      </c>
+      <c r="D6" s="6">
+        <f>ABS((B6-C6)/C6)</f>
+        <v>0.19562667167190656</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="35">
+        <v>-0.39229999999999998</v>
+      </c>
+      <c r="I6" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J6" s="38">
+        <f>ABS((H6-I6)/I6)</f>
+        <v>0.5494904810806539</v>
+      </c>
+      <c r="L6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-0.4042</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-0.40884999999999999</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1373364314540755E-2</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="6">
+        <v>-1.7008000000000001</v>
+      </c>
+      <c r="I7" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" ref="J7:J8" si="2">ABS((H7-I7)/I7)</f>
+        <v>6.3018196442245711E-2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>245</v>
+      </c>
+      <c r="S7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-1.8168</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-1.88056</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3904794316586571E-2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="6">
+        <v>-0.52749999999999997</v>
+      </c>
+      <c r="I8" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="2"/>
+        <v>4.2997097242380357E-2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>244</v>
+      </c>
+      <c r="S8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-0.49859999999999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-0.46009</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>8.3701015018800645E-2</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="L9" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>238</v>
+      </c>
+      <c r="S9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="L12" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="M12" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="N12" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="O12" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q12" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="R12" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="S12" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="T12" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="6">
+        <v>-0.95389999999999997</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-0.99063000000000001</v>
+      </c>
+      <c r="D13" s="6">
+        <f>ABS((B13-C13)/C13)</f>
+        <v>3.70774153821306E-2</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="13">
+        <v>-0.70240000000000002</v>
+      </c>
+      <c r="I13" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J13" s="6">
+        <f>ABS((H13-I13)/I13)</f>
+        <v>0.12214265181907938</v>
+      </c>
+      <c r="L13" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="M13">
+        <v>-0.76649999999999996</v>
+      </c>
+      <c r="N13" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ref="O13:O19" si="3">ABS((M13-N13)/N13)</f>
+        <v>4.2030670016122443E-2</v>
+      </c>
+      <c r="Q13" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="R13">
+        <v>-0.77049999999999996</v>
+      </c>
+      <c r="S13" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ref="T13:T20" si="4">ABS((R13-S13)/S13)</f>
+        <v>3.7031482384112635E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-1.2363</v>
+      </c>
+      <c r="C14" s="6">
+        <v>-1.2237</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" ref="D14:D20" si="5">ABS((B14-C14)/C14)</f>
+        <v>1.0296641333660166E-2</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="6">
+        <v>-0.41199999999999998</v>
+      </c>
+      <c r="I14" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J14" s="6">
+        <f>ABS((H14-I14)/I14)</f>
+        <v>0.149906500320969</v>
+      </c>
+      <c r="L14" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="M14">
+        <v>0.30830000000000002</v>
+      </c>
+      <c r="N14" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="O14" s="48">
+        <f t="shared" si="3"/>
+        <v>0.33752711496746207</v>
+      </c>
+      <c r="Q14" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="R14">
+        <v>0.30420000000000003</v>
+      </c>
+      <c r="S14" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="T14" s="48">
+        <f t="shared" si="4"/>
+        <v>0.31973969631236449</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="6">
+        <v>-2.5068000000000001</v>
+      </c>
+      <c r="C15" s="6">
+        <v>-2.4157999999999999</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="5"/>
+        <v>3.7668681182217154E-2</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="6">
+        <v>-2.2928000000000002</v>
+      </c>
+      <c r="I15" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" ref="J15:J16" si="6">ABS((H15-I15)/I15)</f>
+        <v>3.278814059396145E-2</v>
+      </c>
+      <c r="L15" t="s">
+        <v>239</v>
+      </c>
+      <c r="M15">
+        <v>-0.39500000000000002</v>
+      </c>
+      <c r="N15" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>0.10245890200675437</v>
+      </c>
+      <c r="Q15" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="R15">
+        <v>0.20019999999999999</v>
+      </c>
+      <c r="S15" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="T15" s="50">
+        <f t="shared" si="4"/>
+        <v>0.18812603917433804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.69769999999999999</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.63932999999999995</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="5"/>
+        <v>9.1298703330048706E-2</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="6">
+        <v>-0.70389999999999997</v>
+      </c>
+      <c r="I16" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="6"/>
+        <v>4.7792973770004035E-2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>246</v>
+      </c>
+      <c r="M16">
+        <v>-2.3134000000000001</v>
+      </c>
+      <c r="N16" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>4.2067378074873679E-2</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>239</v>
+      </c>
+      <c r="R16">
+        <v>-0.41899999999999998</v>
+      </c>
+      <c r="S16" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="4"/>
+        <v>0.16944374668564566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6">
+        <v>-0.3952</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-0.40884999999999999</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="5"/>
+        <v>3.338632750397455E-2</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="37">
+        <v>-0.39290000000000003</v>
+      </c>
+      <c r="I17" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J17" s="38">
+        <f>ABS((H17-I17)/I17)</f>
+        <v>0.55186033651947231</v>
+      </c>
+      <c r="L17" t="s">
+        <v>247</v>
+      </c>
+      <c r="M17">
+        <v>-0.68379999999999996</v>
+      </c>
+      <c r="N17" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="3"/>
+        <v>7.4983428702839555E-2</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>246</v>
+      </c>
+      <c r="R17">
+        <v>-2.3285999999999998</v>
+      </c>
+      <c r="S17" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="4"/>
+        <v>4.8914194080206835E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-1.7975000000000001</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-1.88056</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="5"/>
+        <v>4.4167694729229545E-2</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="6">
+        <v>-1.7048000000000001</v>
+      </c>
+      <c r="I18" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" ref="J18:J19" si="7">ABS((H18-I18)/I18)</f>
+        <v>6.0814570375552962E-2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>248</v>
+      </c>
+      <c r="M18">
+        <v>-0.37059999999999998</v>
+      </c>
+      <c r="N18" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="O18" s="48">
+        <f t="shared" si="3"/>
+        <v>0.46378070937672788</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>247</v>
+      </c>
+      <c r="R18">
+        <v>-0.69</v>
+      </c>
+      <c r="S18" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="4"/>
+        <v>6.6596323201168928E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-0.4667</v>
+      </c>
+      <c r="C19" s="6">
+        <v>-0.46009</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="5"/>
+        <v>1.4366754330674443E-2</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="6">
+        <v>-0.50390000000000001</v>
+      </c>
+      <c r="I19" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="7"/>
+        <v>8.5812772133526866E-2</v>
+      </c>
+      <c r="L19" t="s">
+        <v>249</v>
+      </c>
+      <c r="M19">
+        <v>-1.6984999999999999</v>
+      </c>
+      <c r="N19" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="3"/>
+        <v>6.4285281430594143E-2</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>248</v>
+      </c>
+      <c r="R19">
+        <v>-0.34520000000000001</v>
+      </c>
+      <c r="S19" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="T19" s="48">
+        <f t="shared" si="4"/>
+        <v>0.36345682913342281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="6">
+        <v>-0.31540000000000001</v>
+      </c>
+      <c r="C20" s="6">
+        <v>-0.24127999999999999</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="5"/>
+        <v>0.30719496021220166</v>
+      </c>
+      <c r="L20" t="s">
+        <v>250</v>
+      </c>
+      <c r="M20">
+        <v>-0.5071</v>
+      </c>
+      <c r="N20" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="O20">
+        <f>ABS((M20-N20)/N20)</f>
+        <v>8.0007256894049389E-2</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>249</v>
+      </c>
+      <c r="R20">
+        <v>-1.7601</v>
+      </c>
+      <c r="S20" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="4"/>
+        <v>3.0349440003525845E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="40"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="Q21" t="s">
+        <v>250</v>
+      </c>
+      <c r="R21">
+        <v>-0.53420000000000001</v>
+      </c>
+      <c r="S21" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="T21">
+        <f>ABS((R21-S21)/S21)</f>
+        <v>3.0841799709724265E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="L23" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="M23" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="N23" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="O23" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q23" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="R23" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="S23" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="T23" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="6">
+        <v>-0.95469999999999999</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-0.99063000000000001</v>
+      </c>
+      <c r="D24" s="6">
+        <f>ABS((B24-C24)/C24)</f>
+        <v>3.6269848480260054E-2</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="13">
+        <v>-0.70889999999999997</v>
+      </c>
+      <c r="I24" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J24" s="6">
+        <f>ABS((H24-I24)/I24)</f>
+        <v>0.11401897191706352</v>
+      </c>
+      <c r="L24" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="M24">
+        <v>-0.70889999999999997</v>
+      </c>
+      <c r="N24" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ref="O24:O30" si="8">ABS((M24-N24)/N24)</f>
+        <v>0.11401897191706352</v>
+      </c>
+      <c r="Q24" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="R24">
+        <v>-0.78459999999999996</v>
+      </c>
+      <c r="S24" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="T24">
+        <f t="shared" ref="T24:T31" si="9">ABS((R24-S24)/S24)</f>
+        <v>1.9409345981278098E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="6">
+        <v>-1.2494000000000001</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-1.2237</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" ref="D25:D32" si="10">ABS((B25-C25)/C25)</f>
+        <v>2.1001879545640319E-2</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0.2019</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="J25" s="6">
+        <f>ABS((H25-I25)/I25)</f>
+        <v>0.18123200454195226</v>
+      </c>
+      <c r="L25" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="M25">
+        <v>0.2019</v>
+      </c>
+      <c r="N25" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="O25" s="50">
+        <f t="shared" si="8"/>
+        <v>0.18123200454195226</v>
+      </c>
+      <c r="Q25" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="R25">
+        <v>0.2853</v>
+      </c>
+      <c r="S25" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="T25" s="48">
+        <f t="shared" si="9"/>
+        <v>0.2377440347071583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="6">
+        <v>-2.5242</v>
+      </c>
+      <c r="C26" s="6">
+        <v>-2.4157999999999999</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" si="10"/>
+        <v>4.4871264177498163E-2</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="6">
+        <v>-0.43569999999999998</v>
+      </c>
+      <c r="I26" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J26" s="46">
+        <f>ABS((H26-I26)/I26)</f>
+        <v>0.21605403444137425</v>
+      </c>
+      <c r="L26" t="s">
+        <v>239</v>
+      </c>
+      <c r="M26">
+        <v>-0.43569999999999998</v>
+      </c>
+      <c r="N26" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="O26" s="48">
+        <f t="shared" si="8"/>
+        <v>0.21605403444137425</v>
+      </c>
+      <c r="Q26" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="R26">
+        <v>-0.1608</v>
+      </c>
+      <c r="S26" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="T26" s="48">
+        <f t="shared" si="9"/>
+        <v>0.37927041111754489</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.70009999999999994</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.63932999999999995</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="10"/>
+        <v>9.5052633225407843E-2</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="6">
+        <v>-2.3079000000000001</v>
+      </c>
+      <c r="I27" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" ref="J27:J28" si="11">ABS((H27-I27)/I27)</f>
+        <v>3.9589911757154359E-2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>246</v>
+      </c>
+      <c r="M27">
+        <v>-2.3079000000000001</v>
+      </c>
+      <c r="N27" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="O27">
+        <f>ABS((M27-N27)/N27)</f>
+        <v>3.9589911757154359E-2</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>239</v>
+      </c>
+      <c r="R27">
+        <v>-0.35389999999999999</v>
+      </c>
+      <c r="S27" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="9"/>
+        <v>1.2252644505847232E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="6">
+        <v>-0.3957</v>
+      </c>
+      <c r="C28" s="6">
+        <v>-0.40884999999999999</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="10"/>
+        <v>3.2163385104561563E-2</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="6">
+        <v>-0.70899999999999996</v>
+      </c>
+      <c r="I28" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="11"/>
+        <v>4.0893903115403987E-2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>247</v>
+      </c>
+      <c r="M28">
+        <v>-0.70899999999999996</v>
+      </c>
+      <c r="N28" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="O28">
+        <f>ABS((M28-N28)/N28)</f>
+        <v>4.0893903115403987E-2</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>246</v>
+      </c>
+      <c r="R28">
+        <v>-2.2522000000000002</v>
+      </c>
+      <c r="S28" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="9"/>
+        <v>1.4499934684979071E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="6">
+        <v>-1.8623000000000001</v>
+      </c>
+      <c r="C29" s="6">
+        <v>-1.88056</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="10"/>
+        <v>9.7098736546560298E-3</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="37">
+        <v>-0.36720000000000003</v>
+      </c>
+      <c r="I29" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J29" s="38">
+        <f>ABS((H29-I29)/I29)</f>
+        <v>0.45035152855675803</v>
+      </c>
+      <c r="L29" t="s">
+        <v>248</v>
+      </c>
+      <c r="M29">
+        <v>-0.36720000000000003</v>
+      </c>
+      <c r="N29" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="O29" s="48">
+        <f t="shared" si="8"/>
+        <v>0.45035152855675803</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>247</v>
+      </c>
+      <c r="R29">
+        <v>-0.70269999999999999</v>
+      </c>
+      <c r="S29" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="9"/>
+        <v>4.9416284512262841E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="6">
+        <v>-0.49349999999999999</v>
+      </c>
+      <c r="C30" s="6">
+        <v>-0.46009</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="10"/>
+        <v>7.2616227259883925E-2</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="6">
+        <v>-1.7668999999999999</v>
+      </c>
+      <c r="I30" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" ref="J30" si="12">ABS((H30-I30)/I30)</f>
+        <v>2.6603275690148229E-2</v>
+      </c>
+      <c r="L30" t="s">
+        <v>249</v>
+      </c>
+      <c r="M30">
+        <v>-1.7668999999999999</v>
+      </c>
+      <c r="N30" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="8"/>
+        <v>2.6603275690148229E-2</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>248</v>
+      </c>
+      <c r="R30">
+        <v>-0.35399999999999998</v>
+      </c>
+      <c r="S30" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="T30" s="48">
+        <f t="shared" si="9"/>
+        <v>0.39821470890275679</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="6">
+        <v>-0.28670000000000001</v>
+      </c>
+      <c r="C31" s="6">
+        <v>-0.24127999999999999</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="10"/>
+        <v>0.18824602122015921</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="6">
+        <v>-0.53069999999999995</v>
+      </c>
+      <c r="I31" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J31" s="6">
+        <f>ABS((H31-I31)/I31)</f>
+        <v>3.7191582002902887E-2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>250</v>
+      </c>
+      <c r="M31">
+        <v>-0.53069999999999995</v>
+      </c>
+      <c r="N31" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="O31">
+        <f>ABS((M31-N31)/N31)</f>
+        <v>3.7191582002902887E-2</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>249</v>
+      </c>
+      <c r="R31">
+        <v>-1.6884999999999999</v>
+      </c>
+      <c r="S31" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="9"/>
+        <v>6.9794346597326001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.22040000000000001</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.22370000000000001</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="10"/>
+        <v>1.4751899865891807E-2</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>250</v>
+      </c>
+      <c r="R32">
+        <v>-0.50160000000000005</v>
+      </c>
+      <c r="S32" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="T32">
+        <f>ABS((R32-S32)/S32)</f>
+        <v>8.9985486211901264E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="7:20">
+      <c r="G34" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="I34" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="L34" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="M34" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="N34" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="O34" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q34" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="R34" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="S34" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="T34" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="7:20">
+      <c r="G35" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="13">
+        <v>-0.73839999999999995</v>
+      </c>
+      <c r="I35" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J35" s="6">
+        <f>ABS((H35-I35)/I35)</f>
+        <v>7.7149963130991289E-2</v>
+      </c>
+      <c r="L35" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="M35">
+        <v>-0.7268</v>
+      </c>
+      <c r="N35" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ref="O35:O37" si="13">ABS((M35-N35)/N35)</f>
+        <v>9.1647607263819639E-2</v>
+      </c>
+      <c r="Q35" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="R35">
+        <v>0.22509999999999999</v>
+      </c>
+      <c r="S35" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="T35">
+        <f t="shared" ref="T35:T42" si="14">ABS((R35-S35)/S35)</f>
+        <v>8.7148708382335086E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="7:20">
+      <c r="G36" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="13">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I36" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="J36" s="6">
+        <f>ABS((H36-I36)/I36)</f>
+        <v>6.3222352893466852E-2</v>
+      </c>
+      <c r="L36" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="M36">
+        <v>-0.17369999999999999</v>
+      </c>
+      <c r="N36" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="O36" s="48">
+        <f t="shared" si="13"/>
+        <v>0.32947307469600468</v>
+      </c>
+      <c r="Q36" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="R36">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="S36" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="T36" s="48">
+        <f t="shared" si="14"/>
+        <v>0.2841648590021692</v>
+      </c>
+    </row>
+    <row r="37" spans="7:20">
+      <c r="G37" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="H37" s="13">
+        <v>-0.20449999999999999</v>
+      </c>
+      <c r="I37" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="J37" s="46">
+        <f>ABS((H37-I37)/I37)</f>
+        <v>0.21057710866628071</v>
+      </c>
+      <c r="L37" t="s">
+        <v>239</v>
+      </c>
+      <c r="M37">
+        <v>-0.36630000000000001</v>
+      </c>
+      <c r="N37" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="O37" s="50">
+        <f t="shared" si="13"/>
+        <v>2.2356191911580052E-2</v>
+      </c>
+      <c r="Q37" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="R37">
+        <v>-0.17549999999999999</v>
+      </c>
+      <c r="S37" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="T37" s="48">
+        <f t="shared" si="14"/>
+        <v>0.32252460914881304</v>
+      </c>
+    </row>
+    <row r="38" spans="7:20">
+      <c r="G38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="6">
+        <v>-0.38669999999999999</v>
+      </c>
+      <c r="I38" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J38" s="8">
+        <f>ABS((H38-I38)/I38)</f>
+        <v>7.929330988863767E-2</v>
+      </c>
+      <c r="L38" t="s">
+        <v>246</v>
+      </c>
+      <c r="M38">
+        <v>-2.2286000000000001</v>
+      </c>
+      <c r="N38" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="O38">
+        <f>ABS((M38-N38)/N38)</f>
+        <v>3.869351939856271E-3</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>239</v>
+      </c>
+      <c r="R38">
+        <v>-0.38030000000000003</v>
+      </c>
+      <c r="S38" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="14"/>
+        <v>6.1430684640933403E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="7:20">
+      <c r="G39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="6">
+        <v>-2.2353000000000001</v>
+      </c>
+      <c r="I39" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J39" s="6">
+        <f t="shared" ref="J39:J40" si="15">ABS((H39-I39)/I39)</f>
+        <v>6.8873563632597373E-3</v>
+      </c>
+      <c r="L39" t="s">
+        <v>247</v>
+      </c>
+      <c r="M39">
+        <v>-0.72309999999999997</v>
+      </c>
+      <c r="N39" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="O39">
+        <f>ABS((M39-N39)/N39)</f>
+        <v>2.1820001893862653E-2</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>246</v>
+      </c>
+      <c r="R39">
+        <v>-2.3028</v>
+      </c>
+      <c r="S39" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="14"/>
+        <v>3.729262480799643E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="7:20">
+      <c r="G40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="6">
+        <v>-0.73209999999999997</v>
+      </c>
+      <c r="I40" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J40" s="6">
+        <f t="shared" si="15"/>
+        <v>9.6451713269213642E-3</v>
+      </c>
+      <c r="L40" t="s">
+        <v>248</v>
+      </c>
+      <c r="M40">
+        <v>-0.37280000000000002</v>
+      </c>
+      <c r="N40" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="O40" s="48">
+        <f t="shared" ref="O40:O41" si="16">ABS((M40-N40)/N40)</f>
+        <v>0.47247017931906155</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>247</v>
+      </c>
+      <c r="R40">
+        <v>-0.72819999999999996</v>
+      </c>
+      <c r="S40" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="14"/>
+        <v>1.4920931239262603E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="7:20">
+      <c r="G41" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="37">
+        <v>-0.34029999999999999</v>
+      </c>
+      <c r="I41" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J41" s="38">
+        <f>ABS((H41-I41)/I41)</f>
+        <v>0.34410300971640717</v>
+      </c>
+      <c r="L41" t="s">
+        <v>249</v>
+      </c>
+      <c r="M41">
+        <v>-1.6936</v>
+      </c>
+      <c r="N41" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="16"/>
+        <v>6.6984723362292692E-2</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>248</v>
+      </c>
+      <c r="R41">
+        <v>-0.33300000000000002</v>
+      </c>
+      <c r="S41" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="T41" s="48">
+        <f t="shared" si="14"/>
+        <v>0.31526976854411881</v>
+      </c>
+    </row>
+    <row r="42" spans="7:20">
+      <c r="G42" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="6">
+        <v>-1.7627999999999999</v>
+      </c>
+      <c r="I42" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J42" s="6">
+        <f t="shared" ref="J42:J43" si="17">ABS((H42-I42)/I42)</f>
+        <v>2.8861992408508286E-2</v>
+      </c>
+      <c r="L42" t="s">
+        <v>250</v>
+      </c>
+      <c r="M42">
+        <v>-0.49869999999999998</v>
+      </c>
+      <c r="N42" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="O42">
+        <f>ABS((M42-N42)/N42)</f>
+        <v>9.5246734397677876E-2</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>249</v>
+      </c>
+      <c r="R42">
+        <v>-1.7545999999999999</v>
+      </c>
+      <c r="S42" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="14"/>
+        <v>3.3379425845228398E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="7:20">
+      <c r="G43" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="6">
+        <v>-0.52829999999999999</v>
+      </c>
+      <c r="I43" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J43" s="6">
+        <f t="shared" si="17"/>
+        <v>4.1545718432510939E-2</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>250</v>
+      </c>
+      <c r="R43">
+        <v>-0.55549999999999999</v>
+      </c>
+      <c r="S43" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="T43">
+        <f>ABS((R43-S43)/S43)</f>
+        <v>7.801161103047842E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="7:20">
+      <c r="L44" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="M44" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="N44" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="O44" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="45" spans="7:20">
+      <c r="L45" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="M45">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="N45" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="O45" s="50">
+        <f t="shared" ref="O45:O50" si="18">ABS((M45-N45)/N45)</f>
+        <v>0.16616052060737527</v>
+      </c>
+    </row>
+    <row r="46" spans="7:20">
+      <c r="G46" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H46" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="L46" t="s">
+        <v>239</v>
+      </c>
+      <c r="M46">
+        <v>-0.39689999999999998</v>
+      </c>
+      <c r="N46" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="18"/>
+        <v>0.10776186887716648</v>
+      </c>
+    </row>
+    <row r="47" spans="7:20">
+      <c r="G47" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="13">
+        <v>-0.79220000000000002</v>
+      </c>
+      <c r="I47" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J47" s="6">
+        <f>ABS((H47-I47)/I47)</f>
+        <v>9.9108894804594162E-3</v>
+      </c>
+      <c r="L47" t="s">
+        <v>246</v>
+      </c>
+      <c r="M47">
+        <v>-2.3517999999999999</v>
+      </c>
+      <c r="N47" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="18"/>
+        <v>5.9364597456768253E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="7:20">
+      <c r="G48" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="13">
+        <v>0.22750000000000001</v>
+      </c>
+      <c r="I48" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="J48" s="6">
+        <f>ABS((H48-I48)/I48)</f>
+        <v>7.7415953607202215E-2</v>
+      </c>
+      <c r="L48" t="s">
+        <v>247</v>
+      </c>
+      <c r="M48">
+        <v>-0.70020000000000004</v>
+      </c>
+      <c r="N48" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="18"/>
+        <v>5.2798181891968679E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="7:15">
+      <c r="G49" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="H49" s="13">
+        <v>-0.19139999999999999</v>
+      </c>
+      <c r="I49" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="J49" s="8">
+        <f>ABS((H49-I49)/I49)</f>
+        <v>0.26114649681528668</v>
+      </c>
+      <c r="L49" t="s">
+        <v>248</v>
+      </c>
+      <c r="M49">
+        <v>-0.37780000000000002</v>
+      </c>
+      <c r="N49" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="O49" s="48">
+        <f t="shared" si="18"/>
+        <v>0.49221897464254682</v>
+      </c>
+    </row>
+    <row r="50" spans="7:15">
+      <c r="G50" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="H50" s="13">
+        <v>0.2757</v>
+      </c>
+      <c r="I50" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="J50" s="8">
+        <f>ABS((H50-I50)/I50)</f>
+        <v>0.19609544468546633</v>
+      </c>
+      <c r="L50" t="s">
+        <v>249</v>
+      </c>
+      <c r="M50">
+        <v>-1.6970000000000001</v>
+      </c>
+      <c r="N50" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="18"/>
+        <v>6.5111641205603824E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="7:15">
+      <c r="G51" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="6">
+        <v>-0.37459999999999999</v>
+      </c>
+      <c r="I51" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J51" s="8">
+        <f>ABS((H51-I51)/I51)</f>
+        <v>4.5521784029696588E-2</v>
+      </c>
+      <c r="L51" t="s">
+        <v>250</v>
+      </c>
+      <c r="M51">
+        <v>-0.53100000000000003</v>
+      </c>
+      <c r="N51" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="O51">
+        <f>ABS((M51-N51)/N51)</f>
+        <v>3.6647314949201731E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="7:15">
+      <c r="G52" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="6">
+        <v>-2.2584</v>
+      </c>
+      <c r="I52" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J52" s="8">
+        <f t="shared" ref="J52:J53" si="19">ABS((H52-I52)/I52)</f>
+        <v>1.7292714897680708E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="7:15">
+      <c r="G53" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="6">
+        <v>-0.71319999999999995</v>
+      </c>
+      <c r="I53" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J53" s="8">
+        <f t="shared" si="19"/>
+        <v>3.521231551749808E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="7:15">
+      <c r="G54" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="37">
+        <v>-0.32250000000000001</v>
+      </c>
+      <c r="I54" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J54" s="38">
+        <f>ABS((H54-I54)/I54)</f>
+        <v>0.27379729836479971</v>
+      </c>
+      <c r="L54" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="M54" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="N54" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="O54" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="7:15">
+      <c r="G55" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H55" s="6">
+        <v>-1.7566999999999999</v>
+      </c>
+      <c r="I55" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J55" s="6">
+        <f t="shared" ref="J55:J56" si="20">ABS((H55-I55)/I55)</f>
+        <v>3.2222522160214713E-2</v>
+      </c>
+      <c r="L55" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="M55">
+        <v>0.16889999999999999</v>
+      </c>
+      <c r="N55" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="O55" s="50">
+        <f t="shared" ref="O55:O59" si="21">ABS((M55-N55)/N55)</f>
+        <v>0.26724511930585687</v>
+      </c>
+    </row>
+    <row r="56" spans="7:15">
+      <c r="G56" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H56" s="6">
+        <v>-0.53120000000000001</v>
+      </c>
+      <c r="I56" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J56" s="6">
+        <f t="shared" si="20"/>
+        <v>3.6284470246734431E-2</v>
+      </c>
+      <c r="L56" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="M56">
+        <v>-0.14510000000000001</v>
+      </c>
+      <c r="N56" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="O56" s="48">
+        <f t="shared" si="21"/>
+        <v>0.43987647172360544</v>
+      </c>
+    </row>
+    <row r="57" spans="7:15">
+      <c r="L57" t="s">
+        <v>239</v>
+      </c>
+      <c r="M57">
+        <v>-0.35870000000000002</v>
+      </c>
+      <c r="N57" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="21"/>
+        <v>1.1443244299311213E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="7:15">
+      <c r="L58" t="s">
+        <v>246</v>
+      </c>
+      <c r="M58">
+        <v>-2.2966000000000002</v>
+      </c>
+      <c r="N58" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="21"/>
+        <v>3.4499844595294787E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="7:15">
+      <c r="G59" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H59" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="I59" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J59" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="L59" t="s">
+        <v>247</v>
+      </c>
+      <c r="M59">
+        <v>-0.7177</v>
+      </c>
+      <c r="N59" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="21"/>
+        <v>2.9124900234027362E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="7:15">
+      <c r="G60" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J60" s="6">
+        <f>ABS((H60-I60)/I60)</f>
+        <v>1</v>
+      </c>
+      <c r="L60" t="s">
+        <v>248</v>
+      </c>
+      <c r="M60">
+        <v>-0.36280000000000001</v>
+      </c>
+      <c r="N60" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="O60" s="48">
+        <f>ABS((M60-N60)/N60)</f>
+        <v>0.43297258867209093</v>
+      </c>
+    </row>
+    <row r="61" spans="7:15">
+      <c r="G61" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="J61" s="6">
+        <f>ABS((H61-I61)/I61)</f>
+        <v>1</v>
+      </c>
+      <c r="L61" t="s">
+        <v>249</v>
+      </c>
+      <c r="M61">
+        <v>-1.6861999999999999</v>
+      </c>
+      <c r="N61" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="O61">
+        <f>ABS((M61-N61)/N61)</f>
+        <v>7.1061431585674309E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="7:15">
+      <c r="G62" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="J62" s="8">
+        <f>ABS((H62-I62)/I62)</f>
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
+        <v>250</v>
+      </c>
+      <c r="M62">
+        <v>-0.52659999999999996</v>
+      </c>
+      <c r="N62" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="O62">
+        <f>ABS((M62-N62)/N62)</f>
+        <v>4.4629898403483428E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="7:15">
+      <c r="G63" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="J63" s="8">
+        <f>ABS((H63-I63)/I63)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="7:15">
+      <c r="G64" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="8"/>
+    </row>
+    <row r="65" spans="7:15">
+      <c r="G65" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J65" s="8">
+        <f>ABS((H65-I65)/I65)</f>
+        <v>1</v>
+      </c>
+      <c r="L65" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="M65" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="N65" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="O65" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="66" spans="7:15">
+      <c r="G66" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J66" s="8">
+        <f t="shared" ref="J66:J67" si="22">ABS((H66-I66)/I66)</f>
+        <v>1</v>
+      </c>
+      <c r="L66" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="M66">
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="N66" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="O66" s="50">
+        <f t="shared" ref="O66:O69" si="23">ABS((M66-N66)/N66)</f>
+        <v>0.16225596529284173</v>
+      </c>
+    </row>
+    <row r="67" spans="7:15">
+      <c r="G67" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J67" s="8">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L67" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="M67">
+        <v>0.19980000000000001</v>
+      </c>
+      <c r="N67" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="O67" s="50">
+        <f>ABS((M67-N67)/N67)</f>
+        <v>0.18974816497019342</v>
+      </c>
+    </row>
+    <row r="68" spans="7:15">
+      <c r="G68" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" s="37"/>
+      <c r="I68" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J68" s="38">
+        <f>ABS((H68-I68)/I68)</f>
+        <v>1</v>
+      </c>
+      <c r="L68" t="s">
+        <v>239</v>
+      </c>
+      <c r="M68">
+        <v>-0.42209999999999998</v>
+      </c>
+      <c r="N68" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="O68" s="50">
+        <f>ABS((M68-N68)/N68)</f>
+        <v>0.17809595579000245</v>
+      </c>
+    </row>
+    <row r="69" spans="7:15">
+      <c r="G69" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J69" s="6">
+        <f t="shared" ref="J69:J70" si="24">ABS((H69-I69)/I69)</f>
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
+        <v>246</v>
+      </c>
+      <c r="M69">
+        <v>-2.367</v>
+      </c>
+      <c r="N69" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="O69" s="50">
+        <f t="shared" si="23"/>
+        <v>6.6211413462101604E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="7:15">
+      <c r="G70" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J70" s="6">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="L70" t="s">
+        <v>247</v>
+      </c>
+      <c r="M70">
+        <v>-0.70640000000000003</v>
+      </c>
+      <c r="N70" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="O70">
+        <f t="shared" ref="O70:O72" si="25">ABS((M70-N70)/N70)</f>
+        <v>4.4411076390298045E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="7:15">
+      <c r="L71" t="s">
+        <v>248</v>
+      </c>
+      <c r="M71">
+        <v>-0.35389999999999999</v>
+      </c>
+      <c r="N71" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="O71" s="48">
+        <f t="shared" si="25"/>
+        <v>0.39781973299628709</v>
+      </c>
+    </row>
+    <row r="72" spans="7:15">
+      <c r="L72" t="s">
+        <v>249</v>
+      </c>
+      <c r="M72">
+        <v>-1.7597</v>
+      </c>
+      <c r="N72" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="25"/>
+        <v>3.0569802610195096E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="7:15">
+      <c r="L73" t="s">
+        <v>250</v>
+      </c>
+      <c r="M73">
+        <v>-0.5575</v>
+      </c>
+      <c r="N73" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="O73">
+        <f>ABS((M73-N73)/N73)</f>
+        <v>1.1429608127721284E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="7:15">
+      <c r="L75" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="M75" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="N75" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="O75" s="47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="76" spans="7:15">
+      <c r="L76" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="M76">
+        <v>-0.184</v>
+      </c>
+      <c r="N76" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="O76" s="48">
+        <f t="shared" ref="O76" si="26">ABS((M76-N76)/N76)</f>
+        <v>0.28971241073151904</v>
+      </c>
+    </row>
+    <row r="77" spans="7:15">
+      <c r="L77" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="M77">
+        <v>0.22589999999999999</v>
+      </c>
+      <c r="N77" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="O77" s="50">
+        <f>ABS((M77-N77)/N77)</f>
+        <v>8.3904456790624166E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="7:15">
+      <c r="L78" t="s">
+        <v>239</v>
+      </c>
+      <c r="M78">
+        <v>-0.38719999999999999</v>
+      </c>
+      <c r="N78" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="O78" s="50">
+        <f>ABS((M78-N78)/N78)</f>
+        <v>8.068882748611457E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="7:15">
+      <c r="L79" t="s">
+        <v>246</v>
+      </c>
+      <c r="M79">
+        <v>-2.2867000000000002</v>
+      </c>
+      <c r="N79" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="O79" s="50">
+        <f t="shared" ref="O79:O82" si="27">ABS((M79-N79)/N79)</f>
+        <v>3.0040405223400058E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="7:15">
+      <c r="L80" t="s">
+        <v>247</v>
+      </c>
+      <c r="M80">
+        <v>-0.73929999999999996</v>
+      </c>
+      <c r="N80" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="O80">
+        <f>ABS((M80-N80)/N80)</f>
+        <v>9.4693126631634902E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="12:15">
+      <c r="L81" t="s">
+        <v>248</v>
+      </c>
+      <c r="M81">
+        <v>-0.34420000000000001</v>
+      </c>
+      <c r="N81" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="O81" s="48">
+        <f t="shared" si="27"/>
+        <v>0.35950707006872573</v>
+      </c>
+    </row>
+    <row r="82" spans="12:15">
+      <c r="L82" t="s">
+        <v>249</v>
+      </c>
+      <c r="M82">
+        <v>-1.7575000000000001</v>
+      </c>
+      <c r="N82" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="O82">
+        <f t="shared" si="27"/>
+        <v>3.1781796946876092E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="12:15">
+      <c r="L83" t="s">
+        <v>250</v>
+      </c>
+      <c r="M83">
+        <v>-0.5524</v>
+      </c>
+      <c r="N83" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="O83">
+        <f>ABS((M83-N83)/N83)</f>
+        <v>2.1770682148040256E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F618E10-1DFA-C44A-B66A-2018A4130538}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1">
+      <c r="A2" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>202</v>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6">
-        <v>-0.95860000000000001</v>
-      </c>
-      <c r="C3" s="6">
-        <v>-0.99063000000000001</v>
-      </c>
-      <c r="D3" s="6">
-        <f>ABS((B3-C3)/C3)</f>
-        <v>3.233295983364122E-2</v>
+      <c r="A3" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44">
+        <v>9.4030000000000006E-5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="6">
-        <v>-1.2376</v>
-      </c>
-      <c r="C4" s="6">
-        <v>-1.2237</v>
-      </c>
+      <c r="A4" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="6">
-        <f t="shared" ref="D4:D9" si="0">ABS((B4-C4)/C4)</f>
-        <v>1.1358993217291839E-2</v>
+        <v>0.16550000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="6">
-        <v>-2.5912999999999999</v>
-      </c>
-      <c r="C5" s="6">
-        <v>-2.4157999999999999</v>
-      </c>
+      <c r="A5" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="6">
-        <f t="shared" si="0"/>
-        <v>7.2646742279990059E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.76439999999999997</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.63932999999999995</v>
-      </c>
+      <c r="A6" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="6">
-        <f>ABS((B6-C6)/C6)</f>
-        <v>0.19562667167190656</v>
+        <v>0.75860000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6">
-        <v>-0.4042</v>
-      </c>
-      <c r="C7" s="6">
-        <v>-0.40884999999999999</v>
-      </c>
+      <c r="A7" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="6">
-        <f t="shared" si="0"/>
-        <v>1.1373364314540755E-2</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="6">
-        <v>-1.8168</v>
-      </c>
-      <c r="C8" s="6">
-        <v>-1.88056</v>
-      </c>
+      <c r="A8" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3904794316586571E-2</v>
+        <v>0.94099999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6">
-        <v>-0.49859999999999999</v>
-      </c>
-      <c r="C9" s="6">
-        <v>-0.46009</v>
-      </c>
+      <c r="A9" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="6">
-        <f t="shared" si="0"/>
-        <v>8.3701015018800645E-2</v>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="6">
+        <v>0.29599999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>202</v>
+      <c r="A12" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="6">
+        <v>0.7409</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="6">
-        <v>-0.95389999999999997</v>
-      </c>
-      <c r="C13" s="6">
-        <v>-0.99063000000000001</v>
-      </c>
+      <c r="A13" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="6">
-        <f>ABS((B13-C13)/C13)</f>
-        <v>3.70774153821306E-2</v>
+        <v>0.6431</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="6">
-        <v>-1.2363</v>
-      </c>
-      <c r="C14" s="6">
-        <v>-1.2237</v>
-      </c>
+      <c r="A14" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="6">
-        <f t="shared" ref="D14:D20" si="1">ABS((B14-C14)/C14)</f>
-        <v>1.0296641333660166E-2</v>
+        <v>0.57550000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="6">
-        <v>-2.5068000000000001</v>
-      </c>
-      <c r="C15" s="6">
-        <v>-2.4157999999999999</v>
-      </c>
+      <c r="A15" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="6">
-        <f t="shared" si="1"/>
-        <v>3.7668681182217154E-2</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.69769999999999999</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0.63932999999999995</v>
-      </c>
+      <c r="A16" s="45" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="6">
-        <f t="shared" si="1"/>
-        <v>9.1298703330048706E-2</v>
+        <v>6.8210000000000007E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6">
-        <v>-0.3952</v>
-      </c>
-      <c r="C17" s="6">
-        <v>-0.40884999999999999</v>
-      </c>
+      <c r="A17" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="6">
-        <f t="shared" si="1"/>
-        <v>3.338632750397455E-2</v>
+        <v>0.14149999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="6">
-        <v>-1.7975000000000001</v>
-      </c>
-      <c r="C18" s="6">
-        <v>-1.88056</v>
-      </c>
+      <c r="A18" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
       <c r="D18" s="6">
-        <f t="shared" si="1"/>
-        <v>4.4167694729229545E-2</v>
+        <v>0.16889999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="6">
-        <v>-0.4667</v>
-      </c>
-      <c r="C19" s="6">
-        <v>-0.46009</v>
-      </c>
+      <c r="A19" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="6">
-        <f t="shared" si="1"/>
-        <v>1.4366754330674443E-2</v>
+        <v>0.44750000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="6">
-        <v>-0.31540000000000001</v>
-      </c>
-      <c r="C20" s="6">
-        <v>-0.24127999999999999</v>
-      </c>
+      <c r="A20" s="45" t="s">
+        <v>224</v>
+      </c>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="6">
-        <f t="shared" si="1"/>
-        <v>0.30719496021220166</v>
+        <v>0.33410000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="6">
+        <v>9.9729999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>202</v>
+      <c r="A22" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="6">
+        <v>0.78190000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="6">
-        <v>-0.95469999999999999</v>
-      </c>
-      <c r="C23" s="6">
-        <v>-0.99063000000000001</v>
-      </c>
+      <c r="A23" s="45" t="s">
+        <v>227</v>
+      </c>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="6">
-        <f>ABS((B23-C23)/C23)</f>
-        <v>3.6269848480260054E-2</v>
+        <v>0.96430000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24" s="6">
-        <v>-1.2494000000000001</v>
-      </c>
-      <c r="C24" s="6">
-        <v>-1.2237</v>
-      </c>
+      <c r="A24" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="6">
-        <f t="shared" ref="D24:D31" si="2">ABS((B24-C24)/C24)</f>
-        <v>2.1001879545640319E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="6">
-        <v>-2.5242</v>
-      </c>
-      <c r="C25" s="6">
-        <v>-2.4157999999999999</v>
-      </c>
-      <c r="D25" s="6">
-        <f t="shared" si="2"/>
-        <v>4.4871264177498163E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="6">
-        <v>0.70009999999999994</v>
-      </c>
-      <c r="C26" s="6">
-        <v>0.63932999999999995</v>
-      </c>
-      <c r="D26" s="6">
-        <f t="shared" si="2"/>
-        <v>9.5052633225407843E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="6">
-        <v>-0.3957</v>
-      </c>
-      <c r="C27" s="6">
-        <v>-0.40884999999999999</v>
-      </c>
-      <c r="D27" s="6">
-        <f t="shared" si="2"/>
-        <v>3.2163385104561563E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="6">
-        <v>-1.8623000000000001</v>
-      </c>
-      <c r="C28" s="6">
-        <v>-1.88056</v>
-      </c>
-      <c r="D28" s="6">
-        <f t="shared" si="2"/>
-        <v>9.7098736546560298E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="6">
-        <v>-0.49349999999999999</v>
-      </c>
-      <c r="C29" s="6">
-        <v>-0.46009</v>
-      </c>
-      <c r="D29" s="6">
-        <f t="shared" si="2"/>
-        <v>7.2616227259883925E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="6">
-        <v>-0.28670000000000001</v>
-      </c>
-      <c r="C30" s="6">
-        <v>-0.24127999999999999</v>
-      </c>
-      <c r="D30" s="6">
-        <f t="shared" si="2"/>
-        <v>0.18824602122015921</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0.22040000000000001</v>
-      </c>
-      <c r="C31" s="6">
-        <v>0.22370000000000001</v>
-      </c>
-      <c r="D31" s="6">
-        <f t="shared" si="2"/>
-        <v>1.4751899865891807E-2</v>
+        <v>0.85829999999999995</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="24">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First order interactions & modeling w/o quality of outfit predictor
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E63813B-C964-0E49-BE48-49BCD8986527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79CC47-AAEF-8243-A386-4C0670A783A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36720" yWindow="1660" windowWidth="23980" windowHeight="17500" activeTab="2" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
@@ -4909,7 +4909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B9891-AE0A-EC49-A442-8B89DE5C2A2B}">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q73" sqref="Q73"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Beta Estimates for Interaction Terms Added
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79CC47-AAEF-8243-A386-4C0670A783A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F086EB-DDD0-0A45-BA8F-15D5D33E0550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36720" yWindow="1660" windowWidth="23980" windowHeight="17500" activeTab="2" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
+    <workbookView xWindow="40180" yWindow="1640" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="RPDR Effect Estimates" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="264">
   <si>
     <t>Age</t>
   </si>
@@ -666,12 +666,6 @@
     <t>Outfit_Reveal:Expressed_Hardship</t>
   </si>
   <si>
-    <t>Gender:Outfit_Reveal</t>
-  </si>
-  <si>
-    <t>Gender:Quality_Of_Outfit</t>
-  </si>
-  <si>
     <t>Gender:Do_They_Know_Words</t>
   </si>
   <si>
@@ -687,9 +681,6 @@
     <t>B Estimate Comparisons (excluding Quality of Outfit Variable)</t>
   </si>
   <si>
-    <t>Quality_Of_Outfit:Outfit_Reveal</t>
-  </si>
-  <si>
     <t>Quality_Of_Outfit:Do_They_Know_Words</t>
   </si>
   <si>
@@ -790,6 +781,45 @@
   </si>
   <si>
     <t>delta b</t>
+  </si>
+  <si>
+    <t>summary(Model_6 &lt;- glm(OUTCOME_LOSS ~ Outfit_Reveal + Quality_Of_Outfit + Do_They_Know_Words + Gender + Sewing + Lip_Sync_Ass + Expressed_Hardship, family = binomial(link='logit'), data = Bottom_Two))</t>
+  </si>
+  <si>
+    <t>Preliminary Main Effects Model:</t>
+  </si>
+  <si>
+    <t>B Estimate</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender:Quality_Of_Outfit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference Levels </t>
+  </si>
+  <si>
+    <t>Quality of Outfit Boot</t>
+  </si>
+  <si>
+    <t>Outfit Reveal 0</t>
+  </si>
+  <si>
+    <t>Gender Cis</t>
+  </si>
+  <si>
+    <t>Do They Know Words 0</t>
+  </si>
+  <si>
+    <t>Sewing 0</t>
+  </si>
+  <si>
+    <t>Lip Sync Ass 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expressed Hardship 0 </t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1085,22 +1115,59 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1450,7 +1517,7 @@
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="H1" s="28" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
@@ -4022,7 +4089,7 @@
       <c r="D1" s="32"/>
       <c r="E1" s="33"/>
       <c r="H1" s="28" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
@@ -4909,8 +4976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B9891-AE0A-EC49-A442-8B89DE5C2A2B}">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q73" sqref="Q73"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4933,7 +5000,7 @@
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
       <c r="G1" s="34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H1" s="34"/>
       <c r="I1" s="34"/>
@@ -4993,13 +5060,13 @@
         <v>0.1379050489826677</v>
       </c>
       <c r="L3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="Q3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="S3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -5030,13 +5097,13 @@
         <v>5.2472736609294648E-2</v>
       </c>
       <c r="L4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q4" t="s">
         <v>241</v>
       </c>
-      <c r="Q4" t="s">
-        <v>244</v>
-      </c>
       <c r="S4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -5067,13 +5134,13 @@
         <v>3.615924678381563E-2</v>
       </c>
       <c r="L5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="Q5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="S5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -5104,7 +5171,7 @@
         <v>0.5494904810806539</v>
       </c>
       <c r="L6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -5135,13 +5202,13 @@
         <v>6.3018196442245711E-2</v>
       </c>
       <c r="L7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="Q7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="S7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -5172,13 +5239,13 @@
         <v>4.2997097242380357E-2</v>
       </c>
       <c r="L8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Q8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="S8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -5200,13 +5267,13 @@
       <c r="I9" s="36"/>
       <c r="J9" s="36"/>
       <c r="L9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="Q9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="S9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -5234,29 +5301,29 @@
       <c r="J12" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L12" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="M12" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="N12" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="O12" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q12" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="R12" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="S12" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="T12" s="47" t="s">
-        <v>253</v>
+      <c r="L12" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N12" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="O12" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q12" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="R12" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="S12" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="T12" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -5286,8 +5353,8 @@
         <f>ABS((H13-I13)/I13)</f>
         <v>0.12214265181907938</v>
       </c>
-      <c r="L13" s="49" t="s">
-        <v>237</v>
+      <c r="L13" s="46" t="s">
+        <v>234</v>
       </c>
       <c r="M13">
         <v>-0.76649999999999996</v>
@@ -5299,8 +5366,8 @@
         <f t="shared" ref="O13:O19" si="3">ABS((M13-N13)/N13)</f>
         <v>4.2030670016122443E-2</v>
       </c>
-      <c r="Q13" s="49" t="s">
-        <v>237</v>
+      <c r="Q13" s="46" t="s">
+        <v>234</v>
       </c>
       <c r="R13">
         <v>-0.77049999999999996</v>
@@ -5340,8 +5407,8 @@
         <f>ABS((H14-I14)/I14)</f>
         <v>0.149906500320969</v>
       </c>
-      <c r="L14" s="49" t="s">
-        <v>238</v>
+      <c r="L14" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="M14">
         <v>0.30830000000000002</v>
@@ -5349,12 +5416,12 @@
       <c r="N14" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="O14" s="48">
+      <c r="O14" s="45">
         <f t="shared" si="3"/>
         <v>0.33752711496746207</v>
       </c>
-      <c r="Q14" s="49" t="s">
-        <v>238</v>
+      <c r="Q14" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="R14">
         <v>0.30420000000000003</v>
@@ -5362,7 +5429,7 @@
       <c r="S14" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="T14" s="48">
+      <c r="T14" s="45">
         <f t="shared" si="4"/>
         <v>0.31973969631236449</v>
       </c>
@@ -5395,7 +5462,7 @@
         <v>3.278814059396145E-2</v>
       </c>
       <c r="L15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M15">
         <v>-0.39500000000000002</v>
@@ -5407,8 +5474,8 @@
         <f t="shared" si="3"/>
         <v>0.10245890200675437</v>
       </c>
-      <c r="Q15" s="49" t="s">
-        <v>244</v>
+      <c r="Q15" s="46" t="s">
+        <v>241</v>
       </c>
       <c r="R15">
         <v>0.20019999999999999</v>
@@ -5416,7 +5483,7 @@
       <c r="S15" s="13">
         <v>0.24659</v>
       </c>
-      <c r="T15" s="50">
+      <c r="T15" s="47">
         <f t="shared" si="4"/>
         <v>0.18812603917433804</v>
       </c>
@@ -5449,7 +5516,7 @@
         <v>4.7792973770004035E-2</v>
       </c>
       <c r="L16" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M16">
         <v>-2.3134000000000001</v>
@@ -5462,7 +5529,7 @@
         <v>4.2067378074873679E-2</v>
       </c>
       <c r="Q16" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="R16">
         <v>-0.41899999999999998</v>
@@ -5503,7 +5570,7 @@
         <v>0.55186033651947231</v>
       </c>
       <c r="L17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M17">
         <v>-0.68379999999999996</v>
@@ -5516,7 +5583,7 @@
         <v>7.4983428702839555E-2</v>
       </c>
       <c r="Q17" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="R17">
         <v>-2.3285999999999998</v>
@@ -5557,7 +5624,7 @@
         <v>6.0814570375552962E-2</v>
       </c>
       <c r="L18" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M18">
         <v>-0.37059999999999998</v>
@@ -5565,12 +5632,12 @@
       <c r="N18" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="O18" s="48">
+      <c r="O18" s="45">
         <f t="shared" si="3"/>
         <v>0.46378070937672788</v>
       </c>
       <c r="Q18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="R18">
         <v>-0.69</v>
@@ -5611,7 +5678,7 @@
         <v>8.5812772133526866E-2</v>
       </c>
       <c r="L19" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M19">
         <v>-1.6984999999999999</v>
@@ -5624,7 +5691,7 @@
         <v>6.4285281430594143E-2</v>
       </c>
       <c r="Q19" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="R19">
         <v>-0.34520000000000001</v>
@@ -5632,7 +5699,7 @@
       <c r="S19" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="T19" s="48">
+      <c r="T19" s="45">
         <f t="shared" si="4"/>
         <v>0.36345682913342281</v>
       </c>
@@ -5652,7 +5719,7 @@
         <v>0.30719496021220166</v>
       </c>
       <c r="L20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M20">
         <v>-0.5071</v>
@@ -5665,7 +5732,7 @@
         <v>8.0007256894049389E-2</v>
       </c>
       <c r="Q20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="R20">
         <v>-1.7601</v>
@@ -5684,7 +5751,7 @@
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
       <c r="Q21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R21">
         <v>-0.53420000000000001</v>
@@ -5722,29 +5789,29 @@
       <c r="J23" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L23" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="M23" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="N23" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="O23" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q23" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="R23" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="S23" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="T23" s="47" t="s">
-        <v>253</v>
+      <c r="L23" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="M23" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N23" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="O23" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q23" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="R23" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="S23" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="T23" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -5774,8 +5841,8 @@
         <f>ABS((H24-I24)/I24)</f>
         <v>0.11401897191706352</v>
       </c>
-      <c r="L24" s="49" t="s">
-        <v>237</v>
+      <c r="L24" s="46" t="s">
+        <v>234</v>
       </c>
       <c r="M24">
         <v>-0.70889999999999997</v>
@@ -5787,8 +5854,8 @@
         <f t="shared" ref="O24:O30" si="8">ABS((M24-N24)/N24)</f>
         <v>0.11401897191706352</v>
       </c>
-      <c r="Q24" s="49" t="s">
-        <v>237</v>
+      <c r="Q24" s="46" t="s">
+        <v>234</v>
       </c>
       <c r="R24">
         <v>-0.78459999999999996</v>
@@ -5828,8 +5895,8 @@
         <f>ABS((H25-I25)/I25)</f>
         <v>0.18123200454195226</v>
       </c>
-      <c r="L25" s="49" t="s">
-        <v>244</v>
+      <c r="L25" s="46" t="s">
+        <v>241</v>
       </c>
       <c r="M25">
         <v>0.2019</v>
@@ -5837,12 +5904,12 @@
       <c r="N25" s="13">
         <v>0.24659</v>
       </c>
-      <c r="O25" s="50">
+      <c r="O25" s="47">
         <f t="shared" si="8"/>
         <v>0.18123200454195226</v>
       </c>
-      <c r="Q25" s="49" t="s">
-        <v>238</v>
+      <c r="Q25" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="R25">
         <v>0.2853</v>
@@ -5850,7 +5917,7 @@
       <c r="S25" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="T25" s="48">
+      <c r="T25" s="45">
         <f t="shared" si="9"/>
         <v>0.2377440347071583</v>
       </c>
@@ -5878,12 +5945,12 @@
       <c r="I26" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="J26" s="46">
+      <c r="J26" s="43">
         <f>ABS((H26-I26)/I26)</f>
         <v>0.21605403444137425</v>
       </c>
       <c r="L26" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M26">
         <v>-0.43569999999999998</v>
@@ -5891,12 +5958,12 @@
       <c r="N26" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="O26" s="48">
+      <c r="O26" s="45">
         <f t="shared" si="8"/>
         <v>0.21605403444137425</v>
       </c>
-      <c r="Q26" s="49" t="s">
-        <v>243</v>
+      <c r="Q26" s="46" t="s">
+        <v>240</v>
       </c>
       <c r="R26">
         <v>-0.1608</v>
@@ -5904,7 +5971,7 @@
       <c r="S26" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="T26" s="48">
+      <c r="T26" s="45">
         <f t="shared" si="9"/>
         <v>0.37927041111754489</v>
       </c>
@@ -5937,7 +6004,7 @@
         <v>3.9589911757154359E-2</v>
       </c>
       <c r="L27" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M27">
         <v>-2.3079000000000001</v>
@@ -5950,7 +6017,7 @@
         <v>3.9589911757154359E-2</v>
       </c>
       <c r="Q27" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="R27">
         <v>-0.35389999999999999</v>
@@ -5991,7 +6058,7 @@
         <v>4.0893903115403987E-2</v>
       </c>
       <c r="L28" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M28">
         <v>-0.70899999999999996</v>
@@ -6004,7 +6071,7 @@
         <v>4.0893903115403987E-2</v>
       </c>
       <c r="Q28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="R28">
         <v>-2.2522000000000002</v>
@@ -6045,7 +6112,7 @@
         <v>0.45035152855675803</v>
       </c>
       <c r="L29" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M29">
         <v>-0.36720000000000003</v>
@@ -6053,12 +6120,12 @@
       <c r="N29" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="O29" s="48">
+      <c r="O29" s="45">
         <f t="shared" si="8"/>
         <v>0.45035152855675803</v>
       </c>
       <c r="Q29" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="R29">
         <v>-0.70269999999999999</v>
@@ -6099,7 +6166,7 @@
         <v>2.6603275690148229E-2</v>
       </c>
       <c r="L30" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M30">
         <v>-1.7668999999999999</v>
@@ -6112,7 +6179,7 @@
         <v>2.6603275690148229E-2</v>
       </c>
       <c r="Q30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="R30">
         <v>-0.35399999999999998</v>
@@ -6120,7 +6187,7 @@
       <c r="S30" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="T30" s="48">
+      <c r="T30" s="45">
         <f t="shared" si="9"/>
         <v>0.39821470890275679</v>
       </c>
@@ -6153,7 +6220,7 @@
         <v>3.7191582002902887E-2</v>
       </c>
       <c r="L31" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M31">
         <v>-0.53069999999999995</v>
@@ -6166,7 +6233,7 @@
         <v>3.7191582002902887E-2</v>
       </c>
       <c r="Q31" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="R31">
         <v>-1.6884999999999999</v>
@@ -6194,7 +6261,7 @@
         <v>1.4751899865891807E-2</v>
       </c>
       <c r="Q32" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R32">
         <v>-0.50160000000000005</v>
@@ -6212,7 +6279,7 @@
         <v>200</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I34" s="24" t="s">
         <v>199</v>
@@ -6220,29 +6287,29 @@
       <c r="J34" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L34" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="M34" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="N34" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="O34" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q34" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="R34" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="S34" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="T34" s="47" t="s">
-        <v>253</v>
+      <c r="L34" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="M34" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N34" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="O34" s="44" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q34" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="R34" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="S34" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="T34" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="7:20">
@@ -6259,8 +6326,8 @@
         <f>ABS((H35-I35)/I35)</f>
         <v>7.7149963130991289E-2</v>
       </c>
-      <c r="L35" s="49" t="s">
-        <v>237</v>
+      <c r="L35" s="46" t="s">
+        <v>234</v>
       </c>
       <c r="M35">
         <v>-0.7268</v>
@@ -6272,8 +6339,8 @@
         <f t="shared" ref="O35:O37" si="13">ABS((M35-N35)/N35)</f>
         <v>9.1647607263819639E-2</v>
       </c>
-      <c r="Q35" s="49" t="s">
-        <v>244</v>
+      <c r="Q35" s="46" t="s">
+        <v>241</v>
       </c>
       <c r="R35">
         <v>0.22509999999999999</v>
@@ -6300,8 +6367,8 @@
         <f>ABS((H36-I36)/I36)</f>
         <v>6.3222352893466852E-2</v>
       </c>
-      <c r="L36" s="49" t="s">
-        <v>243</v>
+      <c r="L36" s="46" t="s">
+        <v>240</v>
       </c>
       <c r="M36">
         <v>-0.17369999999999999</v>
@@ -6309,12 +6376,12 @@
       <c r="N36" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="O36" s="48">
+      <c r="O36" s="45">
         <f t="shared" si="13"/>
         <v>0.32947307469600468</v>
       </c>
-      <c r="Q36" s="49" t="s">
-        <v>238</v>
+      <c r="Q36" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="R36">
         <v>0.16500000000000001</v>
@@ -6322,7 +6389,7 @@
       <c r="S36" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="T36" s="48">
+      <c r="T36" s="45">
         <f t="shared" si="14"/>
         <v>0.2841648590021692</v>
       </c>
@@ -6337,12 +6404,12 @@
       <c r="I37" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="J37" s="46">
+      <c r="J37" s="43">
         <f>ABS((H37-I37)/I37)</f>
         <v>0.21057710866628071</v>
       </c>
       <c r="L37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M37">
         <v>-0.36630000000000001</v>
@@ -6350,12 +6417,12 @@
       <c r="N37" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="O37" s="50">
+      <c r="O37" s="47">
         <f t="shared" si="13"/>
         <v>2.2356191911580052E-2</v>
       </c>
-      <c r="Q37" s="49" t="s">
-        <v>243</v>
+      <c r="Q37" s="46" t="s">
+        <v>240</v>
       </c>
       <c r="R37">
         <v>-0.17549999999999999</v>
@@ -6363,7 +6430,7 @@
       <c r="S37" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="T37" s="48">
+      <c r="T37" s="45">
         <f t="shared" si="14"/>
         <v>0.32252460914881304</v>
       </c>
@@ -6383,7 +6450,7 @@
         <v>7.929330988863767E-2</v>
       </c>
       <c r="L38" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M38">
         <v>-2.2286000000000001</v>
@@ -6396,7 +6463,7 @@
         <v>3.869351939856271E-3</v>
       </c>
       <c r="Q38" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="R38">
         <v>-0.38030000000000003</v>
@@ -6424,7 +6491,7 @@
         <v>6.8873563632597373E-3</v>
       </c>
       <c r="L39" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M39">
         <v>-0.72309999999999997</v>
@@ -6437,7 +6504,7 @@
         <v>2.1820001893862653E-2</v>
       </c>
       <c r="Q39" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="R39">
         <v>-2.3028</v>
@@ -6465,7 +6532,7 @@
         <v>9.6451713269213642E-3</v>
       </c>
       <c r="L40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M40">
         <v>-0.37280000000000002</v>
@@ -6473,12 +6540,12 @@
       <c r="N40" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="O40" s="48">
+      <c r="O40" s="45">
         <f t="shared" ref="O40:O41" si="16">ABS((M40-N40)/N40)</f>
         <v>0.47247017931906155</v>
       </c>
       <c r="Q40" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="R40">
         <v>-0.72819999999999996</v>
@@ -6506,7 +6573,7 @@
         <v>0.34410300971640717</v>
       </c>
       <c r="L41" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M41">
         <v>-1.6936</v>
@@ -6519,7 +6586,7 @@
         <v>6.6984723362292692E-2</v>
       </c>
       <c r="Q41" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="R41">
         <v>-0.33300000000000002</v>
@@ -6527,7 +6594,7 @@
       <c r="S41" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="T41" s="48">
+      <c r="T41" s="45">
         <f t="shared" si="14"/>
         <v>0.31526976854411881</v>
       </c>
@@ -6547,7 +6614,7 @@
         <v>2.8861992408508286E-2</v>
       </c>
       <c r="L42" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M42">
         <v>-0.49869999999999998</v>
@@ -6560,7 +6627,7 @@
         <v>9.5246734397677876E-2</v>
       </c>
       <c r="Q42" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="R42">
         <v>-1.7545999999999999</v>
@@ -6588,7 +6655,7 @@
         <v>4.1545718432510939E-2</v>
       </c>
       <c r="Q43" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R43">
         <v>-0.55549999999999999</v>
@@ -6602,22 +6669,22 @@
       </c>
     </row>
     <row r="44" spans="7:20">
-      <c r="L44" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="M44" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="N44" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="O44" s="47" t="s">
-        <v>253</v>
+      <c r="L44" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="M44" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N44" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="O44" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="7:20">
-      <c r="L45" s="49" t="s">
-        <v>238</v>
+      <c r="L45" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="M45">
         <v>0.19220000000000001</v>
@@ -6625,7 +6692,7 @@
       <c r="N45" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="O45" s="50">
+      <c r="O45" s="47">
         <f t="shared" ref="O45:O50" si="18">ABS((M45-N45)/N45)</f>
         <v>0.16616052060737527</v>
       </c>
@@ -6635,7 +6702,7 @@
         <v>200</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I46" s="24" t="s">
         <v>199</v>
@@ -6644,7 +6711,7 @@
         <v>201</v>
       </c>
       <c r="L46" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M46">
         <v>-0.39689999999999998</v>
@@ -6672,7 +6739,7 @@
         <v>9.9108894804594162E-3</v>
       </c>
       <c r="L47" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M47">
         <v>-2.3517999999999999</v>
@@ -6700,7 +6767,7 @@
         <v>7.7415953607202215E-2</v>
       </c>
       <c r="L48" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M48">
         <v>-0.70020000000000004</v>
@@ -6728,7 +6795,7 @@
         <v>0.26114649681528668</v>
       </c>
       <c r="L49" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M49">
         <v>-0.37780000000000002</v>
@@ -6736,14 +6803,14 @@
       <c r="N49" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="O49" s="48">
+      <c r="O49" s="45">
         <f t="shared" si="18"/>
         <v>0.49221897464254682</v>
       </c>
     </row>
     <row r="50" spans="7:15">
       <c r="G50" s="39" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H50" s="13">
         <v>0.2757</v>
@@ -6756,7 +6823,7 @@
         <v>0.19609544468546633</v>
       </c>
       <c r="L50" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M50">
         <v>-1.6970000000000001</v>
@@ -6784,7 +6851,7 @@
         <v>4.5521784029696588E-2</v>
       </c>
       <c r="L51" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M51">
         <v>-0.53100000000000003</v>
@@ -6841,17 +6908,17 @@
         <f>ABS((H54-I54)/I54)</f>
         <v>0.27379729836479971</v>
       </c>
-      <c r="L54" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="M54" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="N54" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="O54" s="47" t="s">
-        <v>253</v>
+      <c r="L54" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="M54" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N54" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="O54" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="7:15">
@@ -6868,8 +6935,8 @@
         <f t="shared" ref="J55:J56" si="20">ABS((H55-I55)/I55)</f>
         <v>3.2222522160214713E-2</v>
       </c>
-      <c r="L55" s="49" t="s">
-        <v>238</v>
+      <c r="L55" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="M55">
         <v>0.16889999999999999</v>
@@ -6877,7 +6944,7 @@
       <c r="N55" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="O55" s="50">
+      <c r="O55" s="47">
         <f t="shared" ref="O55:O59" si="21">ABS((M55-N55)/N55)</f>
         <v>0.26724511930585687</v>
       </c>
@@ -6896,8 +6963,8 @@
         <f t="shared" si="20"/>
         <v>3.6284470246734431E-2</v>
       </c>
-      <c r="L56" s="49" t="s">
-        <v>243</v>
+      <c r="L56" s="46" t="s">
+        <v>240</v>
       </c>
       <c r="M56">
         <v>-0.14510000000000001</v>
@@ -6905,14 +6972,14 @@
       <c r="N56" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="O56" s="48">
+      <c r="O56" s="45">
         <f t="shared" si="21"/>
         <v>0.43987647172360544</v>
       </c>
     </row>
     <row r="57" spans="7:15">
       <c r="L57" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M57">
         <v>-0.35870000000000002</v>
@@ -6927,7 +6994,7 @@
     </row>
     <row r="58" spans="7:15">
       <c r="L58" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M58">
         <v>-2.2966000000000002</v>
@@ -6945,7 +7012,7 @@
         <v>200</v>
       </c>
       <c r="H59" s="24" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I59" s="24" t="s">
         <v>199</v>
@@ -6954,7 +7021,7 @@
         <v>201</v>
       </c>
       <c r="L59" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M59">
         <v>-0.7177</v>
@@ -6980,7 +7047,7 @@
         <v>1</v>
       </c>
       <c r="L60" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M60">
         <v>-0.36280000000000001</v>
@@ -6988,7 +7055,7 @@
       <c r="N60" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="O60" s="48">
+      <c r="O60" s="45">
         <f>ABS((M60-N60)/N60)</f>
         <v>0.43297258867209093</v>
       </c>
@@ -7006,7 +7073,7 @@
         <v>1</v>
       </c>
       <c r="L61" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M61">
         <v>-1.6861999999999999</v>
@@ -7032,7 +7099,7 @@
         <v>1</v>
       </c>
       <c r="L62" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M62">
         <v>-0.52659999999999996</v>
@@ -7047,7 +7114,7 @@
     </row>
     <row r="63" spans="7:15">
       <c r="G63" s="39" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H63" s="13"/>
       <c r="I63" s="13">
@@ -7060,7 +7127,7 @@
     </row>
     <row r="64" spans="7:15">
       <c r="G64" s="39" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
@@ -7078,17 +7145,17 @@
         <f>ABS((H65-I65)/I65)</f>
         <v>1</v>
       </c>
-      <c r="L65" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="M65" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="N65" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="O65" s="47" t="s">
-        <v>253</v>
+      <c r="L65" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="M65" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N65" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="O65" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="7:15">
@@ -7103,8 +7170,8 @@
         <f t="shared" ref="J66:J67" si="22">ABS((H66-I66)/I66)</f>
         <v>1</v>
       </c>
-      <c r="L66" s="49" t="s">
-        <v>238</v>
+      <c r="L66" s="46" t="s">
+        <v>235</v>
       </c>
       <c r="M66">
         <v>0.19309999999999999</v>
@@ -7112,7 +7179,7 @@
       <c r="N66" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="O66" s="50">
+      <c r="O66" s="47">
         <f t="shared" ref="O66:O69" si="23">ABS((M66-N66)/N66)</f>
         <v>0.16225596529284173</v>
       </c>
@@ -7129,8 +7196,8 @@
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="L67" s="49" t="s">
-        <v>244</v>
+      <c r="L67" s="46" t="s">
+        <v>241</v>
       </c>
       <c r="M67">
         <v>0.19980000000000001</v>
@@ -7138,7 +7205,7 @@
       <c r="N67" s="13">
         <v>0.24659</v>
       </c>
-      <c r="O67" s="50">
+      <c r="O67" s="47">
         <f>ABS((M67-N67)/N67)</f>
         <v>0.18974816497019342</v>
       </c>
@@ -7156,7 +7223,7 @@
         <v>1</v>
       </c>
       <c r="L68" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M68">
         <v>-0.42209999999999998</v>
@@ -7164,7 +7231,7 @@
       <c r="N68" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="O68" s="50">
+      <c r="O68" s="47">
         <f>ABS((M68-N68)/N68)</f>
         <v>0.17809595579000245</v>
       </c>
@@ -7182,7 +7249,7 @@
         <v>1</v>
       </c>
       <c r="L69" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M69">
         <v>-2.367</v>
@@ -7190,7 +7257,7 @@
       <c r="N69" s="6">
         <v>-2.2200099999999998</v>
       </c>
-      <c r="O69" s="50">
+      <c r="O69" s="47">
         <f t="shared" si="23"/>
         <v>6.6211413462101604E-2</v>
       </c>
@@ -7208,7 +7275,7 @@
         <v>1</v>
       </c>
       <c r="L70" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M70">
         <v>-0.70640000000000003</v>
@@ -7223,7 +7290,7 @@
     </row>
     <row r="71" spans="7:15">
       <c r="L71" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M71">
         <v>-0.35389999999999999</v>
@@ -7231,14 +7298,14 @@
       <c r="N71" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="O71" s="48">
+      <c r="O71" s="45">
         <f t="shared" si="25"/>
         <v>0.39781973299628709</v>
       </c>
     </row>
     <row r="72" spans="7:15">
       <c r="L72" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M72">
         <v>-1.7597</v>
@@ -7253,7 +7320,7 @@
     </row>
     <row r="73" spans="7:15">
       <c r="L73" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M73">
         <v>-0.5575</v>
@@ -7267,22 +7334,22 @@
       </c>
     </row>
     <row r="75" spans="7:15">
-      <c r="L75" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="M75" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="N75" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="O75" s="47" t="s">
-        <v>253</v>
+      <c r="L75" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="M75" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="N75" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="O75" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="76" spans="7:15">
-      <c r="L76" s="49" t="s">
-        <v>243</v>
+      <c r="L76" s="46" t="s">
+        <v>240</v>
       </c>
       <c r="M76">
         <v>-0.184</v>
@@ -7290,14 +7357,14 @@
       <c r="N76" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="O76" s="48">
+      <c r="O76" s="45">
         <f t="shared" ref="O76" si="26">ABS((M76-N76)/N76)</f>
         <v>0.28971241073151904</v>
       </c>
     </row>
     <row r="77" spans="7:15">
-      <c r="L77" s="49" t="s">
-        <v>244</v>
+      <c r="L77" s="46" t="s">
+        <v>241</v>
       </c>
       <c r="M77">
         <v>0.22589999999999999</v>
@@ -7305,14 +7372,14 @@
       <c r="N77" s="13">
         <v>0.24659</v>
       </c>
-      <c r="O77" s="50">
+      <c r="O77" s="47">
         <f>ABS((M77-N77)/N77)</f>
         <v>8.3904456790624166E-2</v>
       </c>
     </row>
     <row r="78" spans="7:15">
       <c r="L78" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M78">
         <v>-0.38719999999999999</v>
@@ -7320,14 +7387,14 @@
       <c r="N78" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="O78" s="50">
+      <c r="O78" s="47">
         <f>ABS((M78-N78)/N78)</f>
         <v>8.068882748611457E-2</v>
       </c>
     </row>
     <row r="79" spans="7:15">
       <c r="L79" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M79">
         <v>-2.2867000000000002</v>
@@ -7335,14 +7402,14 @@
       <c r="N79" s="6">
         <v>-2.2200099999999998</v>
       </c>
-      <c r="O79" s="50">
+      <c r="O79" s="47">
         <f t="shared" ref="O79:O82" si="27">ABS((M79-N79)/N79)</f>
         <v>3.0040405223400058E-2</v>
       </c>
     </row>
     <row r="80" spans="7:15">
       <c r="L80" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M80">
         <v>-0.73929999999999996</v>
@@ -7357,7 +7424,7 @@
     </row>
     <row r="81" spans="12:15">
       <c r="L81" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M81">
         <v>-0.34420000000000001</v>
@@ -7365,14 +7432,14 @@
       <c r="N81" s="35">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="O81" s="48">
+      <c r="O81" s="45">
         <f t="shared" si="27"/>
         <v>0.35950707006872573</v>
       </c>
     </row>
     <row r="82" spans="12:15">
       <c r="L82" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M82">
         <v>-1.7575000000000001</v>
@@ -7387,7 +7454,7 @@
     </row>
     <row r="83" spans="12:15">
       <c r="L83" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M83">
         <v>-0.5524</v>
@@ -7411,282 +7478,411 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F618E10-1DFA-C44A-B66A-2018A4130538}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:14">
       <c r="A1" s="34" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
-    </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" customHeight="1">
+      <c r="A2" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2" s="41" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="43" t="s">
+      <c r="G2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16" customHeight="1">
+      <c r="A3" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44">
-        <v>9.4030000000000006E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="45" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65">
+        <v>1.2506999999999999</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="57" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="6">
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="50">
+        <v>-14.5717</v>
+      </c>
+      <c r="E4" s="6">
         <v>0.16550000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="45" t="s">
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="6">
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="61" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5" s="42">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="45" t="s">
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="57" t="s">
         <v>209</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="6">
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="50">
+        <v>0.436</v>
+      </c>
+      <c r="E6" s="6">
         <v>0.75860000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="45" t="s">
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="6">
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="50">
+        <v>-14.1897</v>
+      </c>
+      <c r="E7" s="6">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="45" t="s">
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="6">
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="50">
+        <v>0.13270000000000001</v>
+      </c>
+      <c r="E8" s="6">
         <v>0.94099999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="45" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="50">
+        <v>-1.3482000000000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.29599999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="6">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="45" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="61" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="57" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="6">
-        <v>0.29599999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="45" t="s">
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="50">
+        <v>-0.44040000000000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.7409</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="57" t="s">
         <v>214</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="45" t="s">
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="50">
+        <v>-0.60709999999999997</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.6431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="6">
-        <v>0.7409</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="6">
-        <v>0.6431</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="45" t="s">
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="50">
+        <v>-0.71689999999999998</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.57550000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="57" t="s">
         <v>217</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="6">
-        <v>0.57550000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="45" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="50">
+        <v>-16.180800000000001</v>
+      </c>
+      <c r="E14" s="6">
+        <v>6.8210000000000007E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="50">
+        <v>-0.89485999999999999</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.14149999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="57" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="6">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="45" t="s">
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="50">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.16889999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="57" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="6">
-        <v>6.8210000000000007E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="45" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="50">
+        <v>0.47910000000000003</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.44750000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="6">
-        <v>0.14149999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="45" t="s">
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="50">
+        <v>14.4727</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.33410000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="57" t="s">
         <v>222</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="6">
-        <v>0.16889999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="45" t="s">
+      <c r="B19" s="58"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="50">
+        <v>-16.2044</v>
+      </c>
+      <c r="E19" s="6">
+        <v>9.9729999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="57" t="s">
         <v>223</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="6">
-        <v>0.44750000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="45" t="s">
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="50">
+        <v>11.651999999999999</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.78190000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="57" t="s">
         <v>224</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="6">
-        <v>0.33410000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="45" t="s">
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="50">
+        <v>2.673E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.96430000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="6">
-        <v>9.9729999999999999E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="45" t="s">
-        <v>226</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="6">
-        <v>0.78190000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="45" t="s">
-        <v>227</v>
-      </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="6">
-        <v>0.96430000000000005</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="6">
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="50">
+        <v>0.1087</v>
+      </c>
+      <c r="E22" s="6">
         <v>0.85829999999999995</v>
       </c>
     </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="60" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
+  <mergeCells count="23">
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G3:N7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Beta Estimates For First Order Interaction Terms Added
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F086EB-DDD0-0A45-BA8F-15D5D33E0550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1352DC9D-EE6C-4846-8413-9A6AE40E5EC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40180" yWindow="1640" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
+    <workbookView xWindow="40180" yWindow="1620" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="RPDR Effect Estimates" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Beta comparisons for model without quality of outfit
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAF044D-5C09-5C4A-9410-12DA16678183}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A799DD-B13A-F743-BEC7-50C9200AC318}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40180" yWindow="1620" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
+    <workbookView xWindow="3020" yWindow="500" windowWidth="23980" windowHeight="17500" activeTab="2" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="RPDR Effect Estimates" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="247">
   <si>
     <t>Age</t>
   </si>
@@ -642,9 +642,6 @@
     <t>Model 4</t>
   </si>
   <si>
-    <t xml:space="preserve">B Estimate Comparisons </t>
-  </si>
-  <si>
     <t>Interactions</t>
   </si>
   <si>
@@ -678,9 +675,6 @@
     <t>Gender:Expressed_Hardship</t>
   </si>
   <si>
-    <t>B Estimate Comparisons (excluding Quality of Outfit Variable)</t>
-  </si>
-  <si>
     <t>Quality_Of_Outfit:Do_They_Know_Words</t>
   </si>
   <si>
@@ -726,63 +720,6 @@
     <t>Model 1</t>
   </si>
   <si>
-    <t>Body Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tried </t>
-  </si>
-  <si>
-    <t xml:space="preserve">outfit reveal </t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>carson</t>
-  </si>
-  <si>
-    <t>eliminated variables</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>body type</t>
-  </si>
-  <si>
-    <t>ross</t>
-  </si>
-  <si>
-    <t>dancing</t>
-  </si>
-  <si>
-    <t>outfit reveal</t>
-  </si>
-  <si>
-    <t>do they know words</t>
-  </si>
-  <si>
-    <t>sewing</t>
-  </si>
-  <si>
-    <t>singing</t>
-  </si>
-  <si>
-    <t>lip sync ass</t>
-  </si>
-  <si>
-    <t>expressed hardship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model </t>
-  </si>
-  <si>
-    <t>full model</t>
-  </si>
-  <si>
-    <t>delta b</t>
-  </si>
-  <si>
     <t>summary(Model_6 &lt;- glm(OUTCOME_LOSS ~ Outfit_Reveal + Quality_Of_Outfit + Do_They_Know_Words + Gender + Sewing + Lip_Sync_Ass + Expressed_Hardship, family = binomial(link='logit'), data = Bottom_Two))</t>
   </si>
   <si>
@@ -820,13 +757,25 @@
   </si>
   <si>
     <t xml:space="preserve">Expressed Hardship 0 </t>
+  </si>
+  <si>
+    <t>B Estimate Comparisons For Bottom Two</t>
+  </si>
+  <si>
+    <t>B Estimate Comparisons For Bottom Two (excluding Quality of Outfit)</t>
+  </si>
+  <si>
+    <t>Body Type (Thick n Juicy)</t>
+  </si>
+  <si>
+    <t>Body Type (Chunky Yet Funky)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -865,13 +814,6 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -945,7 +887,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1018,20 +960,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1118,10 +1051,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1517,7 +1446,7 @@
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
       <c r="H1" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
@@ -4089,7 +4018,7 @@
       <c r="D1" s="32"/>
       <c r="E1" s="33"/>
       <c r="H1" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
@@ -4974,10 +4903,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B9891-AE0A-EC49-A442-8B89DE5C2A2B}">
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4986,27 +4915,27 @@
     <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="12" max="12" width="21.5" customWidth="1"/>
     <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:10">
       <c r="A1" s="34" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
       <c r="G1" s="34" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="H1" s="34"/>
       <c r="I1" s="34"/>
       <c r="J1" s="34"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:10">
       <c r="A2" s="24" t="s">
         <v>200</v>
       </c>
@@ -5032,7 +4961,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:10">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -5059,17 +4988,8 @@
         <f>ABS((H3-I3)/I3)</f>
         <v>0.1379050489826677</v>
       </c>
-      <c r="L3" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>242</v>
-      </c>
-      <c r="S3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="6" t="s">
         <v>131</v>
       </c>
@@ -5096,17 +5016,8 @@
         <f t="shared" ref="J4:J5" si="1">ABS((H4-I4)/I4)</f>
         <v>5.2472736609294648E-2</v>
       </c>
-      <c r="L4" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>241</v>
-      </c>
-      <c r="S4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -5133,17 +5044,8 @@
         <f t="shared" si="1"/>
         <v>3.615924678381563E-2</v>
       </c>
-      <c r="L5" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>240</v>
-      </c>
-      <c r="S5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="6" t="s">
         <v>134</v>
       </c>
@@ -5170,11 +5072,8 @@
         <f>ABS((H6-I6)/I6)</f>
         <v>0.5494904810806539</v>
       </c>
-      <c r="L6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -5201,17 +5100,8 @@
         <f t="shared" ref="J7:J8" si="2">ABS((H7-I7)/I7)</f>
         <v>6.3018196442245711E-2</v>
       </c>
-      <c r="L7" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>242</v>
-      </c>
-      <c r="S7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -5238,17 +5128,8 @@
         <f t="shared" si="2"/>
         <v>4.2997097242380357E-2</v>
       </c>
-      <c r="L8" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>241</v>
-      </c>
-      <c r="S8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
@@ -5266,17 +5147,8 @@
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
       <c r="J9" s="36"/>
-      <c r="L9" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>235</v>
-      </c>
-      <c r="S9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="24" t="s">
         <v>200</v>
       </c>
@@ -5301,32 +5173,8 @@
       <c r="J12" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L12" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="M12" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="N12" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="O12" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q12" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="R12" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="S12" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="T12" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -5353,34 +5201,8 @@
         <f>ABS((H13-I13)/I13)</f>
         <v>0.12214265181907938</v>
       </c>
-      <c r="L13" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="M13">
-        <v>-0.76649999999999996</v>
-      </c>
-      <c r="N13" s="13">
-        <v>-0.80013000000000001</v>
-      </c>
-      <c r="O13">
-        <f t="shared" ref="O13:O19" si="3">ABS((M13-N13)/N13)</f>
-        <v>4.2030670016122443E-2</v>
-      </c>
-      <c r="Q13" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="R13">
-        <v>-0.77049999999999996</v>
-      </c>
-      <c r="S13" s="13">
-        <v>-0.80013000000000001</v>
-      </c>
-      <c r="T13">
-        <f t="shared" ref="T13:T20" si="4">ABS((R13-S13)/S13)</f>
-        <v>3.7031482384112635E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="6" t="s">
         <v>131</v>
       </c>
@@ -5391,7 +5213,7 @@
         <v>-1.2237</v>
       </c>
       <c r="D14" s="6">
-        <f t="shared" ref="D14:D20" si="5">ABS((B14-C14)/C14)</f>
+        <f t="shared" ref="D14:D20" si="3">ABS((B14-C14)/C14)</f>
         <v>1.0296641333660166E-2</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -5407,34 +5229,8 @@
         <f>ABS((H14-I14)/I14)</f>
         <v>0.149906500320969</v>
       </c>
-      <c r="L14" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="M14">
-        <v>0.30830000000000002</v>
-      </c>
-      <c r="N14" s="13">
-        <v>0.23050000000000001</v>
-      </c>
-      <c r="O14" s="45">
-        <f t="shared" si="3"/>
-        <v>0.33752711496746207</v>
-      </c>
-      <c r="Q14" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="R14">
-        <v>0.30420000000000003</v>
-      </c>
-      <c r="S14" s="13">
-        <v>0.23050000000000001</v>
-      </c>
-      <c r="T14" s="45">
-        <f t="shared" si="4"/>
-        <v>0.31973969631236449</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -5445,7 +5241,7 @@
         <v>-2.4157999999999999</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3.7668681182217154E-2</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -5458,37 +5254,11 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" ref="J15:J16" si="6">ABS((H15-I15)/I15)</f>
+        <f t="shared" ref="J15:J16" si="4">ABS((H15-I15)/I15)</f>
         <v>3.278814059396145E-2</v>
       </c>
-      <c r="L15" t="s">
-        <v>236</v>
-      </c>
-      <c r="M15">
-        <v>-0.39500000000000002</v>
-      </c>
-      <c r="N15" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="3"/>
-        <v>0.10245890200675437</v>
-      </c>
-      <c r="Q15" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="R15">
-        <v>0.20019999999999999</v>
-      </c>
-      <c r="S15" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="T15" s="47">
-        <f t="shared" si="4"/>
-        <v>0.18812603917433804</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="6" t="s">
         <v>134</v>
       </c>
@@ -5499,7 +5269,7 @@
         <v>0.63932999999999995</v>
       </c>
       <c r="D16" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>9.1298703330048706E-2</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -5512,37 +5282,11 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.7792973770004035E-2</v>
       </c>
-      <c r="L16" t="s">
-        <v>243</v>
-      </c>
-      <c r="M16">
-        <v>-2.3134000000000001</v>
-      </c>
-      <c r="N16" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="3"/>
-        <v>4.2067378074873679E-2</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>236</v>
-      </c>
-      <c r="R16">
-        <v>-0.41899999999999998</v>
-      </c>
-      <c r="S16" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="4"/>
-        <v>0.16944374668564566</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
@@ -5553,7 +5297,7 @@
         <v>-0.40884999999999999</v>
       </c>
       <c r="D17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3.338632750397455E-2</v>
       </c>
       <c r="G17" s="35" t="s">
@@ -5569,34 +5313,8 @@
         <f>ABS((H17-I17)/I17)</f>
         <v>0.55186033651947231</v>
       </c>
-      <c r="L17" t="s">
-        <v>244</v>
-      </c>
-      <c r="M17">
-        <v>-0.68379999999999996</v>
-      </c>
-      <c r="N17" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="3"/>
-        <v>7.4983428702839555E-2</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>243</v>
-      </c>
-      <c r="R17">
-        <v>-2.3285999999999998</v>
-      </c>
-      <c r="S17" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="4"/>
-        <v>4.8914194080206835E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -5607,7 +5325,7 @@
         <v>-1.88056</v>
       </c>
       <c r="D18" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4.4167694729229545E-2</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -5620,37 +5338,11 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" ref="J18:J19" si="7">ABS((H18-I18)/I18)</f>
+        <f t="shared" ref="J18:J19" si="5">ABS((H18-I18)/I18)</f>
         <v>6.0814570375552962E-2</v>
       </c>
-      <c r="L18" t="s">
-        <v>245</v>
-      </c>
-      <c r="M18">
-        <v>-0.37059999999999998</v>
-      </c>
-      <c r="N18" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="O18" s="45">
-        <f t="shared" si="3"/>
-        <v>0.46378070937672788</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>244</v>
-      </c>
-      <c r="R18">
-        <v>-0.69</v>
-      </c>
-      <c r="S18" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="4"/>
-        <v>6.6596323201168928E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -5661,7 +5353,7 @@
         <v>-0.46009</v>
       </c>
       <c r="D19" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.4366754330674443E-2</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -5674,37 +5366,11 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J19" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8.5812772133526866E-2</v>
       </c>
-      <c r="L19" t="s">
-        <v>246</v>
-      </c>
-      <c r="M19">
-        <v>-1.6984999999999999</v>
-      </c>
-      <c r="N19" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="3"/>
-        <v>6.4285281430594143E-2</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>245</v>
-      </c>
-      <c r="R19">
-        <v>-0.34520000000000001</v>
-      </c>
-      <c r="S19" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="T19" s="45">
-        <f t="shared" si="4"/>
-        <v>0.36345682913342281</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="26" t="s">
         <v>22</v>
       </c>
@@ -5715,56 +5381,17 @@
         <v>-0.24127999999999999</v>
       </c>
       <c r="D20" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.30719496021220166</v>
       </c>
-      <c r="L20" t="s">
-        <v>247</v>
-      </c>
-      <c r="M20">
-        <v>-0.5071</v>
-      </c>
-      <c r="N20" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="O20">
-        <f>ABS((M20-N20)/N20)</f>
-        <v>8.0007256894049389E-2</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>246</v>
-      </c>
-      <c r="R20">
-        <v>-1.7601</v>
-      </c>
-      <c r="S20" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="T20">
-        <f t="shared" si="4"/>
-        <v>3.0349440003525845E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="40"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
-      <c r="Q21" t="s">
-        <v>247</v>
-      </c>
-      <c r="R21">
-        <v>-0.53420000000000001</v>
-      </c>
-      <c r="S21" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="T21">
-        <f>ABS((R21-S21)/S21)</f>
-        <v>3.0841799709724265E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="24" t="s">
         <v>200</v>
       </c>
@@ -5789,32 +5416,8 @@
       <c r="J23" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L23" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="M23" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="N23" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="O23" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q23" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="R23" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="S23" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="T23" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -5841,34 +5444,8 @@
         <f>ABS((H24-I24)/I24)</f>
         <v>0.11401897191706352</v>
       </c>
-      <c r="L24" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="M24">
-        <v>-0.70889999999999997</v>
-      </c>
-      <c r="N24" s="13">
-        <v>-0.80013000000000001</v>
-      </c>
-      <c r="O24">
-        <f t="shared" ref="O24:O30" si="8">ABS((M24-N24)/N24)</f>
-        <v>0.11401897191706352</v>
-      </c>
-      <c r="Q24" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="R24">
-        <v>-0.78459999999999996</v>
-      </c>
-      <c r="S24" s="13">
-        <v>-0.80013000000000001</v>
-      </c>
-      <c r="T24">
-        <f t="shared" ref="T24:T31" si="9">ABS((R24-S24)/S24)</f>
-        <v>1.9409345981278098E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="6" t="s">
         <v>131</v>
       </c>
@@ -5879,7 +5456,7 @@
         <v>-1.2237</v>
       </c>
       <c r="D25" s="6">
-        <f t="shared" ref="D25:D32" si="10">ABS((B25-C25)/C25)</f>
+        <f t="shared" ref="D25:D32" si="6">ABS((B25-C25)/C25)</f>
         <v>2.1001879545640319E-2</v>
       </c>
       <c r="G25" s="39" t="s">
@@ -5895,34 +5472,8 @@
         <f>ABS((H25-I25)/I25)</f>
         <v>0.18123200454195226</v>
       </c>
-      <c r="L25" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="M25">
-        <v>0.2019</v>
-      </c>
-      <c r="N25" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="O25" s="47">
-        <f t="shared" si="8"/>
-        <v>0.18123200454195226</v>
-      </c>
-      <c r="Q25" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="R25">
-        <v>0.2853</v>
-      </c>
-      <c r="S25" s="13">
-        <v>0.23050000000000001</v>
-      </c>
-      <c r="T25" s="45">
-        <f t="shared" si="9"/>
-        <v>0.2377440347071583</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="6" t="s">
         <v>11</v>
       </c>
@@ -5933,7 +5484,7 @@
         <v>-2.4157999999999999</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>4.4871264177498163E-2</v>
       </c>
       <c r="G26" s="6" t="s">
@@ -5949,34 +5500,8 @@
         <f>ABS((H26-I26)/I26)</f>
         <v>0.21605403444137425</v>
       </c>
-      <c r="L26" t="s">
-        <v>236</v>
-      </c>
-      <c r="M26">
-        <v>-0.43569999999999998</v>
-      </c>
-      <c r="N26" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="O26" s="45">
-        <f t="shared" si="8"/>
-        <v>0.21605403444137425</v>
-      </c>
-      <c r="Q26" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="R26">
-        <v>-0.1608</v>
-      </c>
-      <c r="S26" s="13">
-        <v>-0.25905</v>
-      </c>
-      <c r="T26" s="45">
-        <f t="shared" si="9"/>
-        <v>0.37927041111754489</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -5987,7 +5512,7 @@
         <v>0.63932999999999995</v>
       </c>
       <c r="D27" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>9.5052633225407843E-2</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -6000,37 +5525,11 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J27" s="6">
-        <f t="shared" ref="J27:J28" si="11">ABS((H27-I27)/I27)</f>
+        <f t="shared" ref="J27:J28" si="7">ABS((H27-I27)/I27)</f>
         <v>3.9589911757154359E-2</v>
       </c>
-      <c r="L27" t="s">
-        <v>243</v>
-      </c>
-      <c r="M27">
-        <v>-2.3079000000000001</v>
-      </c>
-      <c r="N27" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="O27">
-        <f>ABS((M27-N27)/N27)</f>
-        <v>3.9589911757154359E-2</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>236</v>
-      </c>
-      <c r="R27">
-        <v>-0.35389999999999999</v>
-      </c>
-      <c r="S27" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="T27">
-        <f t="shared" si="9"/>
-        <v>1.2252644505847232E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -6041,7 +5540,7 @@
         <v>-0.40884999999999999</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>3.2163385104561563E-2</v>
       </c>
       <c r="G28" s="6" t="s">
@@ -6054,37 +5553,11 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J28" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>4.0893903115403987E-2</v>
       </c>
-      <c r="L28" t="s">
-        <v>244</v>
-      </c>
-      <c r="M28">
-        <v>-0.70899999999999996</v>
-      </c>
-      <c r="N28" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="O28">
-        <f>ABS((M28-N28)/N28)</f>
-        <v>4.0893903115403987E-2</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>243</v>
-      </c>
-      <c r="R28">
-        <v>-2.2522000000000002</v>
-      </c>
-      <c r="S28" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="9"/>
-        <v>1.4499934684979071E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -6095,7 +5568,7 @@
         <v>-1.88056</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>9.7098736546560298E-3</v>
       </c>
       <c r="G29" s="35" t="s">
@@ -6111,34 +5584,8 @@
         <f>ABS((H29-I29)/I29)</f>
         <v>0.45035152855675803</v>
       </c>
-      <c r="L29" t="s">
-        <v>245</v>
-      </c>
-      <c r="M29">
-        <v>-0.36720000000000003</v>
-      </c>
-      <c r="N29" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="O29" s="45">
-        <f t="shared" si="8"/>
-        <v>0.45035152855675803</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>244</v>
-      </c>
-      <c r="R29">
-        <v>-0.70269999999999999</v>
-      </c>
-      <c r="S29" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="9"/>
-        <v>4.9416284512262841E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -6149,7 +5596,7 @@
         <v>-0.46009</v>
       </c>
       <c r="D30" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>7.2616227259883925E-2</v>
       </c>
       <c r="G30" s="6" t="s">
@@ -6162,37 +5609,11 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J30" s="6">
-        <f t="shared" ref="J30" si="12">ABS((H30-I30)/I30)</f>
+        <f t="shared" ref="J30" si="8">ABS((H30-I30)/I30)</f>
         <v>2.6603275690148229E-2</v>
       </c>
-      <c r="L30" t="s">
-        <v>246</v>
-      </c>
-      <c r="M30">
-        <v>-1.7668999999999999</v>
-      </c>
-      <c r="N30" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="8"/>
-        <v>2.6603275690148229E-2</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>245</v>
-      </c>
-      <c r="R30">
-        <v>-0.35399999999999998</v>
-      </c>
-      <c r="S30" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="T30" s="45">
-        <f t="shared" si="9"/>
-        <v>0.39821470890275679</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="26" t="s">
         <v>22</v>
       </c>
@@ -6203,7 +5624,7 @@
         <v>-0.24127999999999999</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0.18824602122015921</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -6219,34 +5640,8 @@
         <f>ABS((H31-I31)/I31)</f>
         <v>3.7191582002902887E-2</v>
       </c>
-      <c r="L31" t="s">
-        <v>247</v>
-      </c>
-      <c r="M31">
-        <v>-0.53069999999999995</v>
-      </c>
-      <c r="N31" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="O31">
-        <f>ABS((M31-N31)/N31)</f>
-        <v>3.7191582002902887E-2</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>246</v>
-      </c>
-      <c r="R31">
-        <v>-1.6884999999999999</v>
-      </c>
-      <c r="S31" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="9"/>
-        <v>6.9794346597326001E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="26" t="s">
         <v>21</v>
       </c>
@@ -6257,29 +5652,16 @@
         <v>0.22370000000000001</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>1.4751899865891807E-2</v>
       </c>
-      <c r="Q32" t="s">
-        <v>247</v>
-      </c>
-      <c r="R32">
-        <v>-0.50160000000000005</v>
-      </c>
-      <c r="S32" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="T32">
-        <f>ABS((R32-S32)/S32)</f>
-        <v>8.9985486211901264E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="7:20">
+    </row>
+    <row r="34" spans="7:10">
       <c r="G34" s="24" t="s">
         <v>200</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I34" s="24" t="s">
         <v>199</v>
@@ -6287,32 +5669,8 @@
       <c r="J34" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L34" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="M34" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="N34" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="O34" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q34" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="R34" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="S34" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="T34" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="35" spans="7:20">
+    </row>
+    <row r="35" spans="7:10">
       <c r="G35" s="39" t="s">
         <v>17</v>
       </c>
@@ -6326,34 +5684,8 @@
         <f>ABS((H35-I35)/I35)</f>
         <v>7.7149963130991289E-2</v>
       </c>
-      <c r="L35" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="M35">
-        <v>-0.7268</v>
-      </c>
-      <c r="N35" s="13">
-        <v>-0.80013000000000001</v>
-      </c>
-      <c r="O35">
-        <f t="shared" ref="O35:O37" si="13">ABS((M35-N35)/N35)</f>
-        <v>9.1647607263819639E-2</v>
-      </c>
-      <c r="Q35" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="R35">
-        <v>0.22509999999999999</v>
-      </c>
-      <c r="S35" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="T35">
-        <f t="shared" ref="T35:T42" si="14">ABS((R35-S35)/S35)</f>
-        <v>8.7148708382335086E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="7:20">
+    </row>
+    <row r="36" spans="7:10">
       <c r="G36" s="39" t="s">
         <v>6</v>
       </c>
@@ -6367,34 +5699,8 @@
         <f>ABS((H36-I36)/I36)</f>
         <v>6.3222352893466852E-2</v>
       </c>
-      <c r="L36" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="M36">
-        <v>-0.17369999999999999</v>
-      </c>
-      <c r="N36" s="13">
-        <v>-0.25905</v>
-      </c>
-      <c r="O36" s="45">
-        <f t="shared" si="13"/>
-        <v>0.32947307469600468</v>
-      </c>
-      <c r="Q36" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="R36">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="S36" s="13">
-        <v>0.23050000000000001</v>
-      </c>
-      <c r="T36" s="45">
-        <f t="shared" si="14"/>
-        <v>0.2841648590021692</v>
-      </c>
-    </row>
-    <row r="37" spans="7:20">
+    </row>
+    <row r="37" spans="7:10">
       <c r="G37" s="39" t="s">
         <v>175</v>
       </c>
@@ -6408,34 +5714,8 @@
         <f>ABS((H37-I37)/I37)</f>
         <v>0.21057710866628071</v>
       </c>
-      <c r="L37" t="s">
-        <v>236</v>
-      </c>
-      <c r="M37">
-        <v>-0.36630000000000001</v>
-      </c>
-      <c r="N37" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="O37" s="47">
-        <f t="shared" si="13"/>
-        <v>2.2356191911580052E-2</v>
-      </c>
-      <c r="Q37" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="R37">
-        <v>-0.17549999999999999</v>
-      </c>
-      <c r="S37" s="13">
-        <v>-0.25905</v>
-      </c>
-      <c r="T37" s="45">
-        <f t="shared" si="14"/>
-        <v>0.32252460914881304</v>
-      </c>
-    </row>
-    <row r="38" spans="7:20">
+    </row>
+    <row r="38" spans="7:10">
       <c r="G38" s="6" t="s">
         <v>12</v>
       </c>
@@ -6449,34 +5729,8 @@
         <f>ABS((H38-I38)/I38)</f>
         <v>7.929330988863767E-2</v>
       </c>
-      <c r="L38" t="s">
-        <v>243</v>
-      </c>
-      <c r="M38">
-        <v>-2.2286000000000001</v>
-      </c>
-      <c r="N38" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="O38">
-        <f>ABS((M38-N38)/N38)</f>
-        <v>3.869351939856271E-3</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>236</v>
-      </c>
-      <c r="R38">
-        <v>-0.38030000000000003</v>
-      </c>
-      <c r="S38" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="T38">
-        <f t="shared" si="14"/>
-        <v>6.1430684640933403E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="7:20">
+    </row>
+    <row r="39" spans="7:10">
       <c r="G39" s="6" t="s">
         <v>11</v>
       </c>
@@ -6487,37 +5741,11 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J39" s="6">
-        <f t="shared" ref="J39:J40" si="15">ABS((H39-I39)/I39)</f>
+        <f t="shared" ref="J39:J40" si="9">ABS((H39-I39)/I39)</f>
         <v>6.8873563632597373E-3</v>
       </c>
-      <c r="L39" t="s">
-        <v>244</v>
-      </c>
-      <c r="M39">
-        <v>-0.72309999999999997</v>
-      </c>
-      <c r="N39" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="O39">
-        <f>ABS((M39-N39)/N39)</f>
-        <v>2.1820001893862653E-2</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>243</v>
-      </c>
-      <c r="R39">
-        <v>-2.3028</v>
-      </c>
-      <c r="S39" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="T39">
-        <f t="shared" si="14"/>
-        <v>3.729262480799643E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="7:20">
+    </row>
+    <row r="40" spans="7:10">
       <c r="G40" s="6" t="s">
         <v>20</v>
       </c>
@@ -6528,37 +5756,11 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J40" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9.6451713269213642E-3</v>
       </c>
-      <c r="L40" t="s">
-        <v>245</v>
-      </c>
-      <c r="M40">
-        <v>-0.37280000000000002</v>
-      </c>
-      <c r="N40" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="O40" s="45">
-        <f t="shared" ref="O40:O41" si="16">ABS((M40-N40)/N40)</f>
-        <v>0.47247017931906155</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>244</v>
-      </c>
-      <c r="R40">
-        <v>-0.72819999999999996</v>
-      </c>
-      <c r="S40" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="T40">
-        <f t="shared" si="14"/>
-        <v>1.4920931239262603E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="7:20">
+    </row>
+    <row r="41" spans="7:10">
       <c r="G41" s="35" t="s">
         <v>22</v>
       </c>
@@ -6572,34 +5774,8 @@
         <f>ABS((H41-I41)/I41)</f>
         <v>0.34410300971640717</v>
       </c>
-      <c r="L41" t="s">
-        <v>246</v>
-      </c>
-      <c r="M41">
-        <v>-1.6936</v>
-      </c>
-      <c r="N41" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="O41">
-        <f t="shared" si="16"/>
-        <v>6.6984723362292692E-2</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>245</v>
-      </c>
-      <c r="R41">
-        <v>-0.33300000000000002</v>
-      </c>
-      <c r="S41" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="T41" s="45">
-        <f t="shared" si="14"/>
-        <v>0.31526976854411881</v>
-      </c>
-    </row>
-    <row r="42" spans="7:20">
+    </row>
+    <row r="42" spans="7:10">
       <c r="G42" s="6" t="s">
         <v>23</v>
       </c>
@@ -6610,37 +5786,11 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J42" s="6">
-        <f t="shared" ref="J42:J43" si="17">ABS((H42-I42)/I42)</f>
+        <f t="shared" ref="J42:J43" si="10">ABS((H42-I42)/I42)</f>
         <v>2.8861992408508286E-2</v>
       </c>
-      <c r="L42" t="s">
-        <v>247</v>
-      </c>
-      <c r="M42">
-        <v>-0.49869999999999998</v>
-      </c>
-      <c r="N42" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="O42">
-        <f>ABS((M42-N42)/N42)</f>
-        <v>9.5246734397677876E-2</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>246</v>
-      </c>
-      <c r="R42">
-        <v>-1.7545999999999999</v>
-      </c>
-      <c r="S42" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="T42">
-        <f t="shared" si="14"/>
-        <v>3.3379425845228398E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="7:20">
+    </row>
+    <row r="43" spans="7:10">
       <c r="G43" s="6" t="s">
         <v>24</v>
       </c>
@@ -6651,58 +5801,16 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J43" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="10"/>
         <v>4.1545718432510939E-2</v>
       </c>
-      <c r="Q43" t="s">
-        <v>247</v>
-      </c>
-      <c r="R43">
-        <v>-0.55549999999999999</v>
-      </c>
-      <c r="S43" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="T43">
-        <f>ABS((R43-S43)/S43)</f>
-        <v>7.801161103047842E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="7:20">
-      <c r="L44" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="M44" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="N44" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="O44" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="45" spans="7:20">
-      <c r="L45" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="M45">
-        <v>0.19220000000000001</v>
-      </c>
-      <c r="N45" s="13">
-        <v>0.23050000000000001</v>
-      </c>
-      <c r="O45" s="47">
-        <f t="shared" ref="O45:O50" si="18">ABS((M45-N45)/N45)</f>
-        <v>0.16616052060737527</v>
-      </c>
-    </row>
-    <row r="46" spans="7:20">
+    </row>
+    <row r="46" spans="7:10">
       <c r="G46" s="24" t="s">
         <v>200</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I46" s="24" t="s">
         <v>199</v>
@@ -6710,21 +5818,8 @@
       <c r="J46" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L46" t="s">
-        <v>236</v>
-      </c>
-      <c r="M46">
-        <v>-0.39689999999999998</v>
-      </c>
-      <c r="N46" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="O46">
-        <f t="shared" si="18"/>
-        <v>0.10776186887716648</v>
-      </c>
-    </row>
-    <row r="47" spans="7:20">
+    </row>
+    <row r="47" spans="7:10">
       <c r="G47" s="39" t="s">
         <v>17</v>
       </c>
@@ -6738,21 +5833,8 @@
         <f>ABS((H47-I47)/I47)</f>
         <v>9.9108894804594162E-3</v>
       </c>
-      <c r="L47" t="s">
-        <v>243</v>
-      </c>
-      <c r="M47">
-        <v>-2.3517999999999999</v>
-      </c>
-      <c r="N47" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="O47">
-        <f t="shared" si="18"/>
-        <v>5.9364597456768253E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="7:20">
+    </row>
+    <row r="48" spans="7:10">
       <c r="G48" s="39" t="s">
         <v>6</v>
       </c>
@@ -6766,21 +5848,8 @@
         <f>ABS((H48-I48)/I48)</f>
         <v>7.7415953607202215E-2</v>
       </c>
-      <c r="L48" t="s">
-        <v>244</v>
-      </c>
-      <c r="M48">
-        <v>-0.70020000000000004</v>
-      </c>
-      <c r="N48" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="O48">
-        <f t="shared" si="18"/>
-        <v>5.2798181891968679E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="7:15">
+    </row>
+    <row r="49" spans="7:10">
       <c r="G49" s="39" t="s">
         <v>175</v>
       </c>
@@ -6794,23 +5863,10 @@
         <f>ABS((H49-I49)/I49)</f>
         <v>0.26114649681528668</v>
       </c>
-      <c r="L49" t="s">
-        <v>245</v>
-      </c>
-      <c r="M49">
-        <v>-0.37780000000000002</v>
-      </c>
-      <c r="N49" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="O49" s="45">
-        <f t="shared" si="18"/>
-        <v>0.49221897464254682</v>
-      </c>
-    </row>
-    <row r="50" spans="7:15">
+    </row>
+    <row r="50" spans="7:10">
       <c r="G50" s="39" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H50" s="13">
         <v>0.2757</v>
@@ -6822,21 +5878,8 @@
         <f>ABS((H50-I50)/I50)</f>
         <v>0.19609544468546633</v>
       </c>
-      <c r="L50" t="s">
-        <v>246</v>
-      </c>
-      <c r="M50">
-        <v>-1.6970000000000001</v>
-      </c>
-      <c r="N50" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="O50">
-        <f t="shared" si="18"/>
-        <v>6.5111641205603824E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="7:15">
+    </row>
+    <row r="51" spans="7:10">
       <c r="G51" s="6" t="s">
         <v>12</v>
       </c>
@@ -6850,21 +5893,8 @@
         <f>ABS((H51-I51)/I51)</f>
         <v>4.5521784029696588E-2</v>
       </c>
-      <c r="L51" t="s">
-        <v>247</v>
-      </c>
-      <c r="M51">
-        <v>-0.53100000000000003</v>
-      </c>
-      <c r="N51" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="O51">
-        <f>ABS((M51-N51)/N51)</f>
-        <v>3.6647314949201731E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="7:15">
+    </row>
+    <row r="52" spans="7:10">
       <c r="G52" s="6" t="s">
         <v>11</v>
       </c>
@@ -6875,11 +5905,11 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J52" s="8">
-        <f t="shared" ref="J52:J53" si="19">ABS((H52-I52)/I52)</f>
+        <f t="shared" ref="J52:J53" si="11">ABS((H52-I52)/I52)</f>
         <v>1.7292714897680708E-2</v>
       </c>
     </row>
-    <row r="53" spans="7:15">
+    <row r="53" spans="7:10">
       <c r="G53" s="6" t="s">
         <v>20</v>
       </c>
@@ -6890,11 +5920,11 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J53" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>3.521231551749808E-2</v>
       </c>
     </row>
-    <row r="54" spans="7:15">
+    <row r="54" spans="7:10">
       <c r="G54" s="35" t="s">
         <v>22</v>
       </c>
@@ -6908,20 +5938,8 @@
         <f>ABS((H54-I54)/I54)</f>
         <v>0.27379729836479971</v>
       </c>
-      <c r="L54" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="M54" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="N54" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="O54" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="55" spans="7:15">
+    </row>
+    <row r="55" spans="7:10">
       <c r="G55" s="6" t="s">
         <v>23</v>
       </c>
@@ -6932,24 +5950,11 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J55" s="6">
-        <f t="shared" ref="J55:J56" si="20">ABS((H55-I55)/I55)</f>
+        <f t="shared" ref="J55:J56" si="12">ABS((H55-I55)/I55)</f>
         <v>3.2222522160214713E-2</v>
       </c>
-      <c r="L55" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="M55">
-        <v>0.16889999999999999</v>
-      </c>
-      <c r="N55" s="13">
-        <v>0.23050000000000001</v>
-      </c>
-      <c r="O55" s="47">
-        <f t="shared" ref="O55:O59" si="21">ABS((M55-N55)/N55)</f>
-        <v>0.26724511930585687</v>
-      </c>
-    </row>
-    <row r="56" spans="7:15">
+    </row>
+    <row r="56" spans="7:10">
       <c r="G56" s="6" t="s">
         <v>24</v>
       </c>
@@ -6960,59 +5965,16 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J56" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="12"/>
         <v>3.6284470246734431E-2</v>
       </c>
-      <c r="L56" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="M56">
-        <v>-0.14510000000000001</v>
-      </c>
-      <c r="N56" s="13">
-        <v>-0.25905</v>
-      </c>
-      <c r="O56" s="45">
-        <f t="shared" si="21"/>
-        <v>0.43987647172360544</v>
-      </c>
-    </row>
-    <row r="57" spans="7:15">
-      <c r="L57" t="s">
-        <v>236</v>
-      </c>
-      <c r="M57">
-        <v>-0.35870000000000002</v>
-      </c>
-      <c r="N57" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="O57">
-        <f t="shared" si="21"/>
-        <v>1.1443244299311213E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="7:15">
-      <c r="L58" t="s">
-        <v>243</v>
-      </c>
-      <c r="M58">
-        <v>-2.2966000000000002</v>
-      </c>
-      <c r="N58" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="O58">
-        <f t="shared" si="21"/>
-        <v>3.4499844595294787E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="7:15">
+    </row>
+    <row r="59" spans="7:10">
       <c r="G59" s="24" t="s">
         <v>200</v>
       </c>
       <c r="H59" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I59" s="24" t="s">
         <v>199</v>
@@ -7020,451 +5982,439 @@
       <c r="J59" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="L59" t="s">
-        <v>244</v>
-      </c>
-      <c r="M59">
-        <v>-0.7177</v>
-      </c>
-      <c r="N59" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="O59">
-        <f t="shared" si="21"/>
-        <v>2.9124900234027362E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="7:15">
+    </row>
+    <row r="60" spans="7:10">
       <c r="G60" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="H60" s="13"/>
+      <c r="H60" s="13">
+        <v>-0.80789999999999995</v>
+      </c>
       <c r="I60" s="13">
         <v>-0.80013000000000001</v>
       </c>
       <c r="J60" s="6">
         <f>ABS((H60-I60)/I60)</f>
-        <v>1</v>
-      </c>
-      <c r="L60" t="s">
-        <v>245</v>
-      </c>
-      <c r="M60">
-        <v>-0.36280000000000001</v>
-      </c>
-      <c r="N60" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="O60" s="45">
-        <f>ABS((M60-N60)/N60)</f>
-        <v>0.43297258867209093</v>
-      </c>
-    </row>
-    <row r="61" spans="7:15">
+        <v>9.7109219751789627E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="7:10">
       <c r="G61" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H61" s="13"/>
+      <c r="H61" s="13">
+        <v>0.26939999999999997</v>
+      </c>
       <c r="I61" s="13">
         <v>0.24659</v>
       </c>
       <c r="J61" s="6">
         <f>ABS((H61-I61)/I61)</f>
-        <v>1</v>
-      </c>
-      <c r="L61" t="s">
-        <v>246</v>
-      </c>
-      <c r="M61">
-        <v>-1.6861999999999999</v>
-      </c>
-      <c r="N61" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="O61">
-        <f>ABS((M61-N61)/N61)</f>
-        <v>7.1061431585674309E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="7:15">
+        <v>9.2501723508657971E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="7:10">
       <c r="G62" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="H62" s="13"/>
+      <c r="H62" s="13">
+        <v>-0.21590000000000001</v>
+      </c>
       <c r="I62" s="13">
         <v>-0.25905</v>
       </c>
       <c r="J62" s="8">
         <f>ABS((H62-I62)/I62)</f>
-        <v>1</v>
-      </c>
-      <c r="L62" t="s">
-        <v>247</v>
-      </c>
-      <c r="M62">
-        <v>-0.52659999999999996</v>
-      </c>
-      <c r="N62" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="O62">
-        <f>ABS((M62-N62)/N62)</f>
-        <v>4.4629898403483428E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="7:15">
+        <v>0.16657016020073342</v>
+      </c>
+    </row>
+    <row r="63" spans="7:10">
       <c r="G63" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="H63" s="13"/>
+        <v>228</v>
+      </c>
+      <c r="H63" s="13">
+        <v>0.26889999999999997</v>
+      </c>
       <c r="I63" s="13">
         <v>0.23050000000000001</v>
       </c>
       <c r="J63" s="8">
         <f>ABS((H63-I63)/I63)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="7:15">
+        <v>0.16659436008676773</v>
+      </c>
+    </row>
+    <row r="64" spans="7:10">
       <c r="G64" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="8"/>
-    </row>
-    <row r="65" spans="7:15">
-      <c r="G65" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="H64" s="13">
+        <v>0.28620000000000001</v>
+      </c>
+      <c r="I64" s="13">
+        <v>0.30564000000000002</v>
+      </c>
+      <c r="J64" s="8">
+        <f t="shared" ref="J64:J65" si="13">ABS((H64-I64)/I64)</f>
+        <v>6.3604240282685548E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="7:10">
+      <c r="G65" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="H65" s="13">
+        <v>0.1125</v>
+      </c>
+      <c r="I65" s="13">
+        <v>0.15532000000000001</v>
+      </c>
+      <c r="J65" s="43">
+        <f t="shared" si="13"/>
+        <v>0.27568890033479271</v>
+      </c>
+    </row>
+    <row r="66" spans="7:10">
+      <c r="G66" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6">
+      <c r="H66" s="6">
+        <v>-0.37290000000000001</v>
+      </c>
+      <c r="I66" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="J65" s="8">
-        <f>ABS((H65-I65)/I65)</f>
-        <v>1</v>
-      </c>
-      <c r="L65" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="M65" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="N65" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="O65" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="66" spans="7:15">
-      <c r="G66" s="6" t="s">
+      <c r="J66" s="8">
+        <f>ABS((H66-I66)/I66)</f>
+        <v>4.0777024198275176E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="7:10">
+      <c r="G67" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6">
+      <c r="H67" s="6">
+        <v>-2.2570000000000001</v>
+      </c>
+      <c r="I67" s="6">
         <v>-2.2200099999999998</v>
       </c>
-      <c r="J66" s="8">
-        <f t="shared" ref="J66:J67" si="22">ABS((H66-I66)/I66)</f>
-        <v>1</v>
-      </c>
-      <c r="L66" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="M66">
-        <v>0.19309999999999999</v>
-      </c>
-      <c r="N66" s="13">
+      <c r="J67" s="8">
+        <f t="shared" ref="J67:J68" si="14">ABS((H67-I67)/I67)</f>
+        <v>1.6662087107715867E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="7:10">
+      <c r="G68" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" s="6">
+        <v>-0.71109999999999995</v>
+      </c>
+      <c r="I68" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J68" s="8">
+        <f t="shared" si="14"/>
+        <v>3.8053109316451034E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="7:10">
+      <c r="G69" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H69" s="37">
+        <v>-0.30740000000000001</v>
+      </c>
+      <c r="I69" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J69" s="38">
+        <f>ABS((H69-I69)/I69)</f>
+        <v>0.21415593648787418</v>
+      </c>
+    </row>
+    <row r="70" spans="7:10">
+      <c r="G70" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="6">
+        <v>-1.7656000000000001</v>
+      </c>
+      <c r="I70" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J70" s="6">
+        <f t="shared" ref="J70:J71" si="15">ABS((H70-I70)/I70)</f>
+        <v>2.7319454161823291E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="7:10">
+      <c r="G71" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H71" s="6">
+        <v>-0.55810000000000004</v>
+      </c>
+      <c r="I71" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J71" s="6">
+        <f t="shared" si="15"/>
+        <v>1.2518142235123398E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="7:10">
+      <c r="G73" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H73" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="I73" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="J73" s="25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="7:10">
+      <c r="G74" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="I74" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J74" s="8">
+        <f t="shared" ref="J74:J89" si="16">ABS((H74-I74)/I74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="7:10">
+      <c r="G75" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H75" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="I75" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="J75" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="7:10">
+      <c r="G76" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="H76" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="I76" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="J76" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="7:10">
+      <c r="G77" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="H77" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="O66" s="47">
-        <f t="shared" ref="O66:O69" si="23">ABS((M66-N66)/N66)</f>
-        <v>0.16225596529284173</v>
-      </c>
-    </row>
-    <row r="67" spans="7:15">
-      <c r="G67" s="6" t="s">
+      <c r="I77" s="13">
+        <v>0.23050000000000001</v>
+      </c>
+      <c r="J77" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="7:10">
+      <c r="G78" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="H78" s="13">
+        <v>0.30564000000000002</v>
+      </c>
+      <c r="I78" s="13">
+        <v>0.30564000000000002</v>
+      </c>
+      <c r="J78" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="7:10">
+      <c r="G79" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="H79" s="13">
+        <v>0.15532000000000001</v>
+      </c>
+      <c r="I79" s="13">
+        <v>0.15532000000000001</v>
+      </c>
+      <c r="J79" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="7:10">
+      <c r="G80" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="H80" s="13">
+        <v>0.26494000000000001</v>
+      </c>
+      <c r="I80" s="13">
+        <v>0.26494000000000001</v>
+      </c>
+      <c r="J80" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="7:10">
+      <c r="G81" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="H81" s="13">
+        <v>0.29258000000000001</v>
+      </c>
+      <c r="I81" s="13">
+        <v>0.29258000000000001</v>
+      </c>
+      <c r="J81" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="7:10">
+      <c r="G82" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H82" s="13">
+        <v>-5.5890000000000002E-2</v>
+      </c>
+      <c r="I82" s="13">
+        <v>-5.5890000000000002E-2</v>
+      </c>
+      <c r="J82" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="7:10">
+      <c r="G83" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="H83" s="13">
+        <v>-0.12130000000000001</v>
+      </c>
+      <c r="I83" s="13">
+        <v>-0.12130000000000001</v>
+      </c>
+      <c r="J83" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="7:10">
+      <c r="G84" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H84" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="I84" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J84" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="7:10">
+      <c r="G85" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="I85" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J85" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="7:10">
+      <c r="G86" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6">
+      <c r="H86" s="6">
         <v>-0.73923000000000005</v>
       </c>
-      <c r="J67" s="8">
-        <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-      <c r="L67" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="M67">
-        <v>0.19980000000000001</v>
-      </c>
-      <c r="N67" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="O67" s="47">
-        <f>ABS((M67-N67)/N67)</f>
-        <v>0.18974816497019342</v>
-      </c>
-    </row>
-    <row r="68" spans="7:15">
-      <c r="G68" s="35" t="s">
+      <c r="I86" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J86" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="7:10">
+      <c r="G87" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="H68" s="37"/>
-      <c r="I68" s="35">
+      <c r="H87" s="37">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="J68" s="38">
-        <f>ABS((H68-I68)/I68)</f>
-        <v>1</v>
-      </c>
-      <c r="L68" t="s">
-        <v>236</v>
-      </c>
-      <c r="M68">
-        <v>-0.42209999999999998</v>
-      </c>
-      <c r="N68" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="O68" s="47">
-        <f>ABS((M68-N68)/N68)</f>
-        <v>0.17809595579000245</v>
-      </c>
-    </row>
-    <row r="69" spans="7:15">
-      <c r="G69" s="6" t="s">
+      <c r="I87" s="35">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J87" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="7:10">
+      <c r="G88" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6">
+      <c r="H88" s="6">
         <v>-1.8151900000000001</v>
       </c>
-      <c r="J69" s="6">
-        <f t="shared" ref="J69:J70" si="24">ABS((H69-I69)/I69)</f>
-        <v>1</v>
-      </c>
-      <c r="L69" t="s">
-        <v>243</v>
-      </c>
-      <c r="M69">
-        <v>-2.367</v>
-      </c>
-      <c r="N69" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="O69" s="47">
-        <f t="shared" si="23"/>
-        <v>6.6211413462101604E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="7:15">
-      <c r="G70" s="6" t="s">
+      <c r="I88" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J88" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="7:10">
+      <c r="G89" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6">
+      <c r="H89" s="6">
         <v>-0.55120000000000002</v>
       </c>
-      <c r="J70" s="6">
-        <f t="shared" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="L70" t="s">
-        <v>244</v>
-      </c>
-      <c r="M70">
-        <v>-0.70640000000000003</v>
-      </c>
-      <c r="N70" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="O70">
-        <f t="shared" ref="O70:O72" si="25">ABS((M70-N70)/N70)</f>
-        <v>4.4411076390298045E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="7:15">
-      <c r="L71" t="s">
-        <v>245</v>
-      </c>
-      <c r="M71">
-        <v>-0.35389999999999999</v>
-      </c>
-      <c r="N71" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="O71" s="45">
-        <f t="shared" si="25"/>
-        <v>0.39781973299628709</v>
-      </c>
-    </row>
-    <row r="72" spans="7:15">
-      <c r="L72" t="s">
-        <v>246</v>
-      </c>
-      <c r="M72">
-        <v>-1.7597</v>
-      </c>
-      <c r="N72" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="O72">
-        <f t="shared" si="25"/>
-        <v>3.0569802610195096E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="7:15">
-      <c r="L73" t="s">
-        <v>247</v>
-      </c>
-      <c r="M73">
-        <v>-0.5575</v>
-      </c>
-      <c r="N73" s="6">
+      <c r="I89" s="6">
         <v>-0.55120000000000002</v>
       </c>
-      <c r="O73">
-        <f>ABS((M73-N73)/N73)</f>
-        <v>1.1429608127721284E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="7:15">
-      <c r="L75" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="M75" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="N75" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="O75" s="44" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="76" spans="7:15">
-      <c r="L76" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="M76">
-        <v>-0.184</v>
-      </c>
-      <c r="N76" s="13">
-        <v>-0.25905</v>
-      </c>
-      <c r="O76" s="45">
-        <f t="shared" ref="O76" si="26">ABS((M76-N76)/N76)</f>
-        <v>0.28971241073151904</v>
-      </c>
-    </row>
-    <row r="77" spans="7:15">
-      <c r="L77" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="M77">
-        <v>0.22589999999999999</v>
-      </c>
-      <c r="N77" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="O77" s="47">
-        <f>ABS((M77-N77)/N77)</f>
-        <v>8.3904456790624166E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="7:15">
-      <c r="L78" t="s">
-        <v>236</v>
-      </c>
-      <c r="M78">
-        <v>-0.38719999999999999</v>
-      </c>
-      <c r="N78" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="O78" s="47">
-        <f>ABS((M78-N78)/N78)</f>
-        <v>8.068882748611457E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="7:15">
-      <c r="L79" t="s">
-        <v>243</v>
-      </c>
-      <c r="M79">
-        <v>-2.2867000000000002</v>
-      </c>
-      <c r="N79" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="O79" s="47">
-        <f t="shared" ref="O79:O82" si="27">ABS((M79-N79)/N79)</f>
-        <v>3.0040405223400058E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="7:15">
-      <c r="L80" t="s">
-        <v>244</v>
-      </c>
-      <c r="M80">
-        <v>-0.73929999999999996</v>
-      </c>
-      <c r="N80" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="O80">
-        <f>ABS((M80-N80)/N80)</f>
-        <v>9.4693126631634902E-5</v>
-      </c>
-    </row>
-    <row r="81" spans="12:15">
-      <c r="L81" t="s">
-        <v>245</v>
-      </c>
-      <c r="M81">
-        <v>-0.34420000000000001</v>
-      </c>
-      <c r="N81" s="35">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="O81" s="45">
-        <f t="shared" si="27"/>
-        <v>0.35950707006872573</v>
-      </c>
-    </row>
-    <row r="82" spans="12:15">
-      <c r="L82" t="s">
-        <v>246</v>
-      </c>
-      <c r="M82">
-        <v>-1.7575000000000001</v>
-      </c>
-      <c r="N82" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="O82">
-        <f t="shared" si="27"/>
-        <v>3.1781796946876092E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="12:15">
-      <c r="L83" t="s">
-        <v>247</v>
-      </c>
-      <c r="M83">
-        <v>-0.5524</v>
-      </c>
-      <c r="N83" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="O83">
-        <f>ABS((M83-N83)/N83)</f>
-        <v>2.1770682148040256E-3</v>
+      <c r="J89" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7480,8 +6430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F618E10-1DFA-C44A-B66A-2018A4130538}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7493,7 +6443,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -7501,135 +6451,135 @@
       <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1">
-      <c r="A2" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="49" t="s">
-        <v>253</v>
+      <c r="A2" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="45" t="s">
+        <v>232</v>
       </c>
       <c r="E2" s="41" t="s">
         <v>182</v>
       </c>
       <c r="G2" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1">
-      <c r="A3" s="62" t="s">
-        <v>206</v>
-      </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65">
+      <c r="A3" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="61">
         <v>1.2506999999999999</v>
       </c>
       <c r="E3" s="8">
         <v>0.47</v>
       </c>
-      <c r="G3" s="48" t="s">
-        <v>251</v>
-      </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
+      <c r="G3" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="57" t="s">
-        <v>207</v>
-      </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="50">
+      <c r="A4" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="46">
         <v>-14.5717</v>
       </c>
       <c r="E4" s="6">
         <v>0.16550000000000001</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="54" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="61" t="s">
-        <v>254</v>
+      <c r="A5" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="57" t="s">
+        <v>233</v>
       </c>
       <c r="E5" s="42">
         <v>0</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="57" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="50">
+      <c r="A6" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="46">
         <v>0.436</v>
       </c>
       <c r="E6" s="6">
         <v>0.75860000000000005</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="57" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="50">
+      <c r="A7" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="46">
         <v>-14.1897</v>
       </c>
       <c r="E7" s="6">
         <v>0.24</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="57" t="s">
-        <v>211</v>
-      </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="50">
+      <c r="A8" s="53" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="54"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="46">
         <v>0.13270000000000001</v>
       </c>
       <c r="E8" s="6">
@@ -7637,12 +6587,12 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="57" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="50">
+      <c r="A9" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="46">
         <v>-1.3482000000000001</v>
       </c>
       <c r="E9" s="6">
@@ -7650,25 +6600,25 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="61" t="s">
-        <v>254</v>
+      <c r="A10" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="57" t="s">
+        <v>233</v>
       </c>
       <c r="E10" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="50">
+      <c r="A11" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="46">
         <v>-0.44040000000000001</v>
       </c>
       <c r="E11" s="6">
@@ -7676,12 +6626,12 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="50">
+      <c r="A12" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="46">
         <v>-0.60709999999999997</v>
       </c>
       <c r="E12" s="6">
@@ -7689,12 +6639,12 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="57" t="s">
-        <v>215</v>
-      </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="50">
+      <c r="A13" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="46">
         <v>-0.71689999999999998</v>
       </c>
       <c r="E13" s="6">
@@ -7702,12 +6652,12 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="57" t="s">
-        <v>217</v>
-      </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="50">
+      <c r="A14" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="46">
         <v>-16.180800000000001</v>
       </c>
       <c r="E14" s="6">
@@ -7715,12 +6665,12 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="57" t="s">
-        <v>218</v>
-      </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="50">
+      <c r="A15" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="46">
         <v>-0.89485999999999999</v>
       </c>
       <c r="E15" s="6">
@@ -7728,12 +6678,12 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="57" t="s">
-        <v>219</v>
-      </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="50">
+      <c r="A16" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="54"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="46">
         <v>0.85899999999999999</v>
       </c>
       <c r="E16" s="6">
@@ -7741,12 +6691,12 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="57" t="s">
-        <v>220</v>
-      </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="50">
+      <c r="A17" s="53" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="46">
         <v>0.47910000000000003</v>
       </c>
       <c r="E17" s="6">
@@ -7754,12 +6704,12 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="57" t="s">
-        <v>221</v>
-      </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="50">
+      <c r="A18" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="46">
         <v>14.4727</v>
       </c>
       <c r="E18" s="6">
@@ -7767,12 +6717,12 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="57" t="s">
-        <v>222</v>
-      </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="50">
+      <c r="A19" s="53" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="46">
         <v>-16.2044</v>
       </c>
       <c r="E19" s="6">
@@ -7780,12 +6730,12 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="57" t="s">
-        <v>223</v>
-      </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="50">
+      <c r="A20" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="46">
         <v>11.651999999999999</v>
       </c>
       <c r="E20" s="6">
@@ -7793,12 +6743,12 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="57" t="s">
-        <v>224</v>
-      </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="50">
+      <c r="A21" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="46">
         <v>2.673E-2</v>
       </c>
       <c r="E21" s="6">
@@ -7806,12 +6756,12 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="57" t="s">
-        <v>225</v>
-      </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="50">
+      <c r="A22" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="46">
         <v>0.1087</v>
       </c>
       <c r="E22" s="6">
@@ -7819,43 +6769,43 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="60" t="s">
-        <v>256</v>
+      <c r="A25" s="56" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multivariate Analysis with both Race & Body Type Collapsed
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F60532-219E-1949-85CD-A23551E9C040}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DD4BBE-77F5-D244-AF8A-F857E1C803CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="500" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="RPDR Effect Estimates" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="251">
   <si>
     <t>Age</t>
   </si>
@@ -779,6 +779,9 @@
   </si>
   <si>
     <t>B Estimate Comparisons for Bottom Two 2 (Body Type Collapsed)</t>
+  </si>
+  <si>
+    <t>B Estimate Comparisons for Bottom Two 2 (Body Type &amp; Race Collapsed)</t>
   </si>
 </sst>
 </file>
@@ -974,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1111,6 +1114,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4059,7 +4063,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4970,7 +4974,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5468,13 +5472,13 @@
         <v>3</v>
       </c>
       <c r="I17" s="33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J17" s="40">
-        <v>6.6665000000000001</v>
+        <v>0.22719</v>
       </c>
       <c r="K17" s="38">
-        <v>0.15459999999999999</v>
+        <v>0.63360000000000005</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -5860,10 +5864,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B9891-AE0A-EC49-A442-8B89DE5C2A2B}">
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="K9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5877,9 +5881,10 @@
     <col min="12" max="12" width="10.33203125" customWidth="1"/>
     <col min="13" max="13" width="20.1640625" customWidth="1"/>
     <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:22">
       <c r="A1" s="50" t="s">
         <v>242</v>
       </c>
@@ -5895,8 +5900,11 @@
       <c r="M1" s="37" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="S1" s="37" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="23" t="s">
         <v>199</v>
       </c>
@@ -5933,8 +5941,20 @@
       <c r="P2" s="24" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="S2" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="V2" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -5974,8 +5994,21 @@
         <f>ABS((N3-O3)/O3)</f>
         <v>0.1516623824185758</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="S3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="6">
+        <v>-0.40770000000000001</v>
+      </c>
+      <c r="U3" s="6">
+        <v>-0.37140000000000001</v>
+      </c>
+      <c r="V3" s="6">
+        <f>ABS((T3-U3)/U3)</f>
+        <v>9.7738287560581574E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="6" t="s">
         <v>131</v>
       </c>
@@ -6015,8 +6048,21 @@
         <f t="shared" ref="P4:P5" si="2">ABS((N4-O4)/O4)</f>
         <v>5.4996162008398387E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="S4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="6">
+        <v>-2.3365</v>
+      </c>
+      <c r="U4" s="6">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V4" s="6">
+        <f t="shared" ref="V4:V5" si="3">ABS((T4-U4)/U4)</f>
+        <v>4.719433488705637E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -6056,8 +6102,21 @@
         <f t="shared" si="2"/>
         <v>3.6966952760694713E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="S5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="6">
+        <v>-0.71250000000000002</v>
+      </c>
+      <c r="U5" s="6">
+        <v>-0.72</v>
+      </c>
+      <c r="V5" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0416666666666598E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="6" t="s">
         <v>134</v>
       </c>
@@ -6097,8 +6156,21 @@
         <f>ABS((N6-O6)/O6)</f>
         <v>0.57537547184965065</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="S6" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="26">
+        <v>-0.39229999999999998</v>
+      </c>
+      <c r="U6" s="26">
+        <v>-0.3009</v>
+      </c>
+      <c r="V6" s="29">
+        <f>ABS((T6-U6)/U6)</f>
+        <v>0.30375540046527078</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -6122,7 +6194,7 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" ref="J7:J8" si="3">ABS((H7-I7)/I7)</f>
+        <f t="shared" ref="J7:J8" si="4">ABS((H7-I7)/I7)</f>
         <v>6.3018196442245711E-2</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -6135,11 +6207,24 @@
         <v>-1.8254300000000001</v>
       </c>
       <c r="P7" s="6">
-        <f t="shared" ref="P7:P8" si="4">ABS((N7-O7)/O7)</f>
+        <f t="shared" ref="P7:P8" si="5">ABS((N7-O7)/O7)</f>
         <v>6.8274324405756454E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="S7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="6">
+        <v>-1.7008000000000001</v>
+      </c>
+      <c r="U7" s="6">
+        <v>-1.8142</v>
+      </c>
+      <c r="V7" s="6">
+        <f t="shared" ref="V7:V8" si="6">ABS((T7-U7)/U7)</f>
+        <v>6.2506890089295525E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -6163,7 +6248,7 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2997097242380357E-2</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -6176,11 +6261,24 @@
         <v>-0.55310000000000004</v>
       </c>
       <c r="P8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6284577834026515E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="S8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T8" s="6">
+        <v>-0.52749999999999997</v>
+      </c>
+      <c r="U8" s="6">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V8" s="6">
+        <f t="shared" si="6"/>
+        <v>5.7362401715511109E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
@@ -6194,12 +6292,46 @@
         <f t="shared" si="0"/>
         <v>8.3701015018800645E-2</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-    </row>
-    <row r="12" spans="1:16">
+    </row>
+    <row r="11" spans="1:22">
+      <c r="G11" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="P11" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="S11" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="U11" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="V11" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="23" t="s">
         <v>199</v>
       </c>
@@ -6212,20 +6344,47 @@
       <c r="D12" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="G12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="13">
+        <v>-0.70240000000000002</v>
+      </c>
+      <c r="I12" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J12" s="6">
+        <f>ABS((H12-I12)/I12)</f>
+        <v>0.12214265181907938</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="13">
+        <v>-0.70240000000000002</v>
+      </c>
+      <c r="O12" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="P12" s="6">
+        <f>ABS((N12-O12)/O12)</f>
+        <v>0.12214265181907938</v>
+      </c>
+      <c r="S12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="T12" s="13">
+        <v>-0.70240000000000002</v>
+      </c>
+      <c r="U12" s="13">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V12" s="6">
+        <f>ABS((T12-U12)/U12)</f>
+        <v>8.873897249610796E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -6239,21 +6398,47 @@
         <f>ABS((B13-C13)/C13)</f>
         <v>3.70774153821306E-2</v>
       </c>
-      <c r="G13" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="13">
-        <v>-0.70240000000000002</v>
-      </c>
-      <c r="I13" s="13">
-        <v>-0.80013000000000001</v>
+      <c r="G13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6">
+        <v>-0.41199999999999998</v>
+      </c>
+      <c r="I13" s="6">
+        <v>-0.35829</v>
       </c>
       <c r="J13" s="6">
         <f>ABS((H13-I13)/I13)</f>
-        <v>0.12214265181907938</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>0.149906500320969</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="6">
+        <v>-0.41199999999999998</v>
+      </c>
+      <c r="O13" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="P13" s="6">
+        <f>ABS((N13-O13)/O13)</f>
+        <v>0.149906500320969</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="6">
+        <v>-0.41199999999999998</v>
+      </c>
+      <c r="U13" s="6">
+        <v>-0.37140000000000001</v>
+      </c>
+      <c r="V13" s="6">
+        <f>ABS((T13-U13)/U13)</f>
+        <v>0.10931610123855673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="6" t="s">
         <v>131</v>
       </c>
@@ -6264,24 +6449,50 @@
         <v>-1.2237</v>
       </c>
       <c r="D14" s="6">
-        <f t="shared" ref="D14:D20" si="5">ABS((B14-C14)/C14)</f>
+        <f t="shared" ref="D14:D20" si="7">ABS((B14-C14)/C14)</f>
         <v>1.0296641333660166E-2</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="6">
-        <v>-0.41199999999999998</v>
+        <v>-2.2928000000000002</v>
       </c>
       <c r="I14" s="6">
-        <v>-0.35829</v>
+        <v>-2.2200099999999998</v>
       </c>
       <c r="J14" s="6">
-        <f>ABS((H14-I14)/I14)</f>
-        <v>0.149906500320969</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <f t="shared" ref="J14:J15" si="8">ABS((H14-I14)/I14)</f>
+        <v>3.278814059396145E-2</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="6">
+        <v>-2.2928000000000002</v>
+      </c>
+      <c r="O14" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" ref="P14:P15" si="9">ABS((N14-O14)/O14)</f>
+        <v>3.278814059396145E-2</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T14" s="6">
+        <v>-2.2928000000000002</v>
+      </c>
+      <c r="U14" s="6">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V14" s="6">
+        <f t="shared" ref="V14:V15" si="10">ABS((T14-U14)/U14)</f>
+        <v>2.7608461814270492E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -6292,24 +6503,50 @@
         <v>-2.4157999999999999</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.7668681182217154E-2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H15" s="6">
-        <v>-2.2928000000000002</v>
+        <v>-0.70389999999999997</v>
       </c>
       <c r="I15" s="6">
-        <v>-2.2200099999999998</v>
+        <v>-0.73923000000000005</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" ref="J15:J16" si="6">ABS((H15-I15)/I15)</f>
-        <v>3.278814059396145E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <f t="shared" si="8"/>
+        <v>4.7792973770004035E-2</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="6">
+        <v>-0.70389999999999997</v>
+      </c>
+      <c r="O15" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="P15" s="6">
+        <f t="shared" si="9"/>
+        <v>4.7792973770004035E-2</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="T15" s="6">
+        <v>-0.70389999999999997</v>
+      </c>
+      <c r="U15" s="6">
+        <v>-0.72</v>
+      </c>
+      <c r="V15" s="6">
+        <f t="shared" si="10"/>
+        <v>2.2361111111111116E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="6" t="s">
         <v>134</v>
       </c>
@@ -6320,24 +6557,50 @@
         <v>0.63932999999999995</v>
       </c>
       <c r="D16" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.1298703330048706E-2</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="6">
-        <v>-0.70389999999999997</v>
-      </c>
-      <c r="I16" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="J16" s="6">
-        <f t="shared" si="6"/>
-        <v>4.7792973770004035E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="G16" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="28">
+        <v>-0.39290000000000003</v>
+      </c>
+      <c r="I16" s="26">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J16" s="29">
+        <f>ABS((H16-I16)/I16)</f>
+        <v>0.55186033651947231</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="28">
+        <v>-0.39290000000000003</v>
+      </c>
+      <c r="O16" s="26">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="P16" s="29">
+        <f>ABS((N16-O16)/O16)</f>
+        <v>0.55186033651947231</v>
+      </c>
+      <c r="S16" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" s="28">
+        <v>-0.39290000000000003</v>
+      </c>
+      <c r="U16" s="26">
+        <v>-0.3009</v>
+      </c>
+      <c r="V16" s="29">
+        <f>ABS((T16-U16)/U16)</f>
+        <v>0.30574941841143244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
@@ -6348,24 +6611,50 @@
         <v>-0.40884999999999999</v>
       </c>
       <c r="D17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.338632750397455E-2</v>
       </c>
-      <c r="G17" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="28">
-        <v>-0.39290000000000003</v>
-      </c>
-      <c r="I17" s="26">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="J17" s="29">
-        <f>ABS((H17-I17)/I17)</f>
-        <v>0.55186033651947231</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="G17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="6">
+        <v>-1.7048000000000001</v>
+      </c>
+      <c r="I17" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" ref="J17:J18" si="11">ABS((H17-I17)/I17)</f>
+        <v>6.0814570375552962E-2</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="6">
+        <v>-1.7048000000000001</v>
+      </c>
+      <c r="O17" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="P17" s="6">
+        <f t="shared" ref="P17:P18" si="12">ABS((N17-O17)/O17)</f>
+        <v>6.0814570375552962E-2</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T17" s="6">
+        <v>-1.7048000000000001</v>
+      </c>
+      <c r="U17" s="6">
+        <v>-1.8142</v>
+      </c>
+      <c r="V17" s="6">
+        <f t="shared" ref="V17:V18" si="13">ABS((T17-U17)/U17)</f>
+        <v>6.0302061514717196E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -6376,24 +6665,50 @@
         <v>-1.88056</v>
       </c>
       <c r="D18" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.4167694729229545E-2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H18" s="6">
-        <v>-1.7048000000000001</v>
+        <v>-0.50390000000000001</v>
       </c>
       <c r="I18" s="6">
-        <v>-1.8151900000000001</v>
+        <v>-0.55120000000000002</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" ref="J18:J19" si="7">ABS((H18-I18)/I18)</f>
-        <v>6.0814570375552962E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <f t="shared" si="11"/>
+        <v>8.5812772133526866E-2</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" s="6">
+        <v>-0.50390000000000001</v>
+      </c>
+      <c r="O18" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" si="12"/>
+        <v>8.5812772133526866E-2</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T18" s="6">
+        <v>-0.50390000000000001</v>
+      </c>
+      <c r="U18" s="6">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="13"/>
+        <v>9.9535382416011384E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -6404,24 +6719,11 @@
         <v>-0.46009</v>
       </c>
       <c r="D19" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.4366754330674443E-2</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="6">
-        <v>-0.50390000000000001</v>
-      </c>
-      <c r="I19" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="J19" s="6">
-        <f t="shared" si="7"/>
-        <v>8.5812772133526866E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="25" t="s">
         <v>22</v>
       </c>
@@ -6432,17 +6734,57 @@
         <v>-0.24127999999999999</v>
       </c>
       <c r="D20" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.30719496021220166</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:23">
       <c r="A21" s="31"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="S21" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="T21" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="U21" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="V21" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="G22" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="S22" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="T22" s="13">
+        <v>0.2019</v>
+      </c>
+      <c r="U22" s="13">
+        <v>0.25609999999999999</v>
+      </c>
+      <c r="V22" s="34">
+        <f>ABS((T22-U22)/U22)</f>
+        <v>0.21163607965638423</v>
+      </c>
+      <c r="W22" s="64"/>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="23" t="s">
         <v>199</v>
       </c>
@@ -6455,20 +6797,34 @@
       <c r="D23" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="G23" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="G23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="13">
+        <v>-0.70889999999999997</v>
+      </c>
+      <c r="I23" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J23" s="6">
+        <f>ABS((H23-I23)/I23)</f>
+        <v>0.11401897191706352</v>
+      </c>
+      <c r="S23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="T23" s="13">
+        <v>-0.70889999999999997</v>
+      </c>
+      <c r="U23" s="13">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V23" s="6">
+        <f>ABS((T23-U23)/U23)</f>
+        <v>8.030617540217963E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -6483,20 +6839,33 @@
         <v>3.6269848480260054E-2</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H24" s="13">
-        <v>-0.70889999999999997</v>
+        <v>0.2019</v>
       </c>
       <c r="I24" s="13">
-        <v>-0.80013000000000001</v>
+        <v>0.24659</v>
       </c>
       <c r="J24" s="6">
         <f>ABS((H24-I24)/I24)</f>
-        <v>0.11401897191706352</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>0.18123200454195226</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T24" s="6">
+        <v>-0.43569999999999998</v>
+      </c>
+      <c r="U24" s="6">
+        <v>-0.37140000000000001</v>
+      </c>
+      <c r="V24" s="6">
+        <f>ABS((T24-U24)/U24)</f>
+        <v>0.17312870220786206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="6" t="s">
         <v>131</v>
       </c>
@@ -6507,24 +6876,37 @@
         <v>-1.2237</v>
       </c>
       <c r="D25" s="6">
-        <f t="shared" ref="D25:D32" si="8">ABS((B25-C25)/C25)</f>
+        <f t="shared" ref="D25:D32" si="14">ABS((B25-C25)/C25)</f>
         <v>2.1001879545640319E-2</v>
       </c>
-      <c r="G25" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="13">
-        <v>0.2019</v>
-      </c>
-      <c r="I25" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="J25" s="6">
+      <c r="G25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="6">
+        <v>-0.43569999999999998</v>
+      </c>
+      <c r="I25" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J25" s="34">
         <f>ABS((H25-I25)/I25)</f>
-        <v>0.18123200454195226</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>0.21605403444137425</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T25" s="6">
+        <v>-2.3079000000000001</v>
+      </c>
+      <c r="U25" s="6">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V25" s="6">
+        <f t="shared" ref="V25:V26" si="15">ABS((T25-U25)/U25)</f>
+        <v>3.4376120473288016E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="6" t="s">
         <v>11</v>
       </c>
@@ -6535,24 +6917,37 @@
         <v>-2.4157999999999999</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>4.4871264177498163E-2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H26" s="6">
-        <v>-0.43569999999999998</v>
+        <v>-2.3079000000000001</v>
       </c>
       <c r="I26" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="J26" s="34">
-        <f>ABS((H26-I26)/I26)</f>
-        <v>0.21605403444137425</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" ref="J26:J27" si="16">ABS((H26-I26)/I26)</f>
+        <v>3.9589911757154359E-2</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="T26" s="6">
+        <v>-0.70899999999999996</v>
+      </c>
+      <c r="U26" s="6">
+        <v>-0.72</v>
+      </c>
+      <c r="V26" s="6">
+        <f t="shared" si="15"/>
+        <v>1.5277777777777791E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="6" t="s">
         <v>134</v>
       </c>
@@ -6563,24 +6958,37 @@
         <v>0.63932999999999995</v>
       </c>
       <c r="D27" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>9.5052633225407843E-2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H27" s="6">
-        <v>-2.3079000000000001</v>
+        <v>-0.70899999999999996</v>
       </c>
       <c r="I27" s="6">
-        <v>-2.2200099999999998</v>
+        <v>-0.73923000000000005</v>
       </c>
       <c r="J27" s="6">
-        <f t="shared" ref="J27:J28" si="9">ABS((H27-I27)/I27)</f>
-        <v>3.9589911757154359E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <f t="shared" si="16"/>
+        <v>4.0893903115403987E-2</v>
+      </c>
+      <c r="S27" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="T27" s="28">
+        <v>-0.36720000000000003</v>
+      </c>
+      <c r="U27" s="26">
+        <v>-0.3009</v>
+      </c>
+      <c r="V27" s="29">
+        <f>ABS((T27-U27)/U27)</f>
+        <v>0.22033898305084754</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -6591,24 +6999,37 @@
         <v>-0.40884999999999999</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>3.2163385104561563E-2</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="6">
-        <v>-0.70899999999999996</v>
-      </c>
-      <c r="I28" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="J28" s="6">
-        <f t="shared" si="9"/>
-        <v>4.0893903115403987E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="G28" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="28">
+        <v>-0.36720000000000003</v>
+      </c>
+      <c r="I28" s="26">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J28" s="29">
+        <f>ABS((H28-I28)/I28)</f>
+        <v>0.45035152855675803</v>
+      </c>
+      <c r="S28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T28" s="6">
+        <v>-1.7668999999999999</v>
+      </c>
+      <c r="U28" s="6">
+        <v>-1.8142</v>
+      </c>
+      <c r="V28" s="6">
+        <f t="shared" ref="V28:V29" si="17">ABS((T28-U28)/U28)</f>
+        <v>2.6072097894388777E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -6619,24 +7040,37 @@
         <v>-1.88056</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>9.7098736546560298E-3</v>
       </c>
-      <c r="G29" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="28">
-        <v>-0.36720000000000003</v>
-      </c>
-      <c r="I29" s="26">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="J29" s="29">
-        <f>ABS((H29-I29)/I29)</f>
-        <v>0.45035152855675803</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="G29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="6">
+        <v>-1.7668999999999999</v>
+      </c>
+      <c r="I29" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" ref="J29" si="18">ABS((H29-I29)/I29)</f>
+        <v>2.6603275690148229E-2</v>
+      </c>
+      <c r="S29" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T29" s="6">
+        <v>-0.53069999999999995</v>
+      </c>
+      <c r="U29" s="6">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V29" s="6">
+        <f t="shared" si="17"/>
+        <v>5.1644031451036521E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -6647,24 +7081,24 @@
         <v>-0.46009</v>
       </c>
       <c r="D30" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>7.2616227259883925E-2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H30" s="6">
-        <v>-1.7668999999999999</v>
+        <v>-0.53069999999999995</v>
       </c>
       <c r="I30" s="6">
-        <v>-1.8151900000000001</v>
+        <v>-0.55120000000000002</v>
       </c>
       <c r="J30" s="6">
-        <f t="shared" ref="J30" si="10">ABS((H30-I30)/I30)</f>
-        <v>2.6603275690148229E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <f>ABS((H30-I30)/I30)</f>
+        <v>3.7191582002902887E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" s="25" t="s">
         <v>22</v>
       </c>
@@ -6675,24 +7109,11 @@
         <v>-0.24127999999999999</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0.18824602122015921</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H31" s="6">
-        <v>-0.53069999999999995</v>
-      </c>
-      <c r="I31" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="J31" s="6">
-        <f>ABS((H31-I31)/I31)</f>
-        <v>3.7191582002902887E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" s="25" t="s">
         <v>21</v>
       </c>
@@ -6703,768 +7124,897 @@
         <v>0.22370000000000001</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1.4751899865891807E-2</v>
       </c>
-    </row>
-    <row r="34" spans="7:10">
-      <c r="G34" s="23" t="s">
+      <c r="S32" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="H34" s="23" t="s">
+      <c r="T32" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="I34" s="23" t="s">
+      <c r="U32" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="J34" s="24" t="s">
+      <c r="V32" s="24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="7:10">
+    <row r="33" spans="7:22">
+      <c r="G33" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="J33" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="S33" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="T33" s="13">
+        <v>-0.20449999999999999</v>
+      </c>
+      <c r="U33" s="13">
+        <v>-0.2132</v>
+      </c>
+      <c r="V33" s="8">
+        <f>ABS((T33-U33)/U33)</f>
+        <v>4.0806754221388429E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="7:22">
+      <c r="G34" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="13">
+        <v>-0.73839999999999995</v>
+      </c>
+      <c r="I34" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J34" s="6">
+        <f>ABS((H34-I34)/I34)</f>
+        <v>7.7149963130991289E-2</v>
+      </c>
+      <c r="S34" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="T34" s="13">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="U34" s="13">
+        <v>0.25609999999999999</v>
+      </c>
+      <c r="V34" s="34">
+        <f>ABS((T34-U34)/U34)</f>
+        <v>9.8008590394377135E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="7:22">
       <c r="G35" s="30" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H35" s="13">
-        <v>-0.73839999999999995</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="I35" s="13">
-        <v>-0.80013000000000001</v>
+        <v>0.24659</v>
       </c>
       <c r="J35" s="6">
         <f>ABS((H35-I35)/I35)</f>
-        <v>7.7149963130991289E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="7:10">
+        <v>6.3222352893466852E-2</v>
+      </c>
+      <c r="S35" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="T35" s="13">
+        <v>-0.73839999999999995</v>
+      </c>
+      <c r="U35" s="13">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V35" s="6">
+        <f>ABS((T35-U35)/U35)</f>
+        <v>4.2034250129735461E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="7:22">
       <c r="G36" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="13">
+        <v>-0.20449999999999999</v>
+      </c>
+      <c r="I36" s="13">
+        <v>-0.25905</v>
+      </c>
+      <c r="J36" s="34">
+        <f>ABS((H36-I36)/I36)</f>
+        <v>0.21057710866628071</v>
+      </c>
+      <c r="S36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T36" s="6">
+        <v>-0.38669999999999999</v>
+      </c>
+      <c r="U36" s="6">
+        <v>-0.37140000000000001</v>
+      </c>
+      <c r="V36" s="6">
+        <f>ABS((T36-U36)/U36)</f>
+        <v>4.1195476575121112E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="7:22">
+      <c r="G37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="6">
+        <v>-0.38669999999999999</v>
+      </c>
+      <c r="I37" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J37" s="8">
+        <f>ABS((H37-I37)/I37)</f>
+        <v>7.929330988863767E-2</v>
+      </c>
+      <c r="S37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T37" s="6">
+        <v>-2.2353000000000001</v>
+      </c>
+      <c r="U37" s="6">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V37" s="6">
+        <f t="shared" ref="V37:V38" si="19">ABS((T37-U37)/U37)</f>
+        <v>1.8375761921836746E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="7:22">
+      <c r="G38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="6">
+        <v>-2.2353000000000001</v>
+      </c>
+      <c r="I38" s="6">
+        <v>-2.2200099999999998</v>
+      </c>
+      <c r="J38" s="6">
+        <f t="shared" ref="J38:J39" si="20">ABS((H38-I38)/I38)</f>
+        <v>6.8873563632597373E-3</v>
+      </c>
+      <c r="S38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="T38" s="6">
+        <v>-0.73209999999999997</v>
+      </c>
+      <c r="U38" s="6">
+        <v>-0.72</v>
+      </c>
+      <c r="V38" s="6">
+        <f t="shared" si="19"/>
+        <v>1.6805555555555556E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="7:22">
+      <c r="G39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="6">
+        <v>-0.73209999999999997</v>
+      </c>
+      <c r="I39" s="6">
+        <v>-0.73923000000000005</v>
+      </c>
+      <c r="J39" s="6">
+        <f t="shared" si="20"/>
+        <v>9.6451713269213642E-3</v>
+      </c>
+      <c r="S39" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="T39" s="28">
+        <v>-0.34029999999999999</v>
+      </c>
+      <c r="U39" s="26">
+        <v>-0.3009</v>
+      </c>
+      <c r="V39" s="29">
+        <f>ABS((T39-U39)/U39)</f>
+        <v>0.13094051179793947</v>
+      </c>
+    </row>
+    <row r="40" spans="7:22">
+      <c r="G40" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="28">
+        <v>-0.34029999999999999</v>
+      </c>
+      <c r="I40" s="26">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J40" s="29">
+        <f>ABS((H40-I40)/I40)</f>
+        <v>0.34410300971640717</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T40" s="6">
+        <v>-1.7627999999999999</v>
+      </c>
+      <c r="U40" s="6">
+        <v>-1.8142</v>
+      </c>
+      <c r="V40" s="6">
+        <f t="shared" ref="V40:V41" si="21">ABS((T40-U40)/U40)</f>
+        <v>2.8332047183331557E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="7:22">
+      <c r="G41" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="6">
+        <v>-1.7627999999999999</v>
+      </c>
+      <c r="I41" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J41" s="6">
+        <f t="shared" ref="J41:J42" si="22">ABS((H41-I41)/I41)</f>
+        <v>2.8861992408508286E-2</v>
+      </c>
+      <c r="S41" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T41" s="6">
+        <v>-0.52829999999999999</v>
+      </c>
+      <c r="U41" s="6">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V41" s="6">
+        <f t="shared" si="21"/>
+        <v>5.5932809149392415E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="7:22">
+      <c r="G42" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="6">
+        <v>-0.52829999999999999</v>
+      </c>
+      <c r="I42" s="6">
+        <v>-0.55120000000000002</v>
+      </c>
+      <c r="J42" s="6">
+        <f t="shared" si="22"/>
+        <v>4.1545718432510939E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="7:22">
+      <c r="G45" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="7:22">
+      <c r="G46" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="13">
+        <v>-0.79220000000000002</v>
+      </c>
+      <c r="I46" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J46" s="6">
+        <f>ABS((H46-I46)/I46)</f>
+        <v>9.9108894804594162E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="7:22">
+      <c r="G47" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="13">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I36" s="13">
+      <c r="H47" s="13">
+        <v>0.22750000000000001</v>
+      </c>
+      <c r="I47" s="13">
         <v>0.24659</v>
-      </c>
-      <c r="J36" s="6">
-        <f>ABS((H36-I36)/I36)</f>
-        <v>6.3222352893466852E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="7:10">
-      <c r="G37" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="H37" s="13">
-        <v>-0.20449999999999999</v>
-      </c>
-      <c r="I37" s="13">
-        <v>-0.25905</v>
-      </c>
-      <c r="J37" s="34">
-        <f>ABS((H37-I37)/I37)</f>
-        <v>0.21057710866628071</v>
-      </c>
-    </row>
-    <row r="38" spans="7:10">
-      <c r="G38" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="6">
-        <v>-0.38669999999999999</v>
-      </c>
-      <c r="I38" s="6">
-        <v>-0.35829</v>
-      </c>
-      <c r="J38" s="8">
-        <f>ABS((H38-I38)/I38)</f>
-        <v>7.929330988863767E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="7:10">
-      <c r="G39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="6">
-        <v>-2.2353000000000001</v>
-      </c>
-      <c r="I39" s="6">
-        <v>-2.2200099999999998</v>
-      </c>
-      <c r="J39" s="6">
-        <f t="shared" ref="J39:J40" si="11">ABS((H39-I39)/I39)</f>
-        <v>6.8873563632597373E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="7:10">
-      <c r="G40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="6">
-        <v>-0.73209999999999997</v>
-      </c>
-      <c r="I40" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="J40" s="6">
-        <f t="shared" si="11"/>
-        <v>9.6451713269213642E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="7:10">
-      <c r="G41" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H41" s="28">
-        <v>-0.34029999999999999</v>
-      </c>
-      <c r="I41" s="26">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="J41" s="29">
-        <f>ABS((H41-I41)/I41)</f>
-        <v>0.34410300971640717</v>
-      </c>
-    </row>
-    <row r="42" spans="7:10">
-      <c r="G42" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="6">
-        <v>-1.7627999999999999</v>
-      </c>
-      <c r="I42" s="6">
-        <v>-1.8151900000000001</v>
-      </c>
-      <c r="J42" s="6">
-        <f t="shared" ref="J42:J43" si="12">ABS((H42-I42)/I42)</f>
-        <v>2.8861992408508286E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="7:10">
-      <c r="G43" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H43" s="6">
-        <v>-0.52829999999999999</v>
-      </c>
-      <c r="I43" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="J43" s="6">
-        <f t="shared" si="12"/>
-        <v>4.1545718432510939E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="7:10">
-      <c r="G46" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="H46" s="23" t="s">
-        <v>226</v>
-      </c>
-      <c r="I46" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="J46" s="24" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="7:10">
-      <c r="G47" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="13">
-        <v>-0.79220000000000002</v>
-      </c>
-      <c r="I47" s="13">
-        <v>-0.80013000000000001</v>
       </c>
       <c r="J47" s="6">
         <f>ABS((H47-I47)/I47)</f>
-        <v>9.9108894804594162E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="7:10">
+        <v>7.7415953607202215E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="7:22">
       <c r="G48" s="30" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="H48" s="13">
-        <v>0.22750000000000001</v>
+        <v>-0.19139999999999999</v>
       </c>
       <c r="I48" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="J48" s="6">
+        <v>-0.25905</v>
+      </c>
+      <c r="J48" s="8">
         <f>ABS((H48-I48)/I48)</f>
-        <v>7.7415953607202215E-2</v>
+        <v>0.26114649681528668</v>
       </c>
     </row>
     <row r="49" spans="7:10">
       <c r="G49" s="30" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
       <c r="H49" s="13">
-        <v>-0.19139999999999999</v>
+        <v>0.2757</v>
       </c>
       <c r="I49" s="13">
-        <v>-0.25905</v>
+        <v>0.23050000000000001</v>
       </c>
       <c r="J49" s="8">
         <f>ABS((H49-I49)/I49)</f>
-        <v>0.26114649681528668</v>
+        <v>0.19609544468546633</v>
       </c>
     </row>
     <row r="50" spans="7:10">
-      <c r="G50" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="H50" s="13">
-        <v>0.2757</v>
-      </c>
-      <c r="I50" s="13">
-        <v>0.23050000000000001</v>
+      <c r="G50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="6">
+        <v>-0.37459999999999999</v>
+      </c>
+      <c r="I50" s="6">
+        <v>-0.35829</v>
       </c>
       <c r="J50" s="8">
         <f>ABS((H50-I50)/I50)</f>
-        <v>0.19609544468546633</v>
+        <v>4.5521784029696588E-2</v>
       </c>
     </row>
     <row r="51" spans="7:10">
       <c r="G51" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H51" s="6">
-        <v>-0.37459999999999999</v>
+        <v>-2.2584</v>
       </c>
       <c r="I51" s="6">
-        <v>-0.35829</v>
+        <v>-2.2200099999999998</v>
       </c>
       <c r="J51" s="8">
-        <f>ABS((H51-I51)/I51)</f>
-        <v>4.5521784029696588E-2</v>
+        <f t="shared" ref="J51:J52" si="23">ABS((H51-I51)/I51)</f>
+        <v>1.7292714897680708E-2</v>
       </c>
     </row>
     <row r="52" spans="7:10">
       <c r="G52" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H52" s="6">
-        <v>-2.2584</v>
+        <v>-0.71319999999999995</v>
       </c>
       <c r="I52" s="6">
-        <v>-2.2200099999999998</v>
+        <v>-0.73923000000000005</v>
       </c>
       <c r="J52" s="8">
-        <f t="shared" ref="J52:J53" si="13">ABS((H52-I52)/I52)</f>
-        <v>1.7292714897680708E-2</v>
+        <f t="shared" si="23"/>
+        <v>3.521231551749808E-2</v>
       </c>
     </row>
     <row r="53" spans="7:10">
-      <c r="G53" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" s="6">
-        <v>-0.71319999999999995</v>
-      </c>
-      <c r="I53" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="J53" s="8">
-        <f t="shared" si="13"/>
-        <v>3.521231551749808E-2</v>
+      <c r="G53" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="28">
+        <v>-0.32250000000000001</v>
+      </c>
+      <c r="I53" s="26">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J53" s="29">
+        <f>ABS((H53-I53)/I53)</f>
+        <v>0.27379729836479971</v>
       </c>
     </row>
     <row r="54" spans="7:10">
-      <c r="G54" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="28">
-        <v>-0.32250000000000001</v>
-      </c>
-      <c r="I54" s="26">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="J54" s="29">
-        <f>ABS((H54-I54)/I54)</f>
-        <v>0.27379729836479971</v>
+      <c r="G54" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="6">
+        <v>-1.7566999999999999</v>
+      </c>
+      <c r="I54" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J54" s="6">
+        <f t="shared" ref="J54:J55" si="24">ABS((H54-I54)/I54)</f>
+        <v>3.2222522160214713E-2</v>
       </c>
     </row>
     <row r="55" spans="7:10">
       <c r="G55" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H55" s="6">
-        <v>-1.7566999999999999</v>
+        <v>-0.53120000000000001</v>
       </c>
       <c r="I55" s="6">
-        <v>-1.8151900000000001</v>
+        <v>-0.55120000000000002</v>
       </c>
       <c r="J55" s="6">
-        <f t="shared" ref="J55:J56" si="14">ABS((H55-I55)/I55)</f>
-        <v>3.2222522160214713E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="7:10">
-      <c r="G56" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H56" s="6">
-        <v>-0.53120000000000001</v>
-      </c>
-      <c r="I56" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="J56" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="24"/>
         <v>3.6284470246734431E-2</v>
       </c>
     </row>
+    <row r="58" spans="7:10">
+      <c r="G58" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="I58" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="J58" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
     <row r="59" spans="7:10">
-      <c r="G59" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="H59" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="I59" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="J59" s="24" t="s">
-        <v>200</v>
+      <c r="G59" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="13">
+        <v>-0.80789999999999995</v>
+      </c>
+      <c r="I59" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J59" s="6">
+        <f>ABS((H59-I59)/I59)</f>
+        <v>9.7109219751789627E-3</v>
       </c>
     </row>
     <row r="60" spans="7:10">
       <c r="G60" s="30" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H60" s="13">
-        <v>-0.80789999999999995</v>
+        <v>0.26939999999999997</v>
       </c>
       <c r="I60" s="13">
-        <v>-0.80013000000000001</v>
+        <v>0.24659</v>
       </c>
       <c r="J60" s="6">
         <f>ABS((H60-I60)/I60)</f>
-        <v>9.7109219751789627E-3</v>
+        <v>9.2501723508657971E-2</v>
       </c>
     </row>
     <row r="61" spans="7:10">
       <c r="G61" s="30" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="H61" s="13">
-        <v>0.26939999999999997</v>
+        <v>-0.21590000000000001</v>
       </c>
       <c r="I61" s="13">
-        <v>0.24659</v>
-      </c>
-      <c r="J61" s="6">
+        <v>-0.25905</v>
+      </c>
+      <c r="J61" s="8">
         <f>ABS((H61-I61)/I61)</f>
-        <v>9.2501723508657971E-2</v>
+        <v>0.16657016020073342</v>
       </c>
     </row>
     <row r="62" spans="7:10">
       <c r="G62" s="30" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
       <c r="H62" s="13">
-        <v>-0.21590000000000001</v>
+        <v>0.26889999999999997</v>
       </c>
       <c r="I62" s="13">
-        <v>-0.25905</v>
+        <v>0.23050000000000001</v>
       </c>
       <c r="J62" s="8">
         <f>ABS((H62-I62)/I62)</f>
-        <v>0.16657016020073342</v>
+        <v>0.16659436008676773</v>
       </c>
     </row>
     <row r="63" spans="7:10">
       <c r="G63" s="30" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="H63" s="13">
-        <v>0.26889999999999997</v>
+        <v>0.28620000000000001</v>
       </c>
       <c r="I63" s="13">
-        <v>0.23050000000000001</v>
+        <v>0.30564000000000002</v>
       </c>
       <c r="J63" s="8">
-        <f>ABS((H63-I63)/I63)</f>
-        <v>0.16659436008676773</v>
+        <f t="shared" ref="J63:J64" si="25">ABS((H63-I63)/I63)</f>
+        <v>6.3604240282685548E-2</v>
       </c>
     </row>
     <row r="64" spans="7:10">
       <c r="G64" s="30" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H64" s="13">
-        <v>0.28620000000000001</v>
+        <v>0.1125</v>
       </c>
       <c r="I64" s="13">
-        <v>0.30564000000000002</v>
-      </c>
-      <c r="J64" s="8">
-        <f t="shared" ref="J64:J65" si="15">ABS((H64-I64)/I64)</f>
-        <v>6.3604240282685548E-2</v>
+        <v>0.15532000000000001</v>
+      </c>
+      <c r="J64" s="34">
+        <f t="shared" si="25"/>
+        <v>0.27568890033479271</v>
       </c>
     </row>
     <row r="65" spans="7:10">
-      <c r="G65" s="30" t="s">
-        <v>244</v>
-      </c>
-      <c r="H65" s="13">
-        <v>0.1125</v>
-      </c>
-      <c r="I65" s="13">
-        <v>0.15532000000000001</v>
-      </c>
-      <c r="J65" s="34">
-        <f t="shared" si="15"/>
-        <v>0.27568890033479271</v>
+      <c r="G65" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" s="6">
+        <v>-0.37290000000000001</v>
+      </c>
+      <c r="I65" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="J65" s="8">
+        <f>ABS((H65-I65)/I65)</f>
+        <v>4.0777024198275176E-2</v>
       </c>
     </row>
     <row r="66" spans="7:10">
       <c r="G66" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H66" s="6">
-        <v>-0.37290000000000001</v>
+        <v>-2.2570000000000001</v>
       </c>
       <c r="I66" s="6">
-        <v>-0.35829</v>
+        <v>-2.2200099999999998</v>
       </c>
       <c r="J66" s="8">
-        <f>ABS((H66-I66)/I66)</f>
-        <v>4.0777024198275176E-2</v>
+        <f t="shared" ref="J66:J67" si="26">ABS((H66-I66)/I66)</f>
+        <v>1.6662087107715867E-2</v>
       </c>
     </row>
     <row r="67" spans="7:10">
       <c r="G67" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H67" s="6">
-        <v>-2.2570000000000001</v>
+        <v>-0.71109999999999995</v>
       </c>
       <c r="I67" s="6">
-        <v>-2.2200099999999998</v>
+        <v>-0.73923000000000005</v>
       </c>
       <c r="J67" s="8">
-        <f t="shared" ref="J67:J68" si="16">ABS((H67-I67)/I67)</f>
-        <v>1.6662087107715867E-2</v>
+        <f t="shared" si="26"/>
+        <v>3.8053109316451034E-2</v>
       </c>
     </row>
     <row r="68" spans="7:10">
-      <c r="G68" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H68" s="6">
-        <v>-0.71109999999999995</v>
-      </c>
-      <c r="I68" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="J68" s="8">
-        <f t="shared" si="16"/>
-        <v>3.8053109316451034E-2</v>
+      <c r="G68" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" s="28">
+        <v>-0.30740000000000001</v>
+      </c>
+      <c r="I68" s="26">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="J68" s="29">
+        <f>ABS((H68-I68)/I68)</f>
+        <v>0.21415593648787418</v>
       </c>
     </row>
     <row r="69" spans="7:10">
-      <c r="G69" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H69" s="28">
-        <v>-0.30740000000000001</v>
-      </c>
-      <c r="I69" s="26">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="J69" s="29">
-        <f>ABS((H69-I69)/I69)</f>
-        <v>0.21415593648787418</v>
+      <c r="G69" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" s="6">
+        <v>-1.7656000000000001</v>
+      </c>
+      <c r="I69" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="J69" s="6">
+        <f t="shared" ref="J69:J70" si="27">ABS((H69-I69)/I69)</f>
+        <v>2.7319454161823291E-2</v>
       </c>
     </row>
     <row r="70" spans="7:10">
       <c r="G70" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H70" s="6">
-        <v>-1.7656000000000001</v>
+        <v>-0.55810000000000004</v>
       </c>
       <c r="I70" s="6">
-        <v>-1.8151900000000001</v>
+        <v>-0.55120000000000002</v>
       </c>
       <c r="J70" s="6">
-        <f t="shared" ref="J70:J71" si="17">ABS((H70-I70)/I70)</f>
-        <v>2.7319454161823291E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="7:10">
-      <c r="G71" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H71" s="6">
-        <v>-0.55810000000000004</v>
-      </c>
-      <c r="I71" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="J71" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="27"/>
         <v>1.2518142235123398E-2</v>
       </c>
     </row>
+    <row r="72" spans="7:10">
+      <c r="G72" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="H72" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="I72" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="J72" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
     <row r="73" spans="7:10">
-      <c r="G73" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="H73" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="I73" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="J73" s="24" t="s">
-        <v>200</v>
+      <c r="G73" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="I73" s="13">
+        <v>-0.80013000000000001</v>
+      </c>
+      <c r="J73" s="8">
+        <f t="shared" ref="J73:J88" si="28">ABS((H73-I73)/I73)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="7:10">
       <c r="G74" s="30" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H74" s="13">
-        <v>-0.80013000000000001</v>
+        <v>0.24659</v>
       </c>
       <c r="I74" s="13">
-        <v>-0.80013000000000001</v>
+        <v>0.24659</v>
       </c>
       <c r="J74" s="8">
-        <f t="shared" ref="J74:J89" si="18">ABS((H74-I74)/I74)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="7:10">
       <c r="G75" s="30" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="H75" s="13">
-        <v>0.24659</v>
+        <v>-0.25905</v>
       </c>
       <c r="I75" s="13">
-        <v>0.24659</v>
+        <v>-0.25905</v>
       </c>
       <c r="J75" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="7:10">
       <c r="G76" s="30" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
       <c r="H76" s="13">
-        <v>-0.25905</v>
+        <v>0.23050000000000001</v>
       </c>
       <c r="I76" s="13">
-        <v>-0.25905</v>
+        <v>0.23050000000000001</v>
       </c>
       <c r="J76" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="7:10">
       <c r="G77" s="30" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="H77" s="13">
-        <v>0.23050000000000001</v>
+        <v>0.30564000000000002</v>
       </c>
       <c r="I77" s="13">
-        <v>0.23050000000000001</v>
+        <v>0.30564000000000002</v>
       </c>
       <c r="J77" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="7:10">
       <c r="G78" s="30" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H78" s="13">
-        <v>0.30564000000000002</v>
+        <v>0.15532000000000001</v>
       </c>
       <c r="I78" s="13">
-        <v>0.30564000000000002</v>
+        <v>0.15532000000000001</v>
       </c>
       <c r="J78" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="7:10">
       <c r="G79" s="30" t="s">
-        <v>244</v>
+        <v>137</v>
       </c>
       <c r="H79" s="13">
-        <v>0.15532000000000001</v>
+        <v>0.26494000000000001</v>
       </c>
       <c r="I79" s="13">
-        <v>0.15532000000000001</v>
+        <v>0.26494000000000001</v>
       </c>
       <c r="J79" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="7:10">
       <c r="G80" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H80" s="13">
-        <v>0.26494000000000001</v>
+        <v>0.29258000000000001</v>
       </c>
       <c r="I80" s="13">
-        <v>0.26494000000000001</v>
+        <v>0.29258000000000001</v>
       </c>
       <c r="J80" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="7:10">
       <c r="G81" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H81" s="13">
-        <v>0.29258000000000001</v>
+        <v>-5.5890000000000002E-2</v>
       </c>
       <c r="I81" s="13">
-        <v>0.29258000000000001</v>
+        <v>-5.5890000000000002E-2</v>
       </c>
       <c r="J81" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="7:10">
       <c r="G82" s="30" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H82" s="13">
-        <v>-5.5890000000000002E-2</v>
+        <v>-0.12130000000000001</v>
       </c>
       <c r="I82" s="13">
-        <v>-5.5890000000000002E-2</v>
+        <v>-0.12130000000000001</v>
       </c>
       <c r="J82" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="7:10">
-      <c r="G83" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="H83" s="13">
-        <v>-0.12130000000000001</v>
-      </c>
-      <c r="I83" s="13">
-        <v>-0.12130000000000001</v>
+      <c r="G83" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" s="6">
+        <v>-0.35829</v>
+      </c>
+      <c r="I83" s="6">
+        <v>-0.35829</v>
       </c>
       <c r="J83" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="7:10">
       <c r="G84" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H84" s="6">
-        <v>-0.35829</v>
+        <v>-2.2200099999999998</v>
       </c>
       <c r="I84" s="6">
-        <v>-0.35829</v>
+        <v>-2.2200099999999998</v>
       </c>
       <c r="J84" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="7:10">
       <c r="G85" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H85" s="6">
-        <v>-2.2200099999999998</v>
+        <v>-0.73923000000000005</v>
       </c>
       <c r="I85" s="6">
-        <v>-2.2200099999999998</v>
+        <v>-0.73923000000000005</v>
       </c>
       <c r="J85" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="7:10">
-      <c r="G86" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H86" s="6">
-        <v>-0.73923000000000005</v>
-      </c>
-      <c r="I86" s="6">
-        <v>-0.73923000000000005</v>
+      <c r="G86" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86" s="28">
+        <v>-0.25318000000000002</v>
+      </c>
+      <c r="I86" s="26">
+        <v>-0.25318000000000002</v>
       </c>
       <c r="J86" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="7:10">
-      <c r="G87" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H87" s="28">
-        <v>-0.25318000000000002</v>
-      </c>
-      <c r="I87" s="26">
-        <v>-0.25318000000000002</v>
+      <c r="G87" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H87" s="6">
+        <v>-1.8151900000000001</v>
+      </c>
+      <c r="I87" s="6">
+        <v>-1.8151900000000001</v>
       </c>
       <c r="J87" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="7:10">
       <c r="G88" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H88" s="6">
-        <v>-1.8151900000000001</v>
+        <v>-0.55120000000000002</v>
       </c>
       <c r="I88" s="6">
-        <v>-1.8151900000000001</v>
+        <v>-0.55120000000000002</v>
       </c>
       <c r="J88" s="8">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="7:10">
-      <c r="G89" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H89" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="I89" s="6">
-        <v>-0.55120000000000002</v>
-      </c>
-      <c r="J89" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Preliminary main effects model & re-evaluation of all initial variables completed
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DD4BBE-77F5-D244-AF8A-F857E1C803CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482040B-F148-6F46-9AC7-4A66078C5033}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
+    <workbookView xWindow="2400" yWindow="500" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="RPDR Effect Estimates" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="263">
   <si>
     <t>Age</t>
   </si>
@@ -782,13 +782,49 @@
   </si>
   <si>
     <t>B Estimate Comparisons for Bottom Two 2 (Body Type &amp; Race Collapsed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backward Elimination Round 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Significant test result in LRT comparing Model 11 and 10; Outfit_Reveal retained in the model </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward selection results indicated Ross to be retained in the model </t>
+  </si>
+  <si>
+    <t>Model 13</t>
+  </si>
+  <si>
+    <t>Model 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singing </t>
+  </si>
+  <si>
+    <t>Model 15</t>
+  </si>
+  <si>
+    <t>Model 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dancing retained in model </t>
+  </si>
+  <si>
+    <t>Backward elimination round 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carson </t>
+  </si>
+  <si>
+    <t>Model 19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -831,8 +867,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -899,8 +975,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5B7FF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -973,11 +1055,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1051,6 +1168,24 @@
     <xf numFmtId="11" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1114,7 +1249,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115F1DD9-A0CB-2E42-BC0A-13187B41B5A6}">
   <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1456,19 +1590,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="H1" s="44" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="H1" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="62"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12">
@@ -4063,7 +4197,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4078,19 +4212,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="63" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
-      <c r="H1" s="44" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
+      <c r="H1" s="60" t="s">
         <v>247</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="62"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -4989,19 +5123,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="63" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
-      <c r="H1" s="44" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
+      <c r="H1" s="60" t="s">
         <v>247</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="62"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -5864,10 +5998,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B9891-AE0A-EC49-A442-8B89DE5C2A2B}">
-  <dimension ref="A1:W88"/>
+  <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" topLeftCell="L72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V100" sqref="V100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5885,18 +6019,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="66" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="G1" s="50" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="G1" s="66" t="s">
         <v>246</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
       <c r="M1" s="37" t="s">
         <v>249</v>
       </c>
@@ -5978,7 +6112,7 @@
         <v>-0.35829</v>
       </c>
       <c r="J3" s="6">
-        <f>ABS((H3-I3)/I3)</f>
+        <f t="shared" ref="J3:J8" si="0">ABS((H3-I3)/I3)</f>
         <v>0.1379050489826677</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -5991,7 +6125,7 @@
         <v>-0.35400999999999999</v>
       </c>
       <c r="P3" s="6">
-        <f>ABS((N3-O3)/O3)</f>
+        <f t="shared" ref="P3:P8" si="1">ABS((N3-O3)/O3)</f>
         <v>0.1516623824185758</v>
       </c>
       <c r="S3" s="6" t="s">
@@ -6004,7 +6138,7 @@
         <v>-0.37140000000000001</v>
       </c>
       <c r="V3" s="6">
-        <f>ABS((T3-U3)/U3)</f>
+        <f t="shared" ref="V3:V8" si="2">ABS((T3-U3)/U3)</f>
         <v>9.7738287560581574E-2</v>
       </c>
     </row>
@@ -6019,7 +6153,7 @@
         <v>-1.2237</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" ref="D4:D9" si="0">ABS((B4-C4)/C4)</f>
+        <f t="shared" ref="D4:D9" si="3">ABS((B4-C4)/C4)</f>
         <v>1.1358993217291839E-2</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -6032,7 +6166,7 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" ref="J4:J5" si="1">ABS((H4-I4)/I4)</f>
+        <f t="shared" si="0"/>
         <v>5.2472736609294648E-2</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -6045,7 +6179,7 @@
         <v>-2.2147000000000001</v>
       </c>
       <c r="P4" s="6">
-        <f t="shared" ref="P4:P5" si="2">ABS((N4-O4)/O4)</f>
+        <f t="shared" si="1"/>
         <v>5.4996162008398387E-2</v>
       </c>
       <c r="S4" s="6" t="s">
@@ -6058,7 +6192,7 @@
         <v>-2.2311999999999999</v>
       </c>
       <c r="V4" s="6">
-        <f t="shared" ref="V4:V5" si="3">ABS((T4-U4)/U4)</f>
+        <f t="shared" si="2"/>
         <v>4.719433488705637E-2</v>
       </c>
     </row>
@@ -6073,7 +6207,7 @@
         <v>-2.4157999999999999</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7.2646742279990059E-2</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -6086,7 +6220,7 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.615924678381563E-2</v>
       </c>
       <c r="M5" s="6" t="s">
@@ -6099,7 +6233,7 @@
         <v>-0.73985000000000001</v>
       </c>
       <c r="P5" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.6966952760694713E-2</v>
       </c>
       <c r="S5" s="6" t="s">
@@ -6112,7 +6246,7 @@
         <v>-0.72</v>
       </c>
       <c r="V5" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.0416666666666598E-2</v>
       </c>
     </row>
@@ -6140,7 +6274,7 @@
         <v>-0.25318000000000002</v>
       </c>
       <c r="J6" s="29">
-        <f>ABS((H6-I6)/I6)</f>
+        <f t="shared" si="0"/>
         <v>0.5494904810806539</v>
       </c>
       <c r="M6" s="26" t="s">
@@ -6153,7 +6287,7 @@
         <v>-0.24901999999999999</v>
       </c>
       <c r="P6" s="29">
-        <f>ABS((N6-O6)/O6)</f>
+        <f t="shared" si="1"/>
         <v>0.57537547184965065</v>
       </c>
       <c r="S6" s="26" t="s">
@@ -6166,7 +6300,7 @@
         <v>-0.3009</v>
       </c>
       <c r="V6" s="29">
-        <f>ABS((T6-U6)/U6)</f>
+        <f t="shared" si="2"/>
         <v>0.30375540046527078</v>
       </c>
     </row>
@@ -6181,7 +6315,7 @@
         <v>-0.40884999999999999</v>
       </c>
       <c r="D7" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.1373364314540755E-2</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -6194,7 +6328,7 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" ref="J7:J8" si="4">ABS((H7-I7)/I7)</f>
+        <f t="shared" si="0"/>
         <v>6.3018196442245711E-2</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -6207,7 +6341,7 @@
         <v>-1.8254300000000001</v>
       </c>
       <c r="P7" s="6">
-        <f t="shared" ref="P7:P8" si="5">ABS((N7-O7)/O7)</f>
+        <f t="shared" si="1"/>
         <v>6.8274324405756454E-2</v>
       </c>
       <c r="S7" s="6" t="s">
@@ -6220,7 +6354,7 @@
         <v>-1.8142</v>
       </c>
       <c r="V7" s="6">
-        <f t="shared" ref="V7:V8" si="6">ABS((T7-U7)/U7)</f>
+        <f t="shared" si="2"/>
         <v>6.2506890089295525E-2</v>
       </c>
     </row>
@@ -6235,7 +6369,7 @@
         <v>-1.88056</v>
       </c>
       <c r="D8" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.3904794316586571E-2</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -6248,7 +6382,7 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>4.2997097242380357E-2</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -6261,7 +6395,7 @@
         <v>-0.55310000000000004</v>
       </c>
       <c r="P8" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>4.6284577834026515E-2</v>
       </c>
       <c r="S8" s="6" t="s">
@@ -6274,7 +6408,7 @@
         <v>-0.55959999999999999</v>
       </c>
       <c r="V8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>5.7362401715511109E-2</v>
       </c>
     </row>
@@ -6289,7 +6423,7 @@
         <v>-0.46009</v>
       </c>
       <c r="D9" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.3701015018800645E-2</v>
       </c>
     </row>
@@ -6354,7 +6488,7 @@
         <v>-0.80013000000000001</v>
       </c>
       <c r="J12" s="6">
-        <f>ABS((H12-I12)/I12)</f>
+        <f t="shared" ref="J12:J18" si="4">ABS((H12-I12)/I12)</f>
         <v>0.12214265181907938</v>
       </c>
       <c r="M12" s="30" t="s">
@@ -6367,7 +6501,7 @@
         <v>-0.80013000000000001</v>
       </c>
       <c r="P12" s="6">
-        <f>ABS((N12-O12)/O12)</f>
+        <f t="shared" ref="P12:P18" si="5">ABS((N12-O12)/O12)</f>
         <v>0.12214265181907938</v>
       </c>
       <c r="S12" s="30" t="s">
@@ -6380,7 +6514,7 @@
         <v>-0.77080000000000004</v>
       </c>
       <c r="V12" s="6">
-        <f>ABS((T12-U12)/U12)</f>
+        <f t="shared" ref="V12:V18" si="6">ABS((T12-U12)/U12)</f>
         <v>8.873897249610796E-2</v>
       </c>
     </row>
@@ -6408,7 +6542,7 @@
         <v>-0.35829</v>
       </c>
       <c r="J13" s="6">
-        <f>ABS((H13-I13)/I13)</f>
+        <f t="shared" si="4"/>
         <v>0.149906500320969</v>
       </c>
       <c r="M13" s="6" t="s">
@@ -6421,7 +6555,7 @@
         <v>-0.35829</v>
       </c>
       <c r="P13" s="6">
-        <f>ABS((N13-O13)/O13)</f>
+        <f t="shared" si="5"/>
         <v>0.149906500320969</v>
       </c>
       <c r="S13" s="6" t="s">
@@ -6434,7 +6568,7 @@
         <v>-0.37140000000000001</v>
       </c>
       <c r="V13" s="6">
-        <f>ABS((T13-U13)/U13)</f>
+        <f t="shared" si="6"/>
         <v>0.10931610123855673</v>
       </c>
     </row>
@@ -6462,7 +6596,7 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" ref="J14:J15" si="8">ABS((H14-I14)/I14)</f>
+        <f t="shared" si="4"/>
         <v>3.278814059396145E-2</v>
       </c>
       <c r="M14" s="6" t="s">
@@ -6475,7 +6609,7 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="P14" s="6">
-        <f t="shared" ref="P14:P15" si="9">ABS((N14-O14)/O14)</f>
+        <f t="shared" si="5"/>
         <v>3.278814059396145E-2</v>
       </c>
       <c r="S14" s="6" t="s">
@@ -6488,7 +6622,7 @@
         <v>-2.2311999999999999</v>
       </c>
       <c r="V14" s="6">
-        <f t="shared" ref="V14:V15" si="10">ABS((T14-U14)/U14)</f>
+        <f t="shared" si="6"/>
         <v>2.7608461814270492E-2</v>
       </c>
     </row>
@@ -6516,7 +6650,7 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>4.7792973770004035E-2</v>
       </c>
       <c r="M15" s="6" t="s">
@@ -6529,7 +6663,7 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="P15" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>4.7792973770004035E-2</v>
       </c>
       <c r="S15" s="6" t="s">
@@ -6542,7 +6676,7 @@
         <v>-0.72</v>
       </c>
       <c r="V15" s="6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>2.2361111111111116E-2</v>
       </c>
     </row>
@@ -6570,7 +6704,7 @@
         <v>-0.25318000000000002</v>
       </c>
       <c r="J16" s="29">
-        <f>ABS((H16-I16)/I16)</f>
+        <f t="shared" si="4"/>
         <v>0.55186033651947231</v>
       </c>
       <c r="M16" s="26" t="s">
@@ -6583,7 +6717,7 @@
         <v>-0.25318000000000002</v>
       </c>
       <c r="P16" s="29">
-        <f>ABS((N16-O16)/O16)</f>
+        <f t="shared" si="5"/>
         <v>0.55186033651947231</v>
       </c>
       <c r="S16" s="26" t="s">
@@ -6596,7 +6730,7 @@
         <v>-0.3009</v>
       </c>
       <c r="V16" s="29">
-        <f>ABS((T16-U16)/U16)</f>
+        <f t="shared" si="6"/>
         <v>0.30574941841143244</v>
       </c>
     </row>
@@ -6624,7 +6758,7 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" ref="J17:J18" si="11">ABS((H17-I17)/I17)</f>
+        <f t="shared" si="4"/>
         <v>6.0814570375552962E-2</v>
       </c>
       <c r="M17" s="6" t="s">
@@ -6637,7 +6771,7 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="P17" s="6">
-        <f t="shared" ref="P17:P18" si="12">ABS((N17-O17)/O17)</f>
+        <f t="shared" si="5"/>
         <v>6.0814570375552962E-2</v>
       </c>
       <c r="S17" s="6" t="s">
@@ -6650,7 +6784,7 @@
         <v>-1.8142</v>
       </c>
       <c r="V17" s="6">
-        <f t="shared" ref="V17:V18" si="13">ABS((T17-U17)/U17)</f>
+        <f t="shared" si="6"/>
         <v>6.0302061514717196E-2</v>
       </c>
     </row>
@@ -6678,7 +6812,7 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>8.5812772133526866E-2</v>
       </c>
       <c r="M18" s="6" t="s">
@@ -6691,7 +6825,7 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="P18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>8.5812772133526866E-2</v>
       </c>
       <c r="S18" s="6" t="s">
@@ -6704,7 +6838,7 @@
         <v>-0.55959999999999999</v>
       </c>
       <c r="V18" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>9.9535382416011384E-2</v>
       </c>
     </row>
@@ -6779,10 +6913,10 @@
         <v>0.25609999999999999</v>
       </c>
       <c r="V22" s="34">
-        <f>ABS((T22-U22)/U22)</f>
+        <f t="shared" ref="V22:V29" si="8">ABS((T22-U22)/U22)</f>
         <v>0.21163607965638423</v>
       </c>
-      <c r="W22" s="64"/>
+      <c r="W22" s="43"/>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="23" t="s">
@@ -6807,7 +6941,7 @@
         <v>-0.80013000000000001</v>
       </c>
       <c r="J23" s="6">
-        <f>ABS((H23-I23)/I23)</f>
+        <f t="shared" ref="J23:J30" si="9">ABS((H23-I23)/I23)</f>
         <v>0.11401897191706352</v>
       </c>
       <c r="S23" s="30" t="s">
@@ -6820,7 +6954,7 @@
         <v>-0.77080000000000004</v>
       </c>
       <c r="V23" s="6">
-        <f>ABS((T23-U23)/U23)</f>
+        <f t="shared" si="8"/>
         <v>8.030617540217963E-2</v>
       </c>
     </row>
@@ -6848,7 +6982,7 @@
         <v>0.24659</v>
       </c>
       <c r="J24" s="6">
-        <f>ABS((H24-I24)/I24)</f>
+        <f t="shared" si="9"/>
         <v>0.18123200454195226</v>
       </c>
       <c r="S24" s="6" t="s">
@@ -6861,7 +6995,7 @@
         <v>-0.37140000000000001</v>
       </c>
       <c r="V24" s="6">
-        <f>ABS((T24-U24)/U24)</f>
+        <f t="shared" si="8"/>
         <v>0.17312870220786206</v>
       </c>
     </row>
@@ -6876,7 +7010,7 @@
         <v>-1.2237</v>
       </c>
       <c r="D25" s="6">
-        <f t="shared" ref="D25:D32" si="14">ABS((B25-C25)/C25)</f>
+        <f t="shared" ref="D25:D32" si="10">ABS((B25-C25)/C25)</f>
         <v>2.1001879545640319E-2</v>
       </c>
       <c r="G25" s="6" t="s">
@@ -6889,7 +7023,7 @@
         <v>-0.35829</v>
       </c>
       <c r="J25" s="34">
-        <f>ABS((H25-I25)/I25)</f>
+        <f t="shared" si="9"/>
         <v>0.21605403444137425</v>
       </c>
       <c r="S25" s="6" t="s">
@@ -6902,7 +7036,7 @@
         <v>-2.2311999999999999</v>
       </c>
       <c r="V25" s="6">
-        <f t="shared" ref="V25:V26" si="15">ABS((T25-U25)/U25)</f>
+        <f t="shared" si="8"/>
         <v>3.4376120473288016E-2</v>
       </c>
     </row>
@@ -6917,7 +7051,7 @@
         <v>-2.4157999999999999</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>4.4871264177498163E-2</v>
       </c>
       <c r="G26" s="6" t="s">
@@ -6930,7 +7064,7 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J26" s="6">
-        <f t="shared" ref="J26:J27" si="16">ABS((H26-I26)/I26)</f>
+        <f t="shared" si="9"/>
         <v>3.9589911757154359E-2</v>
       </c>
       <c r="S26" s="6" t="s">
@@ -6943,7 +7077,7 @@
         <v>-0.72</v>
       </c>
       <c r="V26" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="8"/>
         <v>1.5277777777777791E-2</v>
       </c>
     </row>
@@ -6958,7 +7092,7 @@
         <v>0.63932999999999995</v>
       </c>
       <c r="D27" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>9.5052633225407843E-2</v>
       </c>
       <c r="G27" s="6" t="s">
@@ -6971,7 +7105,7 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J27" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>4.0893903115403987E-2</v>
       </c>
       <c r="S27" s="26" t="s">
@@ -6984,7 +7118,7 @@
         <v>-0.3009</v>
       </c>
       <c r="V27" s="29">
-        <f>ABS((T27-U27)/U27)</f>
+        <f t="shared" si="8"/>
         <v>0.22033898305084754</v>
       </c>
     </row>
@@ -6999,7 +7133,7 @@
         <v>-0.40884999999999999</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>3.2163385104561563E-2</v>
       </c>
       <c r="G28" s="26" t="s">
@@ -7012,7 +7146,7 @@
         <v>-0.25318000000000002</v>
       </c>
       <c r="J28" s="29">
-        <f>ABS((H28-I28)/I28)</f>
+        <f t="shared" si="9"/>
         <v>0.45035152855675803</v>
       </c>
       <c r="S28" s="6" t="s">
@@ -7025,7 +7159,7 @@
         <v>-1.8142</v>
       </c>
       <c r="V28" s="6">
-        <f t="shared" ref="V28:V29" si="17">ABS((T28-U28)/U28)</f>
+        <f t="shared" si="8"/>
         <v>2.6072097894388777E-2</v>
       </c>
     </row>
@@ -7040,7 +7174,7 @@
         <v>-1.88056</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>9.7098736546560298E-3</v>
       </c>
       <c r="G29" s="6" t="s">
@@ -7053,7 +7187,7 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J29" s="6">
-        <f t="shared" ref="J29" si="18">ABS((H29-I29)/I29)</f>
+        <f t="shared" si="9"/>
         <v>2.6603275690148229E-2</v>
       </c>
       <c r="S29" s="6" t="s">
@@ -7066,7 +7200,7 @@
         <v>-0.55959999999999999</v>
       </c>
       <c r="V29" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>5.1644031451036521E-2</v>
       </c>
     </row>
@@ -7081,7 +7215,7 @@
         <v>-0.46009</v>
       </c>
       <c r="D30" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>7.2616227259883925E-2</v>
       </c>
       <c r="G30" s="6" t="s">
@@ -7094,7 +7228,7 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J30" s="6">
-        <f>ABS((H30-I30)/I30)</f>
+        <f t="shared" si="9"/>
         <v>3.7191582002902887E-2</v>
       </c>
     </row>
@@ -7109,7 +7243,7 @@
         <v>-0.24127999999999999</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>0.18824602122015921</v>
       </c>
     </row>
@@ -7124,7 +7258,7 @@
         <v>0.22370000000000001</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.4751899865891807E-2</v>
       </c>
       <c r="S32" s="23" t="s">
@@ -7163,7 +7297,7 @@
         <v>-0.2132</v>
       </c>
       <c r="V33" s="8">
-        <f>ABS((T33-U33)/U33)</f>
+        <f t="shared" ref="V33:V41" si="11">ABS((T33-U33)/U33)</f>
         <v>4.0806754221388429E-2</v>
       </c>
     </row>
@@ -7178,7 +7312,7 @@
         <v>-0.80013000000000001</v>
       </c>
       <c r="J34" s="6">
-        <f>ABS((H34-I34)/I34)</f>
+        <f t="shared" ref="J34:J42" si="12">ABS((H34-I34)/I34)</f>
         <v>7.7149963130991289E-2</v>
       </c>
       <c r="S34" s="30" t="s">
@@ -7191,7 +7325,7 @@
         <v>0.25609999999999999</v>
       </c>
       <c r="V34" s="34">
-        <f>ABS((T34-U34)/U34)</f>
+        <f t="shared" si="11"/>
         <v>9.8008590394377135E-2</v>
       </c>
     </row>
@@ -7206,7 +7340,7 @@
         <v>0.24659</v>
       </c>
       <c r="J35" s="6">
-        <f>ABS((H35-I35)/I35)</f>
+        <f t="shared" si="12"/>
         <v>6.3222352893466852E-2</v>
       </c>
       <c r="S35" s="30" t="s">
@@ -7219,7 +7353,7 @@
         <v>-0.77080000000000004</v>
       </c>
       <c r="V35" s="6">
-        <f>ABS((T35-U35)/U35)</f>
+        <f t="shared" si="11"/>
         <v>4.2034250129735461E-2</v>
       </c>
     </row>
@@ -7234,7 +7368,7 @@
         <v>-0.25905</v>
       </c>
       <c r="J36" s="34">
-        <f>ABS((H36-I36)/I36)</f>
+        <f t="shared" si="12"/>
         <v>0.21057710866628071</v>
       </c>
       <c r="S36" s="6" t="s">
@@ -7247,7 +7381,7 @@
         <v>-0.37140000000000001</v>
       </c>
       <c r="V36" s="6">
-        <f>ABS((T36-U36)/U36)</f>
+        <f t="shared" si="11"/>
         <v>4.1195476575121112E-2</v>
       </c>
     </row>
@@ -7262,7 +7396,7 @@
         <v>-0.35829</v>
       </c>
       <c r="J37" s="8">
-        <f>ABS((H37-I37)/I37)</f>
+        <f t="shared" si="12"/>
         <v>7.929330988863767E-2</v>
       </c>
       <c r="S37" s="6" t="s">
@@ -7275,7 +7409,7 @@
         <v>-2.2311999999999999</v>
       </c>
       <c r="V37" s="6">
-        <f t="shared" ref="V37:V38" si="19">ABS((T37-U37)/U37)</f>
+        <f t="shared" si="11"/>
         <v>1.8375761921836746E-3</v>
       </c>
     </row>
@@ -7290,7 +7424,7 @@
         <v>-2.2200099999999998</v>
       </c>
       <c r="J38" s="6">
-        <f t="shared" ref="J38:J39" si="20">ABS((H38-I38)/I38)</f>
+        <f t="shared" si="12"/>
         <v>6.8873563632597373E-3</v>
       </c>
       <c r="S38" s="6" t="s">
@@ -7303,7 +7437,7 @@
         <v>-0.72</v>
       </c>
       <c r="V38" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>1.6805555555555556E-2</v>
       </c>
     </row>
@@ -7318,7 +7452,7 @@
         <v>-0.73923000000000005</v>
       </c>
       <c r="J39" s="6">
-        <f t="shared" si="20"/>
+        <f t="shared" si="12"/>
         <v>9.6451713269213642E-3</v>
       </c>
       <c r="S39" s="26" t="s">
@@ -7331,7 +7465,7 @@
         <v>-0.3009</v>
       </c>
       <c r="V39" s="29">
-        <f>ABS((T39-U39)/U39)</f>
+        <f t="shared" si="11"/>
         <v>0.13094051179793947</v>
       </c>
     </row>
@@ -7346,7 +7480,7 @@
         <v>-0.25318000000000002</v>
       </c>
       <c r="J40" s="29">
-        <f>ABS((H40-I40)/I40)</f>
+        <f t="shared" si="12"/>
         <v>0.34410300971640717</v>
       </c>
       <c r="S40" s="6" t="s">
@@ -7359,7 +7493,7 @@
         <v>-1.8142</v>
       </c>
       <c r="V40" s="6">
-        <f t="shared" ref="V40:V41" si="21">ABS((T40-U40)/U40)</f>
+        <f t="shared" si="11"/>
         <v>2.8332047183331557E-2</v>
       </c>
     </row>
@@ -7374,7 +7508,7 @@
         <v>-1.8151900000000001</v>
       </c>
       <c r="J41" s="6">
-        <f t="shared" ref="J41:J42" si="22">ABS((H41-I41)/I41)</f>
+        <f t="shared" si="12"/>
         <v>2.8861992408508286E-2</v>
       </c>
       <c r="S41" s="6" t="s">
@@ -7387,7 +7521,7 @@
         <v>-0.55959999999999999</v>
       </c>
       <c r="V41" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="11"/>
         <v>5.5932809149392415E-2</v>
       </c>
     </row>
@@ -7402,620 +7536,1342 @@
         <v>-0.55120000000000002</v>
       </c>
       <c r="J42" s="6">
-        <f t="shared" si="22"/>
+        <f t="shared" si="12"/>
         <v>4.1545718432510939E-2</v>
       </c>
-    </row>
-    <row r="45" spans="7:22">
-      <c r="G45" s="23" t="s">
+      <c r="S42" s="56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="46" spans="7:22">
+      <c r="G46" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="H45" s="23" t="s">
+      <c r="H46" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="I45" s="23" t="s">
+      <c r="I46" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="J45" s="24" t="s">
+      <c r="J46" s="24" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="46" spans="7:22">
-      <c r="G46" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" s="13">
-        <v>-0.79220000000000002</v>
-      </c>
-      <c r="I46" s="13">
-        <v>-0.80013000000000001</v>
-      </c>
-      <c r="J46" s="6">
-        <f>ABS((H46-I46)/I46)</f>
-        <v>9.9108894804594162E-3</v>
+      <c r="S46" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="47" spans="7:22">
       <c r="G47" s="30" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H47" s="13">
-        <v>0.22750000000000001</v>
+        <v>-0.79220000000000002</v>
       </c>
       <c r="I47" s="13">
-        <v>0.24659</v>
+        <v>-0.80013000000000001</v>
       </c>
       <c r="J47" s="6">
-        <f>ABS((H47-I47)/I47)</f>
-        <v>7.7415953607202215E-2</v>
+        <f t="shared" ref="J47:J56" si="13">ABS((H47-I47)/I47)</f>
+        <v>9.9108894804594162E-3</v>
       </c>
     </row>
     <row r="48" spans="7:22">
       <c r="G48" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="13">
+        <v>0.22750000000000001</v>
+      </c>
+      <c r="I48" s="13">
+        <v>0.24659</v>
+      </c>
+      <c r="J48" s="6">
+        <f t="shared" si="13"/>
+        <v>7.7415953607202215E-2</v>
+      </c>
+      <c r="S48" s="55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="7:23">
+      <c r="G49" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="H48" s="13">
+      <c r="H49" s="13">
         <v>-0.19139999999999999</v>
       </c>
-      <c r="I48" s="13">
+      <c r="I49" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="J48" s="8">
-        <f>ABS((H48-I48)/I48)</f>
+      <c r="J49" s="8">
+        <f t="shared" si="13"/>
         <v>0.26114649681528668</v>
       </c>
     </row>
-    <row r="49" spans="7:10">
-      <c r="G49" s="30" t="s">
+    <row r="50" spans="7:23">
+      <c r="G50" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="H49" s="13">
+      <c r="H50" s="13">
         <v>0.2757</v>
       </c>
-      <c r="I49" s="13">
+      <c r="I50" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="J49" s="8">
-        <f>ABS((H49-I49)/I49)</f>
+      <c r="J50" s="8">
+        <f t="shared" si="13"/>
         <v>0.19609544468546633</v>
       </c>
-    </row>
-    <row r="50" spans="7:10">
-      <c r="G50" s="6" t="s">
+      <c r="S50" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="T50" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="U50" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="V50" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="W50" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="7:23">
+      <c r="G51" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="6">
+      <c r="H51" s="6">
         <v>-0.37459999999999999</v>
       </c>
-      <c r="I50" s="6">
+      <c r="I51" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="J50" s="8">
-        <f>ABS((H50-I50)/I50)</f>
+      <c r="J51" s="8">
+        <f t="shared" si="13"/>
         <v>4.5521784029696588E-2</v>
       </c>
-    </row>
-    <row r="51" spans="7:10">
-      <c r="G51" s="6" t="s">
+      <c r="S51" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="T51" s="49">
+        <v>-0.72529999999999994</v>
+      </c>
+      <c r="U51" s="49">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V51" s="57">
+        <f t="shared" ref="V51:V56" si="14">ABS((T51-U51)/U51)</f>
+        <v>5.9029579657498825E-2</v>
+      </c>
+      <c r="W51" s="49">
+        <v>0.26108999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="7:23">
+      <c r="G52" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H52" s="6">
         <v>-2.2584</v>
       </c>
-      <c r="I51" s="6">
+      <c r="I52" s="6">
         <v>-2.2200099999999998</v>
       </c>
-      <c r="J51" s="8">
-        <f t="shared" ref="J51:J52" si="23">ABS((H51-I51)/I51)</f>
+      <c r="J52" s="8">
+        <f t="shared" si="13"/>
         <v>1.7292714897680708E-2</v>
       </c>
-    </row>
-    <row r="52" spans="7:10">
-      <c r="G52" s="6" t="s">
+      <c r="S52" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="T52" s="49">
+        <v>-0.28029999999999999</v>
+      </c>
+      <c r="U52" s="49">
+        <v>-0.2132</v>
+      </c>
+      <c r="V52" s="54">
+        <f t="shared" si="14"/>
+        <v>0.3147279549718574</v>
+      </c>
+      <c r="W52" s="49">
+        <v>0.34028000000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="7:23">
+      <c r="G53" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H53" s="6">
         <v>-0.71319999999999995</v>
       </c>
-      <c r="I52" s="6">
+      <c r="I53" s="6">
         <v>-0.73923000000000005</v>
       </c>
-      <c r="J52" s="8">
-        <f t="shared" si="23"/>
+      <c r="J53" s="8">
+        <f t="shared" si="13"/>
         <v>3.521231551749808E-2</v>
       </c>
-    </row>
-    <row r="53" spans="7:10">
-      <c r="G53" s="26" t="s">
+      <c r="S53" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="T53" s="49">
+        <v>-2.2658</v>
+      </c>
+      <c r="U53" s="49">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V53" s="49">
+        <f t="shared" si="14"/>
+        <v>1.5507350304768819E-2</v>
+      </c>
+      <c r="W53" s="49">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="7:23">
+      <c r="G54" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H53" s="28">
+      <c r="H54" s="28">
         <v>-0.32250000000000001</v>
       </c>
-      <c r="I53" s="26">
+      <c r="I54" s="26">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="J53" s="29">
-        <f>ABS((H53-I53)/I53)</f>
+      <c r="J54" s="29">
+        <f t="shared" si="13"/>
         <v>0.27379729836479971</v>
       </c>
-    </row>
-    <row r="54" spans="7:10">
-      <c r="G54" s="6" t="s">
+      <c r="S54" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="T54" s="49">
+        <v>-0.77800000000000002</v>
+      </c>
+      <c r="U54" s="49">
+        <v>-0.72</v>
+      </c>
+      <c r="V54" s="49">
+        <f t="shared" si="14"/>
+        <v>8.055555555555563E-2</v>
+      </c>
+      <c r="W54" s="49">
+        <v>5.0600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="7:23">
+      <c r="G55" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="6">
+      <c r="H55" s="6">
         <v>-1.7566999999999999</v>
       </c>
-      <c r="I54" s="6">
+      <c r="I55" s="6">
         <v>-1.8151900000000001</v>
       </c>
-      <c r="J54" s="6">
-        <f t="shared" ref="J54:J55" si="24">ABS((H54-I54)/I54)</f>
+      <c r="J55" s="6">
+        <f t="shared" si="13"/>
         <v>3.2222522160214713E-2</v>
       </c>
-    </row>
-    <row r="55" spans="7:10">
-      <c r="G55" s="6" t="s">
+      <c r="S55" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="T55" s="52">
+        <v>-1.6968000000000001</v>
+      </c>
+      <c r="U55" s="52">
+        <v>-1.8142</v>
+      </c>
+      <c r="V55" s="49">
+        <f t="shared" si="14"/>
+        <v>6.471171866387386E-2</v>
+      </c>
+      <c r="W55" s="53">
+        <v>4.5699999999999997E-9</v>
+      </c>
+    </row>
+    <row r="56" spans="7:23">
+      <c r="G56" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H56" s="6">
         <v>-0.53120000000000001</v>
       </c>
-      <c r="I55" s="6">
+      <c r="I56" s="6">
         <v>-0.55120000000000002</v>
       </c>
-      <c r="J55" s="6">
-        <f t="shared" si="24"/>
+      <c r="J56" s="6">
+        <f t="shared" si="13"/>
         <v>3.6284470246734431E-2</v>
       </c>
-    </row>
-    <row r="58" spans="7:10">
-      <c r="G58" s="23" t="s">
+      <c r="S56" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="T56" s="49">
+        <v>-0.55720000000000003</v>
+      </c>
+      <c r="U56" s="49">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V56" s="49">
+        <f t="shared" si="14"/>
+        <v>4.2887776983558928E-3</v>
+      </c>
+      <c r="W56" s="49">
+        <v>5.7110000000000001E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="7:23">
+      <c r="G59" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="H58" s="23" t="s">
+      <c r="H59" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="I58" s="23" t="s">
+      <c r="I59" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="24" t="s">
+      <c r="J59" s="24" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="59" spans="7:10">
-      <c r="G59" s="30" t="s">
+      <c r="S59" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="T59" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="U59" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="V59" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="W59" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="7:23">
+      <c r="G60" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="H59" s="13">
+      <c r="H60" s="13">
         <v>-0.80789999999999995</v>
       </c>
-      <c r="I59" s="13">
+      <c r="I60" s="13">
         <v>-0.80013000000000001</v>
       </c>
-      <c r="J59" s="6">
-        <f>ABS((H59-I59)/I59)</f>
+      <c r="J60" s="6">
+        <f t="shared" ref="J60:J71" si="15">ABS((H60-I60)/I60)</f>
         <v>9.7109219751789627E-3</v>
       </c>
-    </row>
-    <row r="60" spans="7:10">
-      <c r="G60" s="30" t="s">
+      <c r="S60" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="T60" s="57">
+        <v>-0.33400000000000002</v>
+      </c>
+      <c r="U60" s="57">
+        <v>-0.3009</v>
+      </c>
+      <c r="V60" s="57">
+        <f t="shared" ref="V60:V66" si="16">ABS((T60-U60)/U60)</f>
+        <v>0.11000332336324366</v>
+      </c>
+      <c r="W60" s="57">
+        <v>6.0699999999999999E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="7:23">
+      <c r="G61" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H60" s="13">
+      <c r="H61" s="13">
         <v>0.26939999999999997</v>
       </c>
-      <c r="I60" s="13">
+      <c r="I61" s="13">
         <v>0.24659</v>
       </c>
-      <c r="J60" s="6">
-        <f>ABS((H60-I60)/I60)</f>
+      <c r="J61" s="6">
+        <f t="shared" si="15"/>
         <v>9.2501723508657971E-2</v>
       </c>
-    </row>
-    <row r="61" spans="7:10">
-      <c r="G61" s="30" t="s">
+      <c r="S61" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="T61" s="49">
+        <v>-0.72419999999999995</v>
+      </c>
+      <c r="U61" s="49">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V61" s="57">
+        <f t="shared" si="16"/>
+        <v>6.0456668396471305E-2</v>
+      </c>
+      <c r="W61" s="49">
+        <v>0.26108999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="7:23">
+      <c r="G62" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="H61" s="13">
+      <c r="H62" s="13">
         <v>-0.21590000000000001</v>
       </c>
-      <c r="I61" s="13">
+      <c r="I62" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="J61" s="8">
-        <f>ABS((H61-I61)/I61)</f>
+      <c r="J62" s="8">
+        <f t="shared" si="15"/>
         <v>0.16657016020073342</v>
       </c>
-    </row>
-    <row r="62" spans="7:10">
-      <c r="G62" s="30" t="s">
+      <c r="S62" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="T62" s="49">
+        <v>-0.25609999999999999</v>
+      </c>
+      <c r="U62" s="49">
+        <v>-0.2132</v>
+      </c>
+      <c r="V62" s="54">
+        <f t="shared" si="16"/>
+        <v>0.20121951219512191</v>
+      </c>
+      <c r="W62" s="49">
+        <v>0.34028000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="7:23">
+      <c r="G63" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="H62" s="13">
+      <c r="H63" s="13">
         <v>0.26889999999999997</v>
       </c>
-      <c r="I62" s="13">
+      <c r="I63" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="J62" s="8">
-        <f>ABS((H62-I62)/I62)</f>
+      <c r="J63" s="8">
+        <f t="shared" si="15"/>
         <v>0.16659436008676773</v>
       </c>
-    </row>
-    <row r="63" spans="7:10">
-      <c r="G63" s="30" t="s">
+      <c r="S63" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="T63" s="49">
+        <v>-2.1962999999999999</v>
+      </c>
+      <c r="U63" s="49">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V63" s="49">
+        <f t="shared" si="16"/>
+        <v>1.5641807099318724E-2</v>
+      </c>
+      <c r="W63" s="49">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="7:23">
+      <c r="G64" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H63" s="13">
+      <c r="H64" s="13">
         <v>0.28620000000000001</v>
       </c>
-      <c r="I63" s="13">
+      <c r="I64" s="13">
         <v>0.30564000000000002</v>
       </c>
-      <c r="J63" s="8">
-        <f t="shared" ref="J63:J64" si="25">ABS((H63-I63)/I63)</f>
+      <c r="J64" s="8">
+        <f t="shared" si="15"/>
         <v>6.3604240282685548E-2</v>
       </c>
-    </row>
-    <row r="64" spans="7:10">
-      <c r="G64" s="30" t="s">
+      <c r="S64" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="T64" s="49">
+        <v>-0.76349999999999996</v>
+      </c>
+      <c r="U64" s="49">
+        <v>-0.72</v>
+      </c>
+      <c r="V64" s="49">
+        <f t="shared" si="16"/>
+        <v>6.0416666666666646E-2</v>
+      </c>
+      <c r="W64" s="49">
+        <v>5.0600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="7:23">
+      <c r="G65" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="H64" s="13">
+      <c r="H65" s="13">
         <v>0.1125</v>
       </c>
-      <c r="I64" s="13">
+      <c r="I65" s="13">
         <v>0.15532000000000001</v>
       </c>
-      <c r="J64" s="34">
-        <f t="shared" si="25"/>
+      <c r="J65" s="34">
+        <f t="shared" si="15"/>
         <v>0.27568890033479271</v>
       </c>
-    </row>
-    <row r="65" spans="7:10">
-      <c r="G65" s="6" t="s">
+      <c r="S65" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="T65" s="52">
+        <v>-1.6696</v>
+      </c>
+      <c r="U65" s="52">
+        <v>-1.8142</v>
+      </c>
+      <c r="V65" s="49">
+        <f t="shared" si="16"/>
+        <v>7.9704552971006537E-2</v>
+      </c>
+      <c r="W65" s="53">
+        <v>4.5699999999999997E-9</v>
+      </c>
+    </row>
+    <row r="66" spans="7:23">
+      <c r="G66" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="6">
+      <c r="H66" s="6">
         <v>-0.37290000000000001</v>
       </c>
-      <c r="I65" s="6">
+      <c r="I66" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="J65" s="8">
-        <f>ABS((H65-I65)/I65)</f>
+      <c r="J66" s="8">
+        <f t="shared" si="15"/>
         <v>4.0777024198275176E-2</v>
       </c>
-    </row>
-    <row r="66" spans="7:10">
-      <c r="G66" s="6" t="s">
+      <c r="S66" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="T66" s="49">
+        <v>-0.5252</v>
+      </c>
+      <c r="U66" s="49">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V66" s="49">
+        <f t="shared" si="16"/>
+        <v>6.1472480343102195E-2</v>
+      </c>
+      <c r="W66" s="49">
+        <v>5.7110000000000001E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="7:23">
+      <c r="G67" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H66" s="6">
+      <c r="H67" s="6">
         <v>-2.2570000000000001</v>
       </c>
-      <c r="I66" s="6">
+      <c r="I67" s="6">
         <v>-2.2200099999999998</v>
       </c>
-      <c r="J66" s="8">
-        <f t="shared" ref="J66:J67" si="26">ABS((H66-I66)/I66)</f>
+      <c r="J67" s="8">
+        <f t="shared" si="15"/>
         <v>1.6662087107715867E-2</v>
       </c>
     </row>
-    <row r="67" spans="7:10">
-      <c r="G67" s="6" t="s">
+    <row r="68" spans="7:23">
+      <c r="G68" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H67" s="6">
+      <c r="H68" s="6">
         <v>-0.71109999999999995</v>
       </c>
-      <c r="I67" s="6">
+      <c r="I68" s="6">
         <v>-0.73923000000000005</v>
       </c>
-      <c r="J67" s="8">
-        <f t="shared" si="26"/>
+      <c r="J68" s="8">
+        <f t="shared" si="15"/>
         <v>3.8053109316451034E-2</v>
       </c>
     </row>
-    <row r="68" spans="7:10">
-      <c r="G68" s="26" t="s">
+    <row r="69" spans="7:23">
+      <c r="G69" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H68" s="28">
+      <c r="H69" s="28">
         <v>-0.30740000000000001</v>
       </c>
-      <c r="I68" s="26">
+      <c r="I69" s="26">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="J68" s="29">
-        <f>ABS((H68-I68)/I68)</f>
+      <c r="J69" s="29">
+        <f t="shared" si="15"/>
         <v>0.21415593648787418</v>
       </c>
-    </row>
-    <row r="69" spans="7:10">
-      <c r="G69" s="6" t="s">
+      <c r="S69" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="T69" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="U69" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="V69" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="W69" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="7:23">
+      <c r="G70" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H69" s="6">
+      <c r="H70" s="6">
         <v>-1.7656000000000001</v>
       </c>
-      <c r="I69" s="6">
+      <c r="I70" s="6">
         <v>-1.8151900000000001</v>
       </c>
-      <c r="J69" s="6">
-        <f t="shared" ref="J69:J70" si="27">ABS((H69-I69)/I69)</f>
+      <c r="J70" s="6">
+        <f t="shared" si="15"/>
         <v>2.7319454161823291E-2</v>
       </c>
-    </row>
-    <row r="70" spans="7:10">
-      <c r="G70" s="6" t="s">
+      <c r="S70" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="T70" s="57">
+        <v>-0.36630000000000001</v>
+      </c>
+      <c r="U70" s="57">
+        <v>-0.37140000000000001</v>
+      </c>
+      <c r="V70" s="57">
+        <f t="shared" ref="V70:V77" si="17">ABS((T70-U70)/U70)</f>
+        <v>1.373182552504037E-2</v>
+      </c>
+      <c r="W70" s="57">
+        <v>0.27082000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="7:23">
+      <c r="G71" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H70" s="6">
+      <c r="H71" s="6">
         <v>-0.55810000000000004</v>
       </c>
-      <c r="I70" s="6">
+      <c r="I71" s="6">
         <v>-0.55120000000000002</v>
       </c>
-      <c r="J70" s="6">
-        <f t="shared" si="27"/>
+      <c r="J71" s="6">
+        <f t="shared" si="15"/>
         <v>1.2518142235123398E-2</v>
       </c>
-    </row>
-    <row r="72" spans="7:10">
-      <c r="G72" s="23" t="s">
+      <c r="S71" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="T71" s="57">
+        <v>-0.37280000000000002</v>
+      </c>
+      <c r="U71" s="57">
+        <v>-0.3009</v>
+      </c>
+      <c r="V71" s="54">
+        <f t="shared" si="17"/>
+        <v>0.23894981721502168</v>
+      </c>
+      <c r="W71" s="57">
+        <v>6.0699999999999999E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="7:23">
+      <c r="S72" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="T72" s="49">
+        <v>-0.7268</v>
+      </c>
+      <c r="U72" s="49">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V72" s="57">
+        <f t="shared" si="17"/>
+        <v>5.7083549558899889E-2</v>
+      </c>
+      <c r="W72" s="49">
+        <v>0.26108999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="7:23">
+      <c r="G73" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="H72" s="23" t="s">
+      <c r="H73" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="I72" s="23" t="s">
+      <c r="I73" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="J72" s="24" t="s">
+      <c r="J73" s="24" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="73" spans="7:10">
-      <c r="G73" s="30" t="s">
+      <c r="S73" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="T73" s="49">
+        <v>-0.17369999999999999</v>
+      </c>
+      <c r="U73" s="49">
+        <v>-0.2132</v>
+      </c>
+      <c r="V73" s="57">
+        <f t="shared" si="17"/>
+        <v>0.18527204502814262</v>
+      </c>
+      <c r="W73" s="49">
+        <v>0.34028000000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="7:23">
+      <c r="G74" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="H73" s="13">
+      <c r="H74" s="13">
         <v>-0.80013000000000001</v>
       </c>
-      <c r="I73" s="13">
+      <c r="I74" s="13">
         <v>-0.80013000000000001</v>
       </c>
-      <c r="J73" s="8">
-        <f t="shared" ref="J73:J88" si="28">ABS((H73-I73)/I73)</f>
+      <c r="J74" s="8">
+        <f t="shared" ref="J74:J89" si="18">ABS((H74-I74)/I74)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="7:10">
-      <c r="G74" s="30" t="s">
+      <c r="S74" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="T74" s="49">
+        <v>-2.2286000000000001</v>
+      </c>
+      <c r="U74" s="49">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V74" s="49">
+        <f t="shared" si="17"/>
+        <v>1.1652922194333604E-3</v>
+      </c>
+      <c r="W74" s="49">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="7:23">
+      <c r="G75" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H74" s="13">
+      <c r="H75" s="13">
         <v>0.24659</v>
       </c>
-      <c r="I74" s="13">
+      <c r="I75" s="13">
         <v>0.24659</v>
       </c>
-      <c r="J74" s="8">
-        <f t="shared" si="28"/>
+      <c r="J75" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="7:10">
-      <c r="G75" s="30" t="s">
+      <c r="S75" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="T75" s="49">
+        <v>-0.72309999999999997</v>
+      </c>
+      <c r="U75" s="49">
+        <v>-0.72</v>
+      </c>
+      <c r="V75" s="49">
+        <f t="shared" si="17"/>
+        <v>4.3055555555555442E-3</v>
+      </c>
+      <c r="W75" s="49">
+        <v>5.0600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="7:23">
+      <c r="G76" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="H75" s="13">
+      <c r="H76" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="I75" s="13">
+      <c r="I76" s="13">
         <v>-0.25905</v>
       </c>
-      <c r="J75" s="8">
-        <f t="shared" si="28"/>
+      <c r="J76" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="7:10">
-      <c r="G76" s="30" t="s">
+      <c r="S76" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="T76" s="52">
+        <v>-1.6936</v>
+      </c>
+      <c r="U76" s="52">
+        <v>-1.8142</v>
+      </c>
+      <c r="V76" s="49">
+        <f t="shared" si="17"/>
+        <v>6.6475581523536567E-2</v>
+      </c>
+      <c r="W76" s="53">
+        <v>4.5699999999999997E-9</v>
+      </c>
+    </row>
+    <row r="77" spans="7:23">
+      <c r="G77" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="H76" s="13">
+      <c r="H77" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="I76" s="13">
+      <c r="I77" s="13">
         <v>0.23050000000000001</v>
       </c>
-      <c r="J76" s="8">
-        <f t="shared" si="28"/>
+      <c r="J77" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="7:10">
-      <c r="G77" s="30" t="s">
+      <c r="S77" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="T77" s="49">
+        <v>-0.49869999999999998</v>
+      </c>
+      <c r="U77" s="49">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V77" s="49">
+        <f t="shared" si="17"/>
+        <v>0.10882773409578272</v>
+      </c>
+      <c r="W77" s="49">
+        <v>5.7110000000000001E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="7:23">
+      <c r="G78" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="H77" s="13">
+      <c r="H78" s="13">
         <v>0.30564000000000002</v>
       </c>
-      <c r="I77" s="13">
+      <c r="I78" s="13">
         <v>0.30564000000000002</v>
       </c>
-      <c r="J77" s="8">
-        <f t="shared" si="28"/>
+      <c r="J78" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="7:10">
-      <c r="G78" s="30" t="s">
+    <row r="79" spans="7:23">
+      <c r="G79" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="H78" s="13">
+      <c r="H79" s="13">
         <v>0.15532000000000001</v>
       </c>
-      <c r="I78" s="13">
+      <c r="I79" s="13">
         <v>0.15532000000000001</v>
       </c>
-      <c r="J78" s="8">
-        <f t="shared" si="28"/>
+      <c r="J79" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="7:10">
-      <c r="G79" s="30" t="s">
+    <row r="80" spans="7:23">
+      <c r="G80" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="H79" s="13">
+      <c r="H80" s="13">
         <v>0.26494000000000001</v>
       </c>
-      <c r="I79" s="13">
+      <c r="I80" s="13">
         <v>0.26494000000000001</v>
       </c>
-      <c r="J79" s="8">
-        <f t="shared" si="28"/>
+      <c r="J80" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="7:10">
-      <c r="G80" s="30" t="s">
+      <c r="S80" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="T80" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="U80" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="V80" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="W80" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="7:23">
+      <c r="G81" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="H80" s="13">
+      <c r="H81" s="13">
         <v>0.29258000000000001</v>
       </c>
-      <c r="I80" s="13">
+      <c r="I81" s="13">
         <v>0.29258000000000001</v>
       </c>
-      <c r="J80" s="8">
-        <f t="shared" si="28"/>
+      <c r="J81" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="7:10">
-      <c r="G81" s="30" t="s">
+      <c r="S81" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="T81" s="57">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="U81" s="57">
+        <v>0.25609999999999999</v>
+      </c>
+      <c r="V81" s="57">
+        <f>ABS((T81-U81)/U81)</f>
+        <v>9.8008590394377135E-2</v>
+      </c>
+      <c r="W81" s="57">
+        <v>0.46418999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="7:23">
+      <c r="G82" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="H81" s="13">
+      <c r="H82" s="13">
         <v>-5.5890000000000002E-2</v>
       </c>
-      <c r="I81" s="13">
+      <c r="I82" s="13">
         <v>-5.5890000000000002E-2</v>
       </c>
-      <c r="J81" s="8">
-        <f t="shared" si="28"/>
+      <c r="J82" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="7:10">
-      <c r="G82" s="30" t="s">
+      <c r="S82" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="T82" s="57">
+        <v>-0.38669999999999999</v>
+      </c>
+      <c r="U82" s="57">
+        <v>-0.37140000000000001</v>
+      </c>
+      <c r="V82" s="57">
+        <f t="shared" ref="V82:V89" si="19">ABS((T82-U82)/U82)</f>
+        <v>4.1195476575121112E-2</v>
+      </c>
+      <c r="W82" s="57">
+        <v>0.27082000000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="7:23">
+      <c r="G83" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="H82" s="13">
+      <c r="H83" s="13">
         <v>-0.12130000000000001</v>
       </c>
-      <c r="I82" s="13">
+      <c r="I83" s="13">
         <v>-0.12130000000000001</v>
       </c>
-      <c r="J82" s="8">
-        <f t="shared" si="28"/>
+      <c r="J83" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="7:10">
-      <c r="G83" s="6" t="s">
+      <c r="S83" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="T83" s="57">
+        <v>-0.34029999999999999</v>
+      </c>
+      <c r="U83" s="57">
+        <v>-0.3009</v>
+      </c>
+      <c r="V83" s="57">
+        <f t="shared" si="19"/>
+        <v>0.13094051179793947</v>
+      </c>
+      <c r="W83" s="57">
+        <v>6.0699999999999999E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="7:23">
+      <c r="G84" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H83" s="6">
+      <c r="H84" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="I83" s="6">
+      <c r="I84" s="6">
         <v>-0.35829</v>
       </c>
-      <c r="J83" s="8">
-        <f t="shared" si="28"/>
+      <c r="J84" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="7:10">
-      <c r="G84" s="6" t="s">
+      <c r="S84" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="T84" s="49">
+        <v>-0.73839999999999995</v>
+      </c>
+      <c r="U84" s="49">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V84" s="57">
+        <f t="shared" si="19"/>
+        <v>4.2034250129735461E-2</v>
+      </c>
+      <c r="W84" s="49">
+        <v>0.26108999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="7:23">
+      <c r="G85" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H84" s="6">
+      <c r="H85" s="6">
         <v>-2.2200099999999998</v>
       </c>
-      <c r="I84" s="6">
+      <c r="I85" s="6">
         <v>-2.2200099999999998</v>
       </c>
-      <c r="J84" s="8">
-        <f t="shared" si="28"/>
+      <c r="J85" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="7:10">
-      <c r="G85" s="6" t="s">
+      <c r="S85" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="T85" s="49">
+        <v>-0.20449999999999999</v>
+      </c>
+      <c r="U85" s="49">
+        <v>-0.2132</v>
+      </c>
+      <c r="V85" s="57">
+        <f t="shared" si="19"/>
+        <v>4.0806754221388429E-2</v>
+      </c>
+      <c r="W85" s="49">
+        <v>0.34028000000000003</v>
+      </c>
+    </row>
+    <row r="86" spans="7:23">
+      <c r="G86" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H85" s="6">
+      <c r="H86" s="6">
         <v>-0.73923000000000005</v>
       </c>
-      <c r="I85" s="6">
+      <c r="I86" s="6">
         <v>-0.73923000000000005</v>
       </c>
-      <c r="J85" s="8">
-        <f t="shared" si="28"/>
+      <c r="J86" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="7:10">
-      <c r="G86" s="26" t="s">
+      <c r="S86" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="T86" s="49">
+        <v>-2.2353000000000001</v>
+      </c>
+      <c r="U86" s="49">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V86" s="49">
+        <f t="shared" si="19"/>
+        <v>1.8375761921836746E-3</v>
+      </c>
+      <c r="W86" s="49">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="7:23">
+      <c r="G87" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H86" s="28">
+      <c r="H87" s="28">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="I86" s="26">
+      <c r="I87" s="26">
         <v>-0.25318000000000002</v>
       </c>
-      <c r="J86" s="8">
-        <f t="shared" si="28"/>
+      <c r="J87" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="7:10">
-      <c r="G87" s="6" t="s">
+      <c r="S87" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="T87" s="49">
+        <v>-0.73209999999999997</v>
+      </c>
+      <c r="U87" s="49">
+        <v>-0.72</v>
+      </c>
+      <c r="V87" s="49">
+        <f t="shared" si="19"/>
+        <v>1.6805555555555556E-2</v>
+      </c>
+      <c r="W87" s="49">
+        <v>5.0600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="7:23">
+      <c r="G88" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H87" s="6">
+      <c r="H88" s="6">
         <v>-1.8151900000000001</v>
       </c>
-      <c r="I87" s="6">
+      <c r="I88" s="6">
         <v>-1.8151900000000001</v>
       </c>
-      <c r="J87" s="8">
-        <f t="shared" si="28"/>
+      <c r="J88" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="7:10">
-      <c r="G88" s="6" t="s">
+      <c r="S88" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="T88" s="52">
+        <v>-1.7627999999999999</v>
+      </c>
+      <c r="U88" s="52">
+        <v>-1.8142</v>
+      </c>
+      <c r="V88" s="49">
+        <f t="shared" si="19"/>
+        <v>2.8332047183331557E-2</v>
+      </c>
+      <c r="W88" s="53">
+        <v>4.5699999999999997E-9</v>
+      </c>
+    </row>
+    <row r="89" spans="7:23">
+      <c r="G89" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H88" s="6">
+      <c r="H89" s="6">
         <v>-0.55120000000000002</v>
       </c>
-      <c r="I88" s="6">
+      <c r="I89" s="6">
         <v>-0.55120000000000002</v>
       </c>
-      <c r="J88" s="8">
-        <f t="shared" si="28"/>
+      <c r="J89" s="8">
+        <f t="shared" si="18"/>
         <v>0</v>
+      </c>
+      <c r="S89" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="T89" s="49">
+        <v>-0.52829999999999999</v>
+      </c>
+      <c r="U89" s="49">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V89" s="49">
+        <f t="shared" si="19"/>
+        <v>5.5932809149392415E-2</v>
+      </c>
+      <c r="W89" s="49">
+        <v>5.7110000000000001E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="7:23">
+      <c r="S92" s="55" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="93" spans="7:23">
+      <c r="S93" s="55" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="95" spans="7:23">
+      <c r="S95" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="T95" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="U95" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="V95" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="W95" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="7:23">
+      <c r="S96" s="58" t="s">
+        <v>261</v>
+      </c>
+      <c r="T96" s="57">
+        <v>-0.35289999999999999</v>
+      </c>
+      <c r="U96" s="57">
+        <v>-0.37140000000000001</v>
+      </c>
+      <c r="V96" s="49">
+        <f>ABS((T96-U96)/U96)</f>
+        <v>4.9811523963381843E-2</v>
+      </c>
+      <c r="W96" s="57">
+        <v>0.28316999999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="19:23">
+      <c r="S97" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="T97" s="49">
+        <v>0.27650000000000002</v>
+      </c>
+      <c r="U97" s="49">
+        <v>0.25609999999999999</v>
+      </c>
+      <c r="V97" s="49">
+        <f>ABS((T97-U97)/U97)</f>
+        <v>7.9656384224912266E-2</v>
+      </c>
+      <c r="W97" s="49">
+        <v>0.46418999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="19:23">
+      <c r="S98" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="T98" s="49">
+        <v>-0.74409999999999998</v>
+      </c>
+      <c r="U98" s="49">
+        <v>-0.77080000000000004</v>
+      </c>
+      <c r="V98" s="49">
+        <f t="shared" ref="V98:V103" si="20">ABS((T98-U98)/U98)</f>
+        <v>3.4639335755059751E-2</v>
+      </c>
+      <c r="W98" s="49">
+        <v>0.26108999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="19:23">
+      <c r="S99" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="T99" s="49">
+        <v>-0.24310000000000001</v>
+      </c>
+      <c r="U99" s="49">
+        <v>-0.2132</v>
+      </c>
+      <c r="V99" s="57">
+        <f t="shared" si="20"/>
+        <v>0.14024390243902443</v>
+      </c>
+      <c r="W99" s="49">
+        <v>0.34028000000000003</v>
+      </c>
+    </row>
+    <row r="100" spans="19:23">
+      <c r="S100" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="T100" s="49">
+        <v>-2.3006000000000002</v>
+      </c>
+      <c r="U100" s="49">
+        <v>-2.2311999999999999</v>
+      </c>
+      <c r="V100" s="49">
+        <f t="shared" si="20"/>
+        <v>3.1104338472570974E-2</v>
+      </c>
+      <c r="W100" s="49">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="19:23">
+      <c r="S101" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="T101" s="49">
+        <v>-0.75149999999999995</v>
+      </c>
+      <c r="U101" s="49">
+        <v>-0.72</v>
+      </c>
+      <c r="V101" s="49">
+        <f t="shared" si="20"/>
+        <v>4.3749999999999963E-2</v>
+      </c>
+      <c r="W101" s="49">
+        <v>5.0600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="19:23">
+      <c r="S102" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="T102" s="49">
+        <v>-1.7986</v>
+      </c>
+      <c r="U102" s="49">
+        <v>-1.8142</v>
+      </c>
+      <c r="V102" s="49">
+        <f t="shared" si="20"/>
+        <v>8.5988314408555061E-3</v>
+      </c>
+      <c r="W102" s="53">
+        <v>4.5699999999999997E-9</v>
+      </c>
+    </row>
+    <row r="103" spans="19:23">
+      <c r="S103" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="T103" s="49">
+        <v>-0.57150000000000001</v>
+      </c>
+      <c r="U103" s="49">
+        <v>-0.55959999999999999</v>
+      </c>
+      <c r="V103" s="49">
+        <f t="shared" si="20"/>
+        <v>2.126518942101505E-2</v>
+      </c>
+      <c r="W103" s="49">
+        <v>5.7110000000000001E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8043,20 +8899,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="66" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="73"/>
       <c r="D2" s="35" t="s">
         <v>231</v>
       </c>
@@ -8068,118 +8924,118 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="74" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
       <c r="D3" s="39">
         <v>1.2506999999999999</v>
       </c>
       <c r="E3" s="8">
         <v>0.47</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="70" t="s">
         <v>229</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="67" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="36">
         <v>-14.5717</v>
       </c>
       <c r="E4" s="6">
         <v>0.16550000000000001</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="77" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="38" t="s">
         <v>232</v>
       </c>
       <c r="E5" s="33">
         <v>0</v>
       </c>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="67" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="36">
         <v>0.436</v>
       </c>
       <c r="E6" s="6">
         <v>0.75860000000000005</v>
       </c>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="67" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="36">
         <v>-14.1897</v>
       </c>
       <c r="E7" s="6">
         <v>0.24</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="67" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="36">
         <v>0.13270000000000001</v>
       </c>
@@ -8188,11 +9044,11 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="36">
         <v>-1.3482000000000001</v>
       </c>
@@ -8201,11 +9057,11 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="77" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="63"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="38" t="s">
         <v>232</v>
       </c>
@@ -8214,11 +9070,11 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="36">
         <v>-0.44040000000000001</v>
       </c>
@@ -8227,11 +9083,11 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="53"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="36">
         <v>-0.60709999999999997</v>
       </c>
@@ -8240,11 +9096,11 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="36">
         <v>-0.71689999999999998</v>
       </c>
@@ -8253,11 +9109,11 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="36">
         <v>-16.180800000000001</v>
       </c>
@@ -8266,11 +9122,11 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="67" t="s">
         <v>215</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="36">
         <v>-0.89485999999999999</v>
       </c>
@@ -8279,11 +9135,11 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="67" t="s">
         <v>216</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="36">
         <v>0.85899999999999999</v>
       </c>
@@ -8292,11 +9148,11 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="67" t="s">
         <v>217</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="69"/>
       <c r="D17" s="36">
         <v>0.47910000000000003</v>
       </c>
@@ -8305,11 +9161,11 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="67" t="s">
         <v>218</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="36">
         <v>14.4727</v>
       </c>
@@ -8318,11 +9174,11 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="67" t="s">
         <v>219</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="53"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
       <c r="D19" s="36">
         <v>-16.2044</v>
       </c>
@@ -8331,11 +9187,11 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="69"/>
       <c r="D20" s="36">
         <v>11.651999999999999</v>
       </c>
@@ -8344,11 +9200,11 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="67" t="s">
         <v>221</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="53"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="69"/>
       <c r="D21" s="36">
         <v>2.673E-2</v>
       </c>
@@ -8357,11 +9213,11 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="67" t="s">
         <v>222</v>
       </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="69"/>
       <c r="D22" s="36">
         <v>0.1087</v>
       </c>

</xml_diff>

<commit_message>
Bottom_2_2 without quality of outfit, race & body type collapsed - preliminary main effects model
</commit_message>
<xml_diff>
--- a/Summary of Effect Estimates and P Values.xlsx
+++ b/Summary of Effect Estimates and P Values.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michelle/Desktop/Research with Becca/RPDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482040B-F148-6F46-9AC7-4A66078C5033}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC57C2D0-5114-1742-9D33-B0182CE6681A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="500" windowWidth="23980" windowHeight="17500" activeTab="3" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="25380" windowHeight="17500" activeTab="5" xr2:uid="{91B86367-0610-F24F-88C2-86F9A112A2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="RPDR Effect Estimates" sheetId="1" r:id="rId1"/>
     <sheet name="Bottom Two - Unit bivariate eff" sheetId="2" r:id="rId2"/>
     <sheet name="Bottom Two 2 wo quality of out" sheetId="5" r:id="rId3"/>
     <sheet name="Delta B Comparisons" sheetId="3" r:id="rId4"/>
-    <sheet name="Variable Interactions" sheetId="4" r:id="rId5"/>
+    <sheet name="Interactions_Bottom2" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="294">
   <si>
     <t>Age</t>
   </si>
@@ -818,6 +819,100 @@
   </si>
   <si>
     <t>Model 19</t>
+  </si>
+  <si>
+    <t>summary(Model_20 &lt;- glm(OUTCOME_LOSS ~ Age + Carson + Dancing + Outfit_Reveal + Ross + Do_They_Know_Words + Sewing + Lip_Sync_Ass + Expressed_Hardship, family = binomial(link='logit'), data = Bottom_Two_2))</t>
+  </si>
+  <si>
+    <t>Age:Carson</t>
+  </si>
+  <si>
+    <t>Age:Dancing</t>
+  </si>
+  <si>
+    <t>Age:Outfit_Reveal</t>
+  </si>
+  <si>
+    <t>Age:Ross</t>
+  </si>
+  <si>
+    <t>Age:Do_They_Know_Words</t>
+  </si>
+  <si>
+    <t>Age:Sewing</t>
+  </si>
+  <si>
+    <t>Age:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Carson:Dancing</t>
+  </si>
+  <si>
+    <t>Carson:Outfit_Reveal</t>
+  </si>
+  <si>
+    <t>Carson:Ross</t>
+  </si>
+  <si>
+    <t>Carson:Do_They_Know_Words</t>
+  </si>
+  <si>
+    <t>Carson:Sewing</t>
+  </si>
+  <si>
+    <t>Carson:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Carson:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Dancing:Outfit_Reveal</t>
+  </si>
+  <si>
+    <t>Dancing:Ross</t>
+  </si>
+  <si>
+    <t>Dancing:Do_They_Know_Words</t>
+  </si>
+  <si>
+    <t>Dancing:Sewing</t>
+  </si>
+  <si>
+    <t>Dancing:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Dancing:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Outfit_Reveal:Ross</t>
+  </si>
+  <si>
+    <t>Ross:Do_They_Know_Words</t>
+  </si>
+  <si>
+    <t>Ross:Sewing</t>
+  </si>
+  <si>
+    <t>Ross:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Ross:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t>Lip_Sync_Ass:Expressed_Hardship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warning message:
+glm.fit: fitted probabilities numerically 0 or 1 occurred </t>
+  </si>
+  <si>
+    <t>Age:Lip_Sync_Ass</t>
+  </si>
+  <si>
+    <t>Do_They_Know_Words:Expressed_Hardship11.77439</t>
+  </si>
+  <si>
+    <t>Dancing 0</t>
   </si>
 </sst>
 </file>
@@ -982,7 +1077,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1090,11 +1185,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1219,6 +1343,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1240,14 +1373,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1571,7 +1701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115F1DD9-A0CB-2E42-BC0A-13187B41B5A6}">
   <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
@@ -5107,8 +5237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8CE274-EB9F-1B4B-B822-29A7242BA18E}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6000,7 +6130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81B9891-AE0A-EC49-A442-8B89DE5C2A2B}">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L72" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V100" sqref="V100"/>
     </sheetView>
   </sheetViews>
@@ -8888,7 +9018,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8908,11 +9038,11 @@
       <c r="E1" s="66"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
       <c r="D2" s="35" t="s">
         <v>231</v>
       </c>
@@ -8924,27 +9054,27 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="77" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="76"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="39">
         <v>1.2506999999999999</v>
       </c>
       <c r="E3" s="8">
         <v>0.47</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="73" t="s">
         <v>229</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="67" t="s">
@@ -8958,35 +9088,35 @@
       <c r="E4" s="6">
         <v>0.16550000000000001</v>
       </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="70" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="38" t="s">
         <v>232</v>
       </c>
       <c r="E5" s="33">
         <v>0</v>
       </c>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="67" t="s">
@@ -9000,14 +9130,14 @@
       <c r="E6" s="6">
         <v>0.75860000000000005</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="67" t="s">
@@ -9021,14 +9151,14 @@
       <c r="E7" s="6">
         <v>0.24</v>
       </c>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="70"/>
-      <c r="N7" s="70"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="67" t="s">
@@ -9057,11 +9187,11 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="70" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="72"/>
       <c r="D10" s="38" t="s">
         <v>232</v>
       </c>
@@ -9267,6 +9397,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G3:N7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A7:C7"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A13:C13"/>
@@ -9279,17 +9420,608 @@
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2543501B-1CBC-384D-9B0C-8DC9CE8C4FE1}">
+  <dimension ref="A2:N49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="6" max="6" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14">
+      <c r="A2" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="G2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="74" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="73" t="s">
+        <v>263</v>
+      </c>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="80" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="6">
+        <v>5.8160000000000003E-2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.39362000000000003</v>
+      </c>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="80" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="6">
+        <v>5.465E-4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.99275000000000002</v>
+      </c>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="80" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="6">
+        <v>-0.26884999999999998</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.22325</v>
+      </c>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="80" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="6">
+        <v>-1.387E-3</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.97957000000000005</v>
+      </c>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+    </row>
+    <row r="8" spans="1:14" ht="51">
+      <c r="A8" s="80" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="6">
+        <v>-6.3948</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="F8" s="83" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="80" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="6">
+        <v>-1.6719999999999999E-2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.75280000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="80" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="6">
+        <v>1.8020000000000001E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.74878999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="80" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="6">
+        <v>5.1923999999999998E-2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.33317000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="80" t="s">
+        <v>271</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="6">
+        <v>0.44742999999999999</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.49162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="80" t="s">
+        <v>272</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="6">
+        <v>-15.210380000000001</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.98616000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="80" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="6">
+        <v>-2.648E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.96860000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="80" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="6">
+        <v>16.341000000000001</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0.98533999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="80" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="6">
+        <v>6.2630000000000005E-2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="80" t="s">
+        <v>276</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="6">
+        <v>-0.77766000000000002</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.31548999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="80" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="6">
+        <v>0.36030000000000001</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.61240000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="80" t="s">
+        <v>278</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="6">
+        <v>0.39377000000000001</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.76817000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="80" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="6">
+        <v>-9.8150000000000001E-2</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.87292000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="80" t="s">
+        <v>280</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="6">
+        <v>-14.580590000000001</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0.98689000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="80" t="s">
+        <v>281</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="6">
+        <v>-0.39684000000000003</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.50549999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="80" t="s">
+        <v>282</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="6">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.95760000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="80" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="6">
+        <v>-0.34738000000000002</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.59894999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="80" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="6">
+        <v>-14.401070000000001</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.98695999999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="80" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="80" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="6">
+        <v>0.18479000000000001</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.88861000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="80" t="s">
+        <v>208</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="6">
+        <v>-14.70152</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.98492000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="80" t="s">
+        <v>209</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="6">
+        <v>0.34131</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.83150999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="80" t="s">
+        <v>285</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="80" t="s">
+        <v>286</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="6">
+        <v>-0.30080000000000001</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.62670000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="80" t="s">
+        <v>287</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="6">
+        <v>-0.71014999999999995</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.27012000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="80" t="s">
+        <v>288</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="6">
+        <v>-0.36325000000000002</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.57177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="80" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="6">
+        <v>14.94811</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.98740000000000006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="80" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="6">
+        <v>-15.80132</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.98770000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="80" t="s">
+        <v>292</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6">
+        <v>0.99087000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="80" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="6">
+        <v>0.14974999999999999</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.79710000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="80" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="6">
+        <v>0.30077999999999999</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.61539999999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="81" t="s">
+        <v>289</v>
+      </c>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="6">
+        <v>0.72711000000000003</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.2707</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="37" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
     <mergeCell ref="G3:N7"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>